<commit_message>
Update automatico via Actualizar 06-15-2021 19-08-48
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci_diario.xlsx
+++ b/input/Camas_uci/last_uci_diario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="676"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="676" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UCI HABILITADA" sheetId="2" r:id="rId1"/>
@@ -259,7 +259,27 @@
     <cellStyle name="Millares [0] 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="256">
+  <dxfs count="258">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3130,12 +3150,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PF20"/>
+  <dimension ref="A1:PM20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OV1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="PC1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="PB22" sqref="PB22"/>
+      <selection pane="topRight" activeCell="PJ22" sqref="PJ22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3156,7 +3176,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4423,8 +4443,29 @@
       <c r="PF1" s="8">
         <v>44355</v>
       </c>
+      <c r="PG1" s="8">
+        <v>44356</v>
+      </c>
+      <c r="PH1" s="8">
+        <v>44357</v>
+      </c>
+      <c r="PI1" s="8">
+        <v>44358</v>
+      </c>
+      <c r="PJ1" s="8">
+        <v>44359</v>
+      </c>
+      <c r="PK1" s="8">
+        <v>44360</v>
+      </c>
+      <c r="PL1" s="8">
+        <v>44361</v>
+      </c>
+      <c r="PM1" s="8">
+        <v>44362</v>
+      </c>
     </row>
-    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5691,8 +5732,29 @@
       <c r="PF2" s="11">
         <v>33</v>
       </c>
+      <c r="PG2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PH2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PI2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PJ2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PK2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PL2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PM2" s="11">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -6959,8 +7021,29 @@
       <c r="PF3" s="11">
         <v>62</v>
       </c>
+      <c r="PG3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PH3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PI3" s="11">
+        <v>62</v>
+      </c>
+      <c r="PJ3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PK3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PL3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PM3" s="11">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -8227,8 +8310,29 @@
       <c r="PF4" s="11">
         <v>165</v>
       </c>
+      <c r="PG4" s="11">
+        <v>166</v>
+      </c>
+      <c r="PH4" s="11">
+        <v>164</v>
+      </c>
+      <c r="PI4" s="11">
+        <v>163</v>
+      </c>
+      <c r="PJ4" s="11">
+        <v>163</v>
+      </c>
+      <c r="PK4" s="11">
+        <v>163</v>
+      </c>
+      <c r="PL4" s="11">
+        <v>163</v>
+      </c>
+      <c r="PM4" s="11">
+        <v>163</v>
+      </c>
     </row>
-    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -9495,8 +9599,29 @@
       <c r="PF5" s="11">
         <v>34</v>
       </c>
+      <c r="PG5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PH5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PI5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PJ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PK5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PL5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PM5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -10763,8 +10888,29 @@
       <c r="PF6" s="11">
         <v>135</v>
       </c>
+      <c r="PG6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PH6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PI6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PJ6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PK6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PL6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PM6" s="11">
+        <v>136</v>
+      </c>
     </row>
-    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -12031,8 +12177,29 @@
       <c r="PF7" s="11">
         <v>330</v>
       </c>
+      <c r="PG7" s="11">
+        <v>334</v>
+      </c>
+      <c r="PH7" s="11">
+        <v>336</v>
+      </c>
+      <c r="PI7" s="11">
+        <v>336</v>
+      </c>
+      <c r="PJ7" s="11">
+        <v>336</v>
+      </c>
+      <c r="PK7" s="11">
+        <v>336</v>
+      </c>
+      <c r="PL7" s="11">
+        <v>335</v>
+      </c>
+      <c r="PM7" s="11">
+        <v>335</v>
+      </c>
     </row>
-    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -13299,8 +13466,29 @@
       <c r="PF8" s="11">
         <v>2599</v>
       </c>
+      <c r="PG8" s="11">
+        <v>2602</v>
+      </c>
+      <c r="PH8" s="11">
+        <v>2613</v>
+      </c>
+      <c r="PI8" s="11">
+        <v>2621</v>
+      </c>
+      <c r="PJ8" s="11">
+        <v>2623</v>
+      </c>
+      <c r="PK8" s="11">
+        <v>2619</v>
+      </c>
+      <c r="PL8" s="11">
+        <v>2621</v>
+      </c>
+      <c r="PM8" s="11">
+        <v>2621</v>
+      </c>
     </row>
-    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -14567,8 +14755,29 @@
       <c r="PF9" s="11">
         <v>206</v>
       </c>
+      <c r="PG9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PH9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PI9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PJ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PK9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PL9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PM9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -15835,8 +16044,29 @@
       <c r="PF10" s="11">
         <v>158</v>
       </c>
+      <c r="PG10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PH10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PI10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PJ10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PK10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PL10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PM10" s="11">
+        <v>158</v>
+      </c>
     </row>
-    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -17103,8 +17333,29 @@
       <c r="PF11" s="11">
         <v>70</v>
       </c>
+      <c r="PG11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PH11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PI11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PJ11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PK11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PL11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PM11" s="11">
+        <v>70</v>
+      </c>
     </row>
-    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -18371,8 +18622,29 @@
       <c r="PF12" s="11">
         <v>310</v>
       </c>
+      <c r="PG12" s="11">
+        <v>310</v>
+      </c>
+      <c r="PH12" s="11">
+        <v>310</v>
+      </c>
+      <c r="PI12" s="11">
+        <v>310</v>
+      </c>
+      <c r="PJ12" s="11">
+        <v>312</v>
+      </c>
+      <c r="PK12" s="11">
+        <v>312</v>
+      </c>
+      <c r="PL12" s="11">
+        <v>312</v>
+      </c>
+      <c r="PM12" s="11">
+        <v>311</v>
+      </c>
     </row>
-    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -19639,8 +19911,29 @@
       <c r="PF13" s="11">
         <v>150</v>
       </c>
+      <c r="PG13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PH13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PI13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PJ13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PK13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PL13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PM13" s="11">
+        <v>150</v>
+      </c>
     </row>
-    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -20907,8 +21200,29 @@
       <c r="PF14" s="11">
         <v>44</v>
       </c>
+      <c r="PG14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PH14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PI14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PJ14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PK14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PL14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PM14" s="11">
+        <v>44</v>
+      </c>
     </row>
-    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -22175,8 +22489,29 @@
       <c r="PF15" s="11">
         <v>134</v>
       </c>
+      <c r="PG15" s="11">
+        <v>134</v>
+      </c>
+      <c r="PH15" s="11">
+        <v>134</v>
+      </c>
+      <c r="PI15" s="11">
+        <v>134</v>
+      </c>
+      <c r="PJ15" s="11">
+        <v>134</v>
+      </c>
+      <c r="PK15" s="11">
+        <v>137</v>
+      </c>
+      <c r="PL15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PM15" s="11">
+        <v>139</v>
+      </c>
     </row>
-    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -23443,8 +23778,29 @@
       <c r="PF16" s="11">
         <v>13</v>
       </c>
+      <c r="PG16" s="11">
+        <v>13</v>
+      </c>
+      <c r="PH16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PI16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PJ16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PK16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PL16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PM16" s="11">
+        <v>17</v>
+      </c>
     </row>
-    <row r="17" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -24711,8 +25067,29 @@
       <c r="PF17" s="11">
         <v>47</v>
       </c>
+      <c r="PG17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PH17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PI17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PJ17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PK17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PL17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PM17" s="11">
+        <v>47</v>
+      </c>
     </row>
-    <row r="18" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -25872,7 +26249,7 @@
         <v>3931</v>
       </c>
       <c r="MU18" s="6">
-        <f t="shared" ref="MU18:PF18" si="7">SUM(MU2:MU17)</f>
+        <f t="shared" ref="MU18:PG18" si="7">SUM(MU2:MU17)</f>
         <v>3954</v>
       </c>
       <c r="MV18" s="6">
@@ -26127,13 +26504,41 @@
         <f t="shared" si="7"/>
         <v>4490</v>
       </c>
+      <c r="PG18" s="6">
+        <f t="shared" si="7"/>
+        <v>4498</v>
+      </c>
+      <c r="PH18" s="6">
+        <f t="shared" ref="PH18:PM18" si="8">SUM(PH2:PH17)</f>
+        <v>4513</v>
+      </c>
+      <c r="PI18" s="6">
+        <f t="shared" si="8"/>
+        <v>4516</v>
+      </c>
+      <c r="PJ18" s="6">
+        <f t="shared" si="8"/>
+        <v>4523</v>
+      </c>
+      <c r="PK18" s="6">
+        <f t="shared" si="8"/>
+        <v>4522</v>
+      </c>
+      <c r="PL18" s="6">
+        <f t="shared" si="8"/>
+        <v>4525</v>
+      </c>
+      <c r="PM18" s="6">
+        <f t="shared" si="8"/>
+        <v>4525</v>
+      </c>
     </row>
-    <row r="19" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:429" x14ac:dyDescent="0.25">
       <c r="HV19" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:429" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -26151,12 +26556,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PF34"/>
+  <dimension ref="A1:PM34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OW1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="PD1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="PC21" sqref="PC21"/>
+      <selection pane="topRight" activeCell="PG18" sqref="PG18:PM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26176,7 +26581,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -27443,8 +27848,29 @@
       <c r="PF1" s="8">
         <v>44355</v>
       </c>
+      <c r="PG1" s="8">
+        <v>44356</v>
+      </c>
+      <c r="PH1" s="8">
+        <v>44357</v>
+      </c>
+      <c r="PI1" s="8">
+        <v>44358</v>
+      </c>
+      <c r="PJ1" s="8">
+        <v>44359</v>
+      </c>
+      <c r="PK1" s="8">
+        <v>44360</v>
+      </c>
+      <c r="PL1" s="8">
+        <v>44361</v>
+      </c>
+      <c r="PM1" s="8">
+        <v>44362</v>
+      </c>
     </row>
-    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -28711,8 +29137,29 @@
       <c r="PF2">
         <v>22</v>
       </c>
+      <c r="PG2">
+        <v>22</v>
+      </c>
+      <c r="PH2">
+        <v>23</v>
+      </c>
+      <c r="PI2">
+        <v>23</v>
+      </c>
+      <c r="PJ2">
+        <v>23</v>
+      </c>
+      <c r="PK2">
+        <v>23</v>
+      </c>
+      <c r="PL2">
+        <v>26</v>
+      </c>
+      <c r="PM2">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -29979,8 +30426,29 @@
       <c r="PF3">
         <v>54</v>
       </c>
+      <c r="PG3">
+        <v>54</v>
+      </c>
+      <c r="PH3">
+        <v>50</v>
+      </c>
+      <c r="PI3">
+        <v>52</v>
+      </c>
+      <c r="PJ3">
+        <v>53</v>
+      </c>
+      <c r="PK3">
+        <v>54</v>
+      </c>
+      <c r="PL3">
+        <v>55</v>
+      </c>
+      <c r="PM3">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -31247,8 +31715,29 @@
       <c r="PF4">
         <v>84</v>
       </c>
+      <c r="PG4">
+        <v>84</v>
+      </c>
+      <c r="PH4">
+        <v>91</v>
+      </c>
+      <c r="PI4">
+        <v>88</v>
+      </c>
+      <c r="PJ4">
+        <v>87</v>
+      </c>
+      <c r="PK4">
+        <v>88</v>
+      </c>
+      <c r="PL4">
+        <v>94</v>
+      </c>
+      <c r="PM4">
+        <v>90</v>
+      </c>
     </row>
-    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -32515,8 +33004,29 @@
       <c r="PF5">
         <v>20</v>
       </c>
+      <c r="PG5">
+        <v>21</v>
+      </c>
+      <c r="PH5">
+        <v>20</v>
+      </c>
+      <c r="PI5">
+        <v>20</v>
+      </c>
+      <c r="PJ5">
+        <v>20</v>
+      </c>
+      <c r="PK5">
+        <v>20</v>
+      </c>
+      <c r="PL5">
+        <v>20</v>
+      </c>
+      <c r="PM5">
+        <v>24</v>
+      </c>
     </row>
-    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -33783,8 +34293,29 @@
       <c r="PF6">
         <v>104</v>
       </c>
+      <c r="PG6">
+        <v>105</v>
+      </c>
+      <c r="PH6">
+        <v>108</v>
+      </c>
+      <c r="PI6">
+        <v>106</v>
+      </c>
+      <c r="PJ6">
+        <v>105</v>
+      </c>
+      <c r="PK6">
+        <v>105</v>
+      </c>
+      <c r="PL6">
+        <v>101</v>
+      </c>
+      <c r="PM6">
+        <v>104</v>
+      </c>
     </row>
-    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -35051,8 +35582,29 @@
       <c r="PF7">
         <v>213</v>
       </c>
+      <c r="PG7">
+        <v>225</v>
+      </c>
+      <c r="PH7">
+        <v>233</v>
+      </c>
+      <c r="PI7">
+        <v>230</v>
+      </c>
+      <c r="PJ7">
+        <v>229</v>
+      </c>
+      <c r="PK7">
+        <v>234</v>
+      </c>
+      <c r="PL7">
+        <v>231</v>
+      </c>
+      <c r="PM7">
+        <v>223</v>
+      </c>
     </row>
-    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -36319,8 +36871,29 @@
       <c r="PF8">
         <v>1971</v>
       </c>
+      <c r="PG8">
+        <v>1979</v>
+      </c>
+      <c r="PH8">
+        <v>1959</v>
+      </c>
+      <c r="PI8">
+        <v>2015</v>
+      </c>
+      <c r="PJ8">
+        <v>1989</v>
+      </c>
+      <c r="PK8">
+        <v>1975</v>
+      </c>
+      <c r="PL8">
+        <v>1970</v>
+      </c>
+      <c r="PM8">
+        <v>1974</v>
+      </c>
     </row>
-    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -37587,8 +38160,29 @@
       <c r="PF9">
         <v>156</v>
       </c>
+      <c r="PG9">
+        <v>156</v>
+      </c>
+      <c r="PH9">
+        <v>150</v>
+      </c>
+      <c r="PI9">
+        <v>153</v>
+      </c>
+      <c r="PJ9">
+        <v>151</v>
+      </c>
+      <c r="PK9">
+        <v>151</v>
+      </c>
+      <c r="PL9">
+        <v>151</v>
+      </c>
+      <c r="PM9">
+        <v>151</v>
+      </c>
     </row>
-    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -38855,8 +39449,29 @@
       <c r="PF10">
         <v>110</v>
       </c>
+      <c r="PG10">
+        <v>106</v>
+      </c>
+      <c r="PH10">
+        <v>109</v>
+      </c>
+      <c r="PI10">
+        <v>103</v>
+      </c>
+      <c r="PJ10">
+        <v>108</v>
+      </c>
+      <c r="PK10">
+        <v>113</v>
+      </c>
+      <c r="PL10">
+        <v>113</v>
+      </c>
+      <c r="PM10">
+        <v>108</v>
+      </c>
     </row>
-    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -40123,8 +40738,29 @@
       <c r="PF11">
         <v>45</v>
       </c>
+      <c r="PG11">
+        <v>47</v>
+      </c>
+      <c r="PH11">
+        <v>47</v>
+      </c>
+      <c r="PI11">
+        <v>45</v>
+      </c>
+      <c r="PJ11">
+        <v>46</v>
+      </c>
+      <c r="PK11">
+        <v>45</v>
+      </c>
+      <c r="PL11">
+        <v>47</v>
+      </c>
+      <c r="PM11">
+        <v>46</v>
+      </c>
     </row>
-    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -41391,8 +42027,29 @@
       <c r="PF12">
         <v>198</v>
       </c>
+      <c r="PG12">
+        <v>194</v>
+      </c>
+      <c r="PH12">
+        <v>196</v>
+      </c>
+      <c r="PI12">
+        <v>196</v>
+      </c>
+      <c r="PJ12">
+        <v>200</v>
+      </c>
+      <c r="PK12">
+        <v>202</v>
+      </c>
+      <c r="PL12">
+        <v>202</v>
+      </c>
+      <c r="PM12">
+        <v>200</v>
+      </c>
     </row>
-    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -42659,8 +43316,29 @@
       <c r="PF13">
         <v>109</v>
       </c>
+      <c r="PG13">
+        <v>109</v>
+      </c>
+      <c r="PH13">
+        <v>108</v>
+      </c>
+      <c r="PI13">
+        <v>108</v>
+      </c>
+      <c r="PJ13">
+        <v>102</v>
+      </c>
+      <c r="PK13">
+        <v>107</v>
+      </c>
+      <c r="PL13">
+        <v>107</v>
+      </c>
+      <c r="PM13">
+        <v>103</v>
+      </c>
     </row>
-    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -43927,8 +44605,29 @@
       <c r="PF14">
         <v>33</v>
       </c>
+      <c r="PG14">
+        <v>32</v>
+      </c>
+      <c r="PH14">
+        <v>30</v>
+      </c>
+      <c r="PI14">
+        <v>29</v>
+      </c>
+      <c r="PJ14">
+        <v>29</v>
+      </c>
+      <c r="PK14">
+        <v>27</v>
+      </c>
+      <c r="PL14">
+        <v>26</v>
+      </c>
+      <c r="PM14">
+        <v>29</v>
+      </c>
     </row>
-    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -45195,8 +45894,29 @@
       <c r="PF15">
         <v>107</v>
       </c>
+      <c r="PG15">
+        <v>106</v>
+      </c>
+      <c r="PH15">
+        <v>103</v>
+      </c>
+      <c r="PI15">
+        <v>102</v>
+      </c>
+      <c r="PJ15">
+        <v>105</v>
+      </c>
+      <c r="PK15">
+        <v>106</v>
+      </c>
+      <c r="PL15">
+        <v>104</v>
+      </c>
+      <c r="PM15">
+        <v>103</v>
+      </c>
     </row>
-    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -46463,8 +47183,29 @@
       <c r="PF16">
         <v>11</v>
       </c>
+      <c r="PG16">
+        <v>10</v>
+      </c>
+      <c r="PH16">
+        <v>11</v>
+      </c>
+      <c r="PI16">
+        <v>13</v>
+      </c>
+      <c r="PJ16">
+        <v>11</v>
+      </c>
+      <c r="PK16">
+        <v>12</v>
+      </c>
+      <c r="PL16">
+        <v>13</v>
+      </c>
+      <c r="PM16">
+        <v>13</v>
+      </c>
     </row>
-    <row r="17" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -47731,8 +48472,29 @@
       <c r="PF17">
         <v>28</v>
       </c>
+      <c r="PG17">
+        <v>29</v>
+      </c>
+      <c r="PH17">
+        <v>28</v>
+      </c>
+      <c r="PI17">
+        <v>29</v>
+      </c>
+      <c r="PJ17">
+        <v>29</v>
+      </c>
+      <c r="PK17">
+        <v>30</v>
+      </c>
+      <c r="PL17">
+        <v>30</v>
+      </c>
+      <c r="PM17">
+        <v>29</v>
+      </c>
     </row>
-    <row r="18" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -49049,7 +49811,7 @@
         <v>2979</v>
       </c>
       <c r="OL18" s="6">
-        <f t="shared" ref="OL18:PF18" si="2">SUM(OL2:OL17)</f>
+        <f t="shared" ref="OL18:PM18" si="2">SUM(OL2:OL17)</f>
         <v>2972</v>
       </c>
       <c r="OM18" s="6">
@@ -49132,50 +49894,78 @@
         <f t="shared" si="2"/>
         <v>3265</v>
       </c>
+      <c r="PG18" s="6">
+        <f t="shared" si="2"/>
+        <v>3279</v>
+      </c>
+      <c r="PH18" s="6">
+        <f t="shared" si="2"/>
+        <v>3266</v>
+      </c>
+      <c r="PI18" s="6">
+        <f t="shared" si="2"/>
+        <v>3312</v>
+      </c>
+      <c r="PJ18" s="6">
+        <f t="shared" si="2"/>
+        <v>3287</v>
+      </c>
+      <c r="PK18" s="6">
+        <f t="shared" si="2"/>
+        <v>3292</v>
+      </c>
+      <c r="PL18" s="6">
+        <f t="shared" si="2"/>
+        <v>3290</v>
+      </c>
+      <c r="PM18" s="6">
+        <f t="shared" si="2"/>
+        <v>3275</v>
+      </c>
     </row>
-    <row r="19" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:429" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:429" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:429" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:429" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -49195,12 +49985,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:PF34"/>
+  <dimension ref="A1:PM34"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="OV1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="PC1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="PF22" sqref="PF22"/>
+      <selection pane="topRight" activeCell="PM22" sqref="PM22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -49217,7 +50007,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -50484,8 +51274,29 @@
       <c r="PF1" s="8">
         <v>44355</v>
       </c>
+      <c r="PG1" s="8">
+        <v>44356</v>
+      </c>
+      <c r="PH1" s="8">
+        <v>44357</v>
+      </c>
+      <c r="PI1" s="8">
+        <v>44358</v>
+      </c>
+      <c r="PJ1" s="8">
+        <v>44359</v>
+      </c>
+      <c r="PK1" s="8">
+        <v>44360</v>
+      </c>
+      <c r="PL1" s="8">
+        <v>44361</v>
+      </c>
+      <c r="PM1" s="8">
+        <v>44362</v>
+      </c>
     </row>
-    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -51752,8 +52563,29 @@
       <c r="PF2">
         <v>8</v>
       </c>
+      <c r="PG2">
+        <v>8</v>
+      </c>
+      <c r="PH2">
+        <v>6</v>
+      </c>
+      <c r="PI2">
+        <v>7</v>
+      </c>
+      <c r="PJ2">
+        <v>7</v>
+      </c>
+      <c r="PK2">
+        <v>7</v>
+      </c>
+      <c r="PL2">
+        <v>4</v>
+      </c>
+      <c r="PM2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -53020,8 +53852,29 @@
       <c r="PF3">
         <v>5</v>
       </c>
+      <c r="PG3">
+        <v>4</v>
+      </c>
+      <c r="PH3">
+        <v>4</v>
+      </c>
+      <c r="PI3">
+        <v>4</v>
+      </c>
+      <c r="PJ3">
+        <v>5</v>
+      </c>
+      <c r="PK3">
+        <v>5</v>
+      </c>
+      <c r="PL3">
+        <v>5</v>
+      </c>
+      <c r="PM3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -54288,8 +55141,29 @@
       <c r="PF4">
         <v>72</v>
       </c>
+      <c r="PG4">
+        <v>72</v>
+      </c>
+      <c r="PH4">
+        <v>62</v>
+      </c>
+      <c r="PI4">
+        <v>66</v>
+      </c>
+      <c r="PJ4">
+        <v>66</v>
+      </c>
+      <c r="PK4">
+        <v>64</v>
+      </c>
+      <c r="PL4">
+        <v>68</v>
+      </c>
+      <c r="PM4">
+        <v>66</v>
+      </c>
     </row>
-    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -55556,8 +56430,29 @@
       <c r="PF5">
         <v>10</v>
       </c>
+      <c r="PG5">
+        <v>11</v>
+      </c>
+      <c r="PH5">
+        <v>12</v>
+      </c>
+      <c r="PI5">
+        <v>10</v>
+      </c>
+      <c r="PJ5">
+        <v>10</v>
+      </c>
+      <c r="PK5">
+        <v>10</v>
+      </c>
+      <c r="PL5">
+        <v>7</v>
+      </c>
+      <c r="PM5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -56824,8 +57719,29 @@
       <c r="PF6">
         <v>28</v>
       </c>
+      <c r="PG6">
+        <v>25</v>
+      </c>
+      <c r="PH6">
+        <v>23</v>
+      </c>
+      <c r="PI6">
+        <v>24</v>
+      </c>
+      <c r="PJ6">
+        <v>27</v>
+      </c>
+      <c r="PK6">
+        <v>26</v>
+      </c>
+      <c r="PL6">
+        <v>33</v>
+      </c>
+      <c r="PM6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -58092,8 +59008,29 @@
       <c r="PF7">
         <v>103</v>
       </c>
+      <c r="PG7">
+        <v>105</v>
+      </c>
+      <c r="PH7">
+        <v>93</v>
+      </c>
+      <c r="PI7">
+        <v>98</v>
+      </c>
+      <c r="PJ7">
+        <v>101</v>
+      </c>
+      <c r="PK7">
+        <v>93</v>
+      </c>
+      <c r="PL7">
+        <v>97</v>
+      </c>
+      <c r="PM7">
+        <v>99</v>
+      </c>
     </row>
-    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -59360,8 +60297,29 @@
       <c r="PF8">
         <v>598</v>
       </c>
+      <c r="PG8">
+        <v>588</v>
+      </c>
+      <c r="PH8">
+        <v>614</v>
+      </c>
+      <c r="PI8">
+        <v>564</v>
+      </c>
+      <c r="PJ8">
+        <v>593</v>
+      </c>
+      <c r="PK8">
+        <v>607</v>
+      </c>
+      <c r="PL8">
+        <v>608</v>
+      </c>
+      <c r="PM8">
+        <v>612</v>
+      </c>
     </row>
-    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -60628,8 +61586,29 @@
       <c r="PF9">
         <v>37</v>
       </c>
+      <c r="PG9">
+        <v>35</v>
+      </c>
+      <c r="PH9">
+        <v>35</v>
+      </c>
+      <c r="PI9">
+        <v>26</v>
+      </c>
+      <c r="PJ9">
+        <v>28</v>
+      </c>
+      <c r="PK9">
+        <v>27</v>
+      </c>
+      <c r="PL9">
+        <v>27</v>
+      </c>
+      <c r="PM9">
+        <v>34</v>
+      </c>
     </row>
-    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -61896,8 +62875,29 @@
       <c r="PF10">
         <v>23</v>
       </c>
+      <c r="PG10">
+        <v>27</v>
+      </c>
+      <c r="PH10">
+        <v>25</v>
+      </c>
+      <c r="PI10">
+        <v>28</v>
+      </c>
+      <c r="PJ10">
+        <v>24</v>
+      </c>
+      <c r="PK10">
+        <v>23</v>
+      </c>
+      <c r="PL10">
+        <v>28</v>
+      </c>
+      <c r="PM10">
+        <v>26</v>
+      </c>
     </row>
-    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -63164,8 +64164,29 @@
       <c r="PF11">
         <v>18</v>
       </c>
+      <c r="PG11">
+        <v>17</v>
+      </c>
+      <c r="PH11">
+        <v>15</v>
+      </c>
+      <c r="PI11">
+        <v>12</v>
+      </c>
+      <c r="PJ11">
+        <v>13</v>
+      </c>
+      <c r="PK11">
+        <v>12</v>
+      </c>
+      <c r="PL11">
+        <v>13</v>
+      </c>
+      <c r="PM11">
+        <v>14</v>
+      </c>
     </row>
-    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -64432,8 +65453,29 @@
       <c r="PF12">
         <v>95</v>
       </c>
+      <c r="PG12">
+        <v>90</v>
+      </c>
+      <c r="PH12">
+        <v>90</v>
+      </c>
+      <c r="PI12">
+        <v>90</v>
+      </c>
+      <c r="PJ12">
+        <v>88</v>
+      </c>
+      <c r="PK12">
+        <v>86</v>
+      </c>
+      <c r="PL12">
+        <v>92</v>
+      </c>
+      <c r="PM12">
+        <v>94</v>
+      </c>
     </row>
-    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -65700,8 +66742,29 @@
       <c r="PF13">
         <v>37</v>
       </c>
+      <c r="PG13">
+        <v>36</v>
+      </c>
+      <c r="PH13">
+        <v>34</v>
+      </c>
+      <c r="PI13">
+        <v>36</v>
+      </c>
+      <c r="PJ13">
+        <v>40</v>
+      </c>
+      <c r="PK13">
+        <v>37</v>
+      </c>
+      <c r="PL13">
+        <v>40</v>
+      </c>
+      <c r="PM13">
+        <v>44</v>
+      </c>
     </row>
-    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -66968,8 +68031,29 @@
       <c r="PF14">
         <v>7</v>
       </c>
+      <c r="PG14">
+        <v>12</v>
+      </c>
+      <c r="PH14">
+        <v>11</v>
+      </c>
+      <c r="PI14">
+        <v>10</v>
+      </c>
+      <c r="PJ14">
+        <v>13</v>
+      </c>
+      <c r="PK14">
+        <v>12</v>
+      </c>
+      <c r="PL14">
+        <v>12</v>
+      </c>
+      <c r="PM14">
+        <v>10</v>
+      </c>
     </row>
-    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -68236,8 +69320,29 @@
       <c r="PF15">
         <v>25</v>
       </c>
+      <c r="PG15">
+        <v>27</v>
+      </c>
+      <c r="PH15">
+        <v>28</v>
+      </c>
+      <c r="PI15">
+        <v>24</v>
+      </c>
+      <c r="PJ15">
+        <v>28</v>
+      </c>
+      <c r="PK15">
+        <v>28</v>
+      </c>
+      <c r="PL15">
+        <v>29</v>
+      </c>
+      <c r="PM15">
+        <v>30</v>
+      </c>
     </row>
-    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -69504,8 +70609,29 @@
       <c r="PF16">
         <v>2</v>
       </c>
+      <c r="PG16">
+        <v>2</v>
+      </c>
+      <c r="PH16">
+        <v>2</v>
+      </c>
+      <c r="PI16">
+        <v>1</v>
+      </c>
+      <c r="PJ16">
+        <v>1</v>
+      </c>
+      <c r="PK16">
+        <v>1</v>
+      </c>
+      <c r="PL16">
+        <v>1</v>
+      </c>
+      <c r="PM16">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -70772,8 +71898,29 @@
       <c r="PF17">
         <v>12</v>
       </c>
+      <c r="PG17">
+        <v>11</v>
+      </c>
+      <c r="PH17">
+        <v>11</v>
+      </c>
+      <c r="PI17">
+        <v>9</v>
+      </c>
+      <c r="PJ17">
+        <v>12</v>
+      </c>
+      <c r="PK17">
+        <v>12</v>
+      </c>
+      <c r="PL17">
+        <v>11</v>
+      </c>
+      <c r="PM17">
+        <v>8</v>
+      </c>
     </row>
-    <row r="18" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -72040,48 +73187,69 @@
       <c r="PF18" s="20">
         <v>1080</v>
       </c>
+      <c r="PG18" s="20">
+        <v>1070</v>
+      </c>
+      <c r="PH18" s="20">
+        <v>1065</v>
+      </c>
+      <c r="PI18" s="20">
+        <v>1009</v>
+      </c>
+      <c r="PJ18" s="20">
+        <v>1056</v>
+      </c>
+      <c r="PK18" s="20">
+        <v>1050</v>
+      </c>
+      <c r="PL18" s="20">
+        <v>1075</v>
+      </c>
+      <c r="PM18" s="20">
+        <v>1083</v>
+      </c>
     </row>
-    <row r="19" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:429" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">
@@ -72092,1177 +73260,1177 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:JP17">
-    <cfRule type="cellIs" dxfId="255" priority="317" operator="lessThan">
+    <cfRule type="cellIs" dxfId="257" priority="317" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DE2:DH2">
-    <cfRule type="cellIs" dxfId="254" priority="316" operator="lessThan">
+    <cfRule type="cellIs" dxfId="256" priority="316" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL2">
-    <cfRule type="cellIs" dxfId="253" priority="236" operator="lessThan">
+    <cfRule type="cellIs" dxfId="255" priority="236" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL2">
-    <cfRule type="cellIs" dxfId="252" priority="235" operator="lessThan">
+    <cfRule type="cellIs" dxfId="254" priority="235" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:JP17 B18:JN18">
-    <cfRule type="cellIs" dxfId="251" priority="238" operator="lessThan">
+    <cfRule type="cellIs" dxfId="253" priority="238" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:JP17">
-    <cfRule type="cellIs" dxfId="250" priority="237" operator="lessThan">
+    <cfRule type="cellIs" dxfId="252" priority="237" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI3:DL18">
-    <cfRule type="cellIs" dxfId="249" priority="234" operator="lessThan">
+    <cfRule type="cellIs" dxfId="251" priority="234" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL17">
-    <cfRule type="cellIs" dxfId="248" priority="233" operator="lessThan">
+    <cfRule type="cellIs" dxfId="250" priority="233" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE2">
-    <cfRule type="cellIs" dxfId="247" priority="232" operator="lessThan">
+    <cfRule type="cellIs" dxfId="249" priority="232" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE2">
-    <cfRule type="cellIs" dxfId="246" priority="231" operator="lessThan">
+    <cfRule type="cellIs" dxfId="248" priority="231" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM3:FE18">
-    <cfRule type="cellIs" dxfId="245" priority="230" operator="lessThan">
+    <cfRule type="cellIs" dxfId="247" priority="230" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE17">
-    <cfRule type="cellIs" dxfId="244" priority="229" operator="lessThan">
+    <cfRule type="cellIs" dxfId="246" priority="229" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2">
-    <cfRule type="cellIs" dxfId="243" priority="228" operator="lessThan">
+    <cfRule type="cellIs" dxfId="245" priority="228" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2">
-    <cfRule type="cellIs" dxfId="242" priority="227" operator="lessThan">
+    <cfRule type="cellIs" dxfId="244" priority="227" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF3:FF18">
-    <cfRule type="cellIs" dxfId="241" priority="226" operator="lessThan">
+    <cfRule type="cellIs" dxfId="243" priority="226" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2:FF17">
-    <cfRule type="cellIs" dxfId="240" priority="225" operator="lessThan">
+    <cfRule type="cellIs" dxfId="242" priority="225" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2">
-    <cfRule type="cellIs" dxfId="239" priority="224" operator="lessThan">
+    <cfRule type="cellIs" dxfId="241" priority="224" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2">
-    <cfRule type="cellIs" dxfId="238" priority="223" operator="lessThan">
+    <cfRule type="cellIs" dxfId="240" priority="223" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG3:FG18">
-    <cfRule type="cellIs" dxfId="237" priority="222" operator="lessThan">
+    <cfRule type="cellIs" dxfId="239" priority="222" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2:FG17">
-    <cfRule type="cellIs" dxfId="236" priority="221" operator="lessThan">
+    <cfRule type="cellIs" dxfId="238" priority="221" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2">
-    <cfRule type="cellIs" dxfId="235" priority="220" operator="lessThan">
+    <cfRule type="cellIs" dxfId="237" priority="220" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2">
-    <cfRule type="cellIs" dxfId="234" priority="219" operator="lessThan">
+    <cfRule type="cellIs" dxfId="236" priority="219" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH3:FH18">
-    <cfRule type="cellIs" dxfId="233" priority="218" operator="lessThan">
+    <cfRule type="cellIs" dxfId="235" priority="218" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2:FH17">
-    <cfRule type="cellIs" dxfId="232" priority="217" operator="lessThan">
+    <cfRule type="cellIs" dxfId="234" priority="217" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2">
-    <cfRule type="cellIs" dxfId="231" priority="216" operator="lessThan">
+    <cfRule type="cellIs" dxfId="233" priority="216" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2">
-    <cfRule type="cellIs" dxfId="230" priority="215" operator="lessThan">
+    <cfRule type="cellIs" dxfId="232" priority="215" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI3:FI18">
-    <cfRule type="cellIs" dxfId="229" priority="214" operator="lessThan">
+    <cfRule type="cellIs" dxfId="231" priority="214" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2:FI17">
-    <cfRule type="cellIs" dxfId="228" priority="213" operator="lessThan">
+    <cfRule type="cellIs" dxfId="230" priority="213" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2">
-    <cfRule type="cellIs" dxfId="227" priority="212" operator="lessThan">
+    <cfRule type="cellIs" dxfId="229" priority="212" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2">
-    <cfRule type="cellIs" dxfId="226" priority="211" operator="lessThan">
+    <cfRule type="cellIs" dxfId="228" priority="211" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ3:FJ18">
-    <cfRule type="cellIs" dxfId="225" priority="210" operator="lessThan">
+    <cfRule type="cellIs" dxfId="227" priority="210" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2:FJ17">
-    <cfRule type="cellIs" dxfId="224" priority="209" operator="lessThan">
+    <cfRule type="cellIs" dxfId="226" priority="209" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2">
-    <cfRule type="cellIs" dxfId="223" priority="208" operator="lessThan">
+    <cfRule type="cellIs" dxfId="225" priority="208" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2">
-    <cfRule type="cellIs" dxfId="222" priority="207" operator="lessThan">
+    <cfRule type="cellIs" dxfId="224" priority="207" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK3:FK18">
-    <cfRule type="cellIs" dxfId="221" priority="206" operator="lessThan">
+    <cfRule type="cellIs" dxfId="223" priority="206" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2:FK17">
-    <cfRule type="cellIs" dxfId="220" priority="205" operator="lessThan">
+    <cfRule type="cellIs" dxfId="222" priority="205" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2">
-    <cfRule type="cellIs" dxfId="219" priority="204" operator="lessThan">
+    <cfRule type="cellIs" dxfId="221" priority="204" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2">
-    <cfRule type="cellIs" dxfId="218" priority="203" operator="lessThan">
+    <cfRule type="cellIs" dxfId="220" priority="203" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL3:FL18">
-    <cfRule type="cellIs" dxfId="217" priority="202" operator="lessThan">
+    <cfRule type="cellIs" dxfId="219" priority="202" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2:FL17">
-    <cfRule type="cellIs" dxfId="216" priority="201" operator="lessThan">
+    <cfRule type="cellIs" dxfId="218" priority="201" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2">
-    <cfRule type="cellIs" dxfId="215" priority="200" operator="lessThan">
+    <cfRule type="cellIs" dxfId="217" priority="200" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2">
-    <cfRule type="cellIs" dxfId="214" priority="199" operator="lessThan">
+    <cfRule type="cellIs" dxfId="216" priority="199" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM3:FM18">
-    <cfRule type="cellIs" dxfId="213" priority="198" operator="lessThan">
+    <cfRule type="cellIs" dxfId="215" priority="198" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2:FM17">
-    <cfRule type="cellIs" dxfId="212" priority="197" operator="lessThan">
+    <cfRule type="cellIs" dxfId="214" priority="197" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2">
-    <cfRule type="cellIs" dxfId="211" priority="196" operator="lessThan">
+    <cfRule type="cellIs" dxfId="213" priority="196" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2">
-    <cfRule type="cellIs" dxfId="210" priority="195" operator="lessThan">
+    <cfRule type="cellIs" dxfId="212" priority="195" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN3:FN18">
-    <cfRule type="cellIs" dxfId="209" priority="194" operator="lessThan">
+    <cfRule type="cellIs" dxfId="211" priority="194" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2:FN17">
-    <cfRule type="cellIs" dxfId="208" priority="193" operator="lessThan">
+    <cfRule type="cellIs" dxfId="210" priority="193" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2">
-    <cfRule type="cellIs" dxfId="207" priority="192" operator="lessThan">
+    <cfRule type="cellIs" dxfId="209" priority="192" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2">
-    <cfRule type="cellIs" dxfId="206" priority="191" operator="lessThan">
+    <cfRule type="cellIs" dxfId="208" priority="191" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO3:FO18">
-    <cfRule type="cellIs" dxfId="205" priority="190" operator="lessThan">
+    <cfRule type="cellIs" dxfId="207" priority="190" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2:FO17">
-    <cfRule type="cellIs" dxfId="204" priority="189" operator="lessThan">
+    <cfRule type="cellIs" dxfId="206" priority="189" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP18:GB18">
-    <cfRule type="cellIs" dxfId="203" priority="188" operator="lessThan">
+    <cfRule type="cellIs" dxfId="205" priority="188" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB2">
-    <cfRule type="cellIs" dxfId="202" priority="187" operator="lessThan">
+    <cfRule type="cellIs" dxfId="204" priority="187" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB2">
-    <cfRule type="cellIs" dxfId="201" priority="186" operator="lessThan">
+    <cfRule type="cellIs" dxfId="203" priority="186" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP3:GB17">
-    <cfRule type="cellIs" dxfId="200" priority="185" operator="lessThan">
+    <cfRule type="cellIs" dxfId="202" priority="185" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB17">
-    <cfRule type="cellIs" dxfId="199" priority="184" operator="lessThan">
+    <cfRule type="cellIs" dxfId="201" priority="184" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC18:GL18">
-    <cfRule type="cellIs" dxfId="198" priority="183" operator="lessThan">
+    <cfRule type="cellIs" dxfId="200" priority="183" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL2">
-    <cfRule type="cellIs" dxfId="197" priority="182" operator="lessThan">
+    <cfRule type="cellIs" dxfId="199" priority="182" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL2">
-    <cfRule type="cellIs" dxfId="196" priority="181" operator="lessThan">
+    <cfRule type="cellIs" dxfId="198" priority="181" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC3:GL17">
-    <cfRule type="cellIs" dxfId="195" priority="180" operator="lessThan">
+    <cfRule type="cellIs" dxfId="197" priority="180" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL17">
-    <cfRule type="cellIs" dxfId="194" priority="179" operator="lessThan">
+    <cfRule type="cellIs" dxfId="196" priority="179" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM18">
-    <cfRule type="cellIs" dxfId="193" priority="178" operator="lessThan">
+    <cfRule type="cellIs" dxfId="195" priority="178" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2">
-    <cfRule type="cellIs" dxfId="192" priority="177" operator="lessThan">
+    <cfRule type="cellIs" dxfId="194" priority="177" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2">
-    <cfRule type="cellIs" dxfId="191" priority="176" operator="lessThan">
+    <cfRule type="cellIs" dxfId="193" priority="176" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM3:GM17">
-    <cfRule type="cellIs" dxfId="190" priority="175" operator="lessThan">
+    <cfRule type="cellIs" dxfId="192" priority="175" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2:GM17">
-    <cfRule type="cellIs" dxfId="189" priority="174" operator="lessThan">
+    <cfRule type="cellIs" dxfId="191" priority="174" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN18">
-    <cfRule type="cellIs" dxfId="188" priority="173" operator="lessThan">
+    <cfRule type="cellIs" dxfId="190" priority="173" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2">
-    <cfRule type="cellIs" dxfId="187" priority="172" operator="lessThan">
+    <cfRule type="cellIs" dxfId="189" priority="172" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2">
-    <cfRule type="cellIs" dxfId="186" priority="171" operator="lessThan">
+    <cfRule type="cellIs" dxfId="188" priority="171" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN3:GN17">
-    <cfRule type="cellIs" dxfId="185" priority="170" operator="lessThan">
+    <cfRule type="cellIs" dxfId="187" priority="170" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2:GN17">
-    <cfRule type="cellIs" dxfId="184" priority="169" operator="lessThan">
+    <cfRule type="cellIs" dxfId="186" priority="169" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO18">
-    <cfRule type="cellIs" dxfId="183" priority="168" operator="lessThan">
+    <cfRule type="cellIs" dxfId="185" priority="168" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2">
-    <cfRule type="cellIs" dxfId="182" priority="167" operator="lessThan">
+    <cfRule type="cellIs" dxfId="184" priority="167" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2">
-    <cfRule type="cellIs" dxfId="181" priority="166" operator="lessThan">
+    <cfRule type="cellIs" dxfId="183" priority="166" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO3:GO17">
-    <cfRule type="cellIs" dxfId="180" priority="165" operator="lessThan">
+    <cfRule type="cellIs" dxfId="182" priority="165" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2:GO17">
-    <cfRule type="cellIs" dxfId="179" priority="164" operator="lessThan">
+    <cfRule type="cellIs" dxfId="181" priority="164" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP18">
-    <cfRule type="cellIs" dxfId="178" priority="163" operator="lessThan">
+    <cfRule type="cellIs" dxfId="180" priority="163" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2">
-    <cfRule type="cellIs" dxfId="177" priority="162" operator="lessThan">
+    <cfRule type="cellIs" dxfId="179" priority="162" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2">
-    <cfRule type="cellIs" dxfId="176" priority="161" operator="lessThan">
+    <cfRule type="cellIs" dxfId="178" priority="161" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP3:GP17">
-    <cfRule type="cellIs" dxfId="175" priority="160" operator="lessThan">
+    <cfRule type="cellIs" dxfId="177" priority="160" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2:GP17">
-    <cfRule type="cellIs" dxfId="174" priority="159" operator="lessThan">
+    <cfRule type="cellIs" dxfId="176" priority="159" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ18:GV18">
-    <cfRule type="cellIs" dxfId="173" priority="158" operator="lessThan">
+    <cfRule type="cellIs" dxfId="175" priority="158" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV2">
-    <cfRule type="cellIs" dxfId="172" priority="157" operator="lessThan">
+    <cfRule type="cellIs" dxfId="174" priority="157" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV2">
-    <cfRule type="cellIs" dxfId="171" priority="156" operator="lessThan">
+    <cfRule type="cellIs" dxfId="173" priority="156" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ3:GV17">
-    <cfRule type="cellIs" dxfId="170" priority="155" operator="lessThan">
+    <cfRule type="cellIs" dxfId="172" priority="155" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV17">
-    <cfRule type="cellIs" dxfId="169" priority="154" operator="lessThan">
+    <cfRule type="cellIs" dxfId="171" priority="154" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW18">
-    <cfRule type="cellIs" dxfId="168" priority="153" operator="lessThan">
+    <cfRule type="cellIs" dxfId="170" priority="153" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2">
-    <cfRule type="cellIs" dxfId="167" priority="152" operator="lessThan">
+    <cfRule type="cellIs" dxfId="169" priority="152" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2">
-    <cfRule type="cellIs" dxfId="166" priority="151" operator="lessThan">
+    <cfRule type="cellIs" dxfId="168" priority="151" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW3:GW17">
-    <cfRule type="cellIs" dxfId="165" priority="150" operator="lessThan">
+    <cfRule type="cellIs" dxfId="167" priority="150" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2:GW17">
-    <cfRule type="cellIs" dxfId="164" priority="149" operator="lessThan">
+    <cfRule type="cellIs" dxfId="166" priority="149" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX18">
-    <cfRule type="cellIs" dxfId="163" priority="148" operator="lessThan">
+    <cfRule type="cellIs" dxfId="165" priority="148" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2">
-    <cfRule type="cellIs" dxfId="162" priority="147" operator="lessThan">
+    <cfRule type="cellIs" dxfId="164" priority="147" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2">
-    <cfRule type="cellIs" dxfId="161" priority="146" operator="lessThan">
+    <cfRule type="cellIs" dxfId="163" priority="146" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX3:GX17">
-    <cfRule type="cellIs" dxfId="160" priority="145" operator="lessThan">
+    <cfRule type="cellIs" dxfId="162" priority="145" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2:GX17">
-    <cfRule type="cellIs" dxfId="159" priority="144" operator="lessThan">
+    <cfRule type="cellIs" dxfId="161" priority="144" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY18">
-    <cfRule type="cellIs" dxfId="158" priority="143" operator="lessThan">
+    <cfRule type="cellIs" dxfId="160" priority="143" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2">
-    <cfRule type="cellIs" dxfId="157" priority="142" operator="lessThan">
+    <cfRule type="cellIs" dxfId="159" priority="142" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2">
-    <cfRule type="cellIs" dxfId="156" priority="141" operator="lessThan">
+    <cfRule type="cellIs" dxfId="158" priority="141" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY3:GY17">
-    <cfRule type="cellIs" dxfId="155" priority="140" operator="lessThan">
+    <cfRule type="cellIs" dxfId="157" priority="140" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2:GY17">
-    <cfRule type="cellIs" dxfId="154" priority="139" operator="lessThan">
+    <cfRule type="cellIs" dxfId="156" priority="139" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ18:HF18">
-    <cfRule type="cellIs" dxfId="153" priority="138" operator="lessThan">
+    <cfRule type="cellIs" dxfId="155" priority="138" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF2">
-    <cfRule type="cellIs" dxfId="152" priority="137" operator="lessThan">
+    <cfRule type="cellIs" dxfId="154" priority="137" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF2">
-    <cfRule type="cellIs" dxfId="151" priority="136" operator="lessThan">
+    <cfRule type="cellIs" dxfId="153" priority="136" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ3:HF17">
-    <cfRule type="cellIs" dxfId="150" priority="135" operator="lessThan">
+    <cfRule type="cellIs" dxfId="152" priority="135" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF17">
-    <cfRule type="cellIs" dxfId="149" priority="134" operator="lessThan">
+    <cfRule type="cellIs" dxfId="151" priority="134" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG18">
-    <cfRule type="cellIs" dxfId="148" priority="128" operator="lessThan">
+    <cfRule type="cellIs" dxfId="150" priority="128" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2">
-    <cfRule type="cellIs" dxfId="147" priority="127" operator="lessThan">
+    <cfRule type="cellIs" dxfId="149" priority="127" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2">
-    <cfRule type="cellIs" dxfId="146" priority="126" operator="lessThan">
+    <cfRule type="cellIs" dxfId="148" priority="126" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG3:HG17">
-    <cfRule type="cellIs" dxfId="145" priority="125" operator="lessThan">
+    <cfRule type="cellIs" dxfId="147" priority="125" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2:HG17">
-    <cfRule type="cellIs" dxfId="144" priority="124" operator="lessThan">
+    <cfRule type="cellIs" dxfId="146" priority="124" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH18">
-    <cfRule type="cellIs" dxfId="143" priority="123" operator="lessThan">
+    <cfRule type="cellIs" dxfId="145" priority="123" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2">
-    <cfRule type="cellIs" dxfId="142" priority="122" operator="lessThan">
+    <cfRule type="cellIs" dxfId="144" priority="122" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2">
-    <cfRule type="cellIs" dxfId="141" priority="121" operator="lessThan">
+    <cfRule type="cellIs" dxfId="143" priority="121" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH3:HH17">
-    <cfRule type="cellIs" dxfId="140" priority="120" operator="lessThan">
+    <cfRule type="cellIs" dxfId="142" priority="120" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2:HH17">
-    <cfRule type="cellIs" dxfId="139" priority="119" operator="lessThan">
+    <cfRule type="cellIs" dxfId="141" priority="119" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI18">
-    <cfRule type="cellIs" dxfId="138" priority="118" operator="lessThan">
+    <cfRule type="cellIs" dxfId="140" priority="118" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2">
-    <cfRule type="cellIs" dxfId="137" priority="117" operator="lessThan">
+    <cfRule type="cellIs" dxfId="139" priority="117" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2">
-    <cfRule type="cellIs" dxfId="136" priority="116" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="116" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI3:HI17">
-    <cfRule type="cellIs" dxfId="135" priority="115" operator="lessThan">
+    <cfRule type="cellIs" dxfId="137" priority="115" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2:HI17">
-    <cfRule type="cellIs" dxfId="134" priority="114" operator="lessThan">
+    <cfRule type="cellIs" dxfId="136" priority="114" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ18">
-    <cfRule type="cellIs" dxfId="133" priority="113" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="113" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2">
-    <cfRule type="cellIs" dxfId="132" priority="112" operator="lessThan">
+    <cfRule type="cellIs" dxfId="134" priority="112" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2">
-    <cfRule type="cellIs" dxfId="131" priority="111" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="111" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ3:HJ17">
-    <cfRule type="cellIs" dxfId="130" priority="110" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="110" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2:HJ17">
-    <cfRule type="cellIs" dxfId="129" priority="109" operator="lessThan">
+    <cfRule type="cellIs" dxfId="131" priority="109" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK18">
-    <cfRule type="cellIs" dxfId="128" priority="108" operator="lessThan">
+    <cfRule type="cellIs" dxfId="130" priority="108" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2">
-    <cfRule type="cellIs" dxfId="127" priority="107" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="107" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2">
-    <cfRule type="cellIs" dxfId="126" priority="106" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="106" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK3:HK17">
-    <cfRule type="cellIs" dxfId="125" priority="105" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="105" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2:HK17">
-    <cfRule type="cellIs" dxfId="124" priority="104" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="104" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL18">
-    <cfRule type="cellIs" dxfId="123" priority="103" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="103" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2">
-    <cfRule type="cellIs" dxfId="122" priority="102" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="102" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2">
-    <cfRule type="cellIs" dxfId="121" priority="101" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="101" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL3:HL17">
-    <cfRule type="cellIs" dxfId="120" priority="100" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="100" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2:HL17">
-    <cfRule type="cellIs" dxfId="119" priority="99" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="99" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM18">
-    <cfRule type="cellIs" dxfId="118" priority="98" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="98" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2">
-    <cfRule type="cellIs" dxfId="117" priority="97" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="97" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2">
-    <cfRule type="cellIs" dxfId="116" priority="96" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="96" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM3:HM17">
-    <cfRule type="cellIs" dxfId="115" priority="95" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="95" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2:HM17">
-    <cfRule type="cellIs" dxfId="114" priority="94" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="94" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN18">
-    <cfRule type="cellIs" dxfId="113" priority="93" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="93" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2">
-    <cfRule type="cellIs" dxfId="112" priority="92" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="92" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2">
-    <cfRule type="cellIs" dxfId="111" priority="91" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="91" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN3:HN17">
-    <cfRule type="cellIs" dxfId="110" priority="90" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="90" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2:HN17">
-    <cfRule type="cellIs" dxfId="109" priority="89" operator="lessThan">
+    <cfRule type="cellIs" dxfId="111" priority="89" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO18">
-    <cfRule type="cellIs" dxfId="108" priority="88" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="88" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2">
-    <cfRule type="cellIs" dxfId="107" priority="87" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="87" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2">
-    <cfRule type="cellIs" dxfId="106" priority="86" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="86" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO3:HO17">
-    <cfRule type="cellIs" dxfId="105" priority="85" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="85" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2:HO17">
-    <cfRule type="cellIs" dxfId="104" priority="84" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="84" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP18">
-    <cfRule type="cellIs" dxfId="103" priority="83" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="83" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2">
-    <cfRule type="cellIs" dxfId="102" priority="82" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="82" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2">
-    <cfRule type="cellIs" dxfId="101" priority="81" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="81" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP3:HP17">
-    <cfRule type="cellIs" dxfId="100" priority="80" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="80" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2:HP17">
-    <cfRule type="cellIs" dxfId="99" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="79" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ18">
-    <cfRule type="cellIs" dxfId="98" priority="78" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="78" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2">
-    <cfRule type="cellIs" dxfId="97" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="77" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2">
-    <cfRule type="cellIs" dxfId="96" priority="76" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="76" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ3:HQ17">
-    <cfRule type="cellIs" dxfId="95" priority="75" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="75" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2:HQ17">
-    <cfRule type="cellIs" dxfId="94" priority="74" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="74" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR18:HZ18">
-    <cfRule type="cellIs" dxfId="93" priority="73" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="73" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ2">
-    <cfRule type="cellIs" dxfId="92" priority="72" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="72" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ2">
-    <cfRule type="cellIs" dxfId="91" priority="71" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="71" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR3:HZ17">
-    <cfRule type="cellIs" dxfId="90" priority="70" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="70" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ17">
-    <cfRule type="cellIs" dxfId="89" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="69" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA18">
-    <cfRule type="cellIs" dxfId="88" priority="68" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="68" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2">
-    <cfRule type="cellIs" dxfId="87" priority="67" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="67" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2">
-    <cfRule type="cellIs" dxfId="86" priority="66" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="66" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA3:IA17">
-    <cfRule type="cellIs" dxfId="85" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="65" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2:IA17">
-    <cfRule type="cellIs" dxfId="84" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="64" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB18:IG18">
-    <cfRule type="cellIs" dxfId="83" priority="63" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="63" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG2">
-    <cfRule type="cellIs" dxfId="82" priority="62" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="62" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG2">
-    <cfRule type="cellIs" dxfId="81" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="61" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB3:IG17">
-    <cfRule type="cellIs" dxfId="80" priority="60" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="60" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG17">
-    <cfRule type="cellIs" dxfId="79" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="59" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH18:IL18">
-    <cfRule type="cellIs" dxfId="78" priority="58" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="58" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL2">
-    <cfRule type="cellIs" dxfId="77" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="57" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL2">
-    <cfRule type="cellIs" dxfId="76" priority="56" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="56" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH3:IL17">
-    <cfRule type="cellIs" dxfId="75" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="55" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL17">
-    <cfRule type="cellIs" dxfId="74" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="54" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM18:IT18">
-    <cfRule type="cellIs" dxfId="73" priority="53" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="53" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT2">
-    <cfRule type="cellIs" dxfId="72" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="52" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT2">
-    <cfRule type="cellIs" dxfId="71" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="51" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM3:IT17">
-    <cfRule type="cellIs" dxfId="70" priority="50" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="50" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT17">
-    <cfRule type="cellIs" dxfId="69" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU18">
-    <cfRule type="cellIs" dxfId="68" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="48" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2">
-    <cfRule type="cellIs" dxfId="67" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="47" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2">
-    <cfRule type="cellIs" dxfId="66" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="46" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU3:IU17">
-    <cfRule type="cellIs" dxfId="65" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="45" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2:IU17">
-    <cfRule type="cellIs" dxfId="64" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="44" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV18">
-    <cfRule type="cellIs" dxfId="63" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="43" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2">
-    <cfRule type="cellIs" dxfId="62" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="42" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2">
-    <cfRule type="cellIs" dxfId="61" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="41" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV3:IV17">
-    <cfRule type="cellIs" dxfId="60" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="40" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2:IV17">
-    <cfRule type="cellIs" dxfId="59" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="39" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW18">
-    <cfRule type="cellIs" dxfId="58" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="38" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2">
-    <cfRule type="cellIs" dxfId="57" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2">
-    <cfRule type="cellIs" dxfId="56" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="36" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW3:IW17">
-    <cfRule type="cellIs" dxfId="55" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2:IW17">
-    <cfRule type="cellIs" dxfId="54" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX18">
-    <cfRule type="cellIs" dxfId="53" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="33" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2">
-    <cfRule type="cellIs" dxfId="52" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="32" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2">
-    <cfRule type="cellIs" dxfId="51" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX3:IX17">
-    <cfRule type="cellIs" dxfId="50" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="30" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2:IX17">
-    <cfRule type="cellIs" dxfId="49" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="29" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY18">
-    <cfRule type="cellIs" dxfId="48" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="28" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2">
-    <cfRule type="cellIs" dxfId="47" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2">
-    <cfRule type="cellIs" dxfId="46" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY3:IY17">
-    <cfRule type="cellIs" dxfId="45" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2:IY17">
-    <cfRule type="cellIs" dxfId="44" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="24" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ18">
-    <cfRule type="cellIs" dxfId="43" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2">
-    <cfRule type="cellIs" dxfId="42" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2">
-    <cfRule type="cellIs" dxfId="41" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ3:IZ17">
-    <cfRule type="cellIs" dxfId="40" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2:IZ17">
-    <cfRule type="cellIs" dxfId="39" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA18">
-    <cfRule type="cellIs" dxfId="38" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2">
-    <cfRule type="cellIs" dxfId="37" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2">
-    <cfRule type="cellIs" dxfId="36" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA3:JA17">
-    <cfRule type="cellIs" dxfId="35" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2:JA17">
-    <cfRule type="cellIs" dxfId="34" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JO18:JU18">
-    <cfRule type="cellIs" dxfId="33" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JQ2:JQ17">
-    <cfRule type="cellIs" dxfId="32" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JQ2:JQ17">
-    <cfRule type="cellIs" dxfId="31" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JR2:JR17">
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JR2:JR17">
-    <cfRule type="cellIs" dxfId="29" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JS2:JS17">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JS2:JS17">
-    <cfRule type="cellIs" dxfId="27" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JT2:JT17">
-    <cfRule type="cellIs" dxfId="26" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JT2:JT17">
-    <cfRule type="cellIs" dxfId="25" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JU2:JU17">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JU2:JU17">
-    <cfRule type="cellIs" dxfId="23" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JV18:KC18">
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="KD18:KP18">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -73273,10 +74441,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PF18"/>
+  <dimension ref="A1:PM18"/>
   <sheetViews>
-    <sheetView topLeftCell="OR1" workbookViewId="0">
-      <selection activeCell="PD21" sqref="PD21"/>
+    <sheetView topLeftCell="PC1" workbookViewId="0">
+      <selection activeCell="PO14" sqref="PO14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73284,7 +74452,7 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -74551,8 +75719,29 @@
       <c r="PF1" s="8">
         <v>44355</v>
       </c>
+      <c r="PG1" s="8">
+        <v>44356</v>
+      </c>
+      <c r="PH1" s="8">
+        <v>44357</v>
+      </c>
+      <c r="PI1" s="8">
+        <v>44358</v>
+      </c>
+      <c r="PJ1" s="8">
+        <v>44359</v>
+      </c>
+      <c r="PK1" s="8">
+        <v>44360</v>
+      </c>
+      <c r="PL1" s="8">
+        <v>44361</v>
+      </c>
+      <c r="PM1" s="8">
+        <v>44362</v>
+      </c>
     </row>
-    <row r="2" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -75819,8 +77008,29 @@
       <c r="PF2">
         <v>9</v>
       </c>
+      <c r="PG2">
+        <v>9</v>
+      </c>
+      <c r="PH2">
+        <v>9</v>
+      </c>
+      <c r="PI2">
+        <v>9</v>
+      </c>
+      <c r="PJ2">
+        <v>9</v>
+      </c>
+      <c r="PK2">
+        <v>9</v>
+      </c>
+      <c r="PL2">
+        <v>9</v>
+      </c>
+      <c r="PM2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -77087,8 +78297,29 @@
       <c r="PF3">
         <v>12</v>
       </c>
+      <c r="PG3">
+        <v>12</v>
+      </c>
+      <c r="PH3">
+        <v>12</v>
+      </c>
+      <c r="PI3">
+        <v>12</v>
+      </c>
+      <c r="PJ3">
+        <v>12</v>
+      </c>
+      <c r="PK3">
+        <v>12</v>
+      </c>
+      <c r="PL3">
+        <v>12</v>
+      </c>
+      <c r="PM3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -78355,8 +79586,29 @@
       <c r="PF4">
         <v>48</v>
       </c>
+      <c r="PG4">
+        <v>48</v>
+      </c>
+      <c r="PH4">
+        <v>48</v>
+      </c>
+      <c r="PI4">
+        <v>48</v>
+      </c>
+      <c r="PJ4">
+        <v>48</v>
+      </c>
+      <c r="PK4">
+        <v>48</v>
+      </c>
+      <c r="PL4">
+        <v>48</v>
+      </c>
+      <c r="PM4">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -79623,8 +80875,29 @@
       <c r="PF5">
         <v>11</v>
       </c>
+      <c r="PG5">
+        <v>11</v>
+      </c>
+      <c r="PH5">
+        <v>11</v>
+      </c>
+      <c r="PI5">
+        <v>11</v>
+      </c>
+      <c r="PJ5">
+        <v>11</v>
+      </c>
+      <c r="PK5">
+        <v>11</v>
+      </c>
+      <c r="PL5">
+        <v>11</v>
+      </c>
+      <c r="PM5">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -80891,8 +82164,29 @@
       <c r="PF6">
         <v>29</v>
       </c>
+      <c r="PG6">
+        <v>29</v>
+      </c>
+      <c r="PH6">
+        <v>29</v>
+      </c>
+      <c r="PI6">
+        <v>29</v>
+      </c>
+      <c r="PJ6">
+        <v>29</v>
+      </c>
+      <c r="PK6">
+        <v>29</v>
+      </c>
+      <c r="PL6">
+        <v>29</v>
+      </c>
+      <c r="PM6">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -82159,8 +83453,29 @@
       <c r="PF7">
         <v>125</v>
       </c>
+      <c r="PG7">
+        <v>125</v>
+      </c>
+      <c r="PH7">
+        <v>125</v>
+      </c>
+      <c r="PI7">
+        <v>125</v>
+      </c>
+      <c r="PJ7">
+        <v>125</v>
+      </c>
+      <c r="PK7">
+        <v>125</v>
+      </c>
+      <c r="PL7">
+        <v>125</v>
+      </c>
+      <c r="PM7">
+        <v>125</v>
+      </c>
     </row>
-    <row r="8" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -83427,8 +84742,29 @@
       <c r="PF8">
         <v>745</v>
       </c>
+      <c r="PG8">
+        <v>745</v>
+      </c>
+      <c r="PH8">
+        <v>745</v>
+      </c>
+      <c r="PI8">
+        <v>745</v>
+      </c>
+      <c r="PJ8">
+        <v>745</v>
+      </c>
+      <c r="PK8">
+        <v>745</v>
+      </c>
+      <c r="PL8">
+        <v>745</v>
+      </c>
+      <c r="PM8">
+        <v>745</v>
+      </c>
     </row>
-    <row r="9" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -84695,8 +86031,29 @@
       <c r="PF9">
         <v>61</v>
       </c>
+      <c r="PG9">
+        <v>61</v>
+      </c>
+      <c r="PH9">
+        <v>61</v>
+      </c>
+      <c r="PI9">
+        <v>61</v>
+      </c>
+      <c r="PJ9">
+        <v>61</v>
+      </c>
+      <c r="PK9">
+        <v>61</v>
+      </c>
+      <c r="PL9">
+        <v>61</v>
+      </c>
+      <c r="PM9">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -85963,8 +87320,29 @@
       <c r="PF10">
         <v>45</v>
       </c>
+      <c r="PG10">
+        <v>45</v>
+      </c>
+      <c r="PH10">
+        <v>45</v>
+      </c>
+      <c r="PI10">
+        <v>45</v>
+      </c>
+      <c r="PJ10">
+        <v>45</v>
+      </c>
+      <c r="PK10">
+        <v>45</v>
+      </c>
+      <c r="PL10">
+        <v>45</v>
+      </c>
+      <c r="PM10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="11" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -87231,8 +88609,29 @@
       <c r="PF11">
         <v>16</v>
       </c>
+      <c r="PG11">
+        <v>16</v>
+      </c>
+      <c r="PH11">
+        <v>16</v>
+      </c>
+      <c r="PI11">
+        <v>16</v>
+      </c>
+      <c r="PJ11">
+        <v>16</v>
+      </c>
+      <c r="PK11">
+        <v>16</v>
+      </c>
+      <c r="PL11">
+        <v>16</v>
+      </c>
+      <c r="PM11">
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -88499,8 +89898,29 @@
       <c r="PF12">
         <v>97</v>
       </c>
+      <c r="PG12">
+        <v>97</v>
+      </c>
+      <c r="PH12">
+        <v>97</v>
+      </c>
+      <c r="PI12">
+        <v>97</v>
+      </c>
+      <c r="PJ12">
+        <v>97</v>
+      </c>
+      <c r="PK12">
+        <v>97</v>
+      </c>
+      <c r="PL12">
+        <v>97</v>
+      </c>
+      <c r="PM12">
+        <v>97</v>
+      </c>
     </row>
-    <row r="13" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -89767,8 +91187,29 @@
       <c r="PF13">
         <v>49</v>
       </c>
+      <c r="PG13">
+        <v>49</v>
+      </c>
+      <c r="PH13">
+        <v>49</v>
+      </c>
+      <c r="PI13">
+        <v>49</v>
+      </c>
+      <c r="PJ13">
+        <v>49</v>
+      </c>
+      <c r="PK13">
+        <v>49</v>
+      </c>
+      <c r="PL13">
+        <v>49</v>
+      </c>
+      <c r="PM13">
+        <v>49</v>
+      </c>
     </row>
-    <row r="14" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -91035,8 +92476,29 @@
       <c r="PF14">
         <v>13</v>
       </c>
+      <c r="PG14">
+        <v>13</v>
+      </c>
+      <c r="PH14">
+        <v>13</v>
+      </c>
+      <c r="PI14">
+        <v>13</v>
+      </c>
+      <c r="PJ14">
+        <v>13</v>
+      </c>
+      <c r="PK14">
+        <v>13</v>
+      </c>
+      <c r="PL14">
+        <v>13</v>
+      </c>
+      <c r="PM14">
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -92303,8 +93765,29 @@
       <c r="PF15">
         <v>49</v>
       </c>
+      <c r="PG15">
+        <v>49</v>
+      </c>
+      <c r="PH15">
+        <v>49</v>
+      </c>
+      <c r="PI15">
+        <v>49</v>
+      </c>
+      <c r="PJ15">
+        <v>49</v>
+      </c>
+      <c r="PK15">
+        <v>49</v>
+      </c>
+      <c r="PL15">
+        <v>49</v>
+      </c>
+      <c r="PM15">
+        <v>49</v>
+      </c>
     </row>
-    <row r="16" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -93571,8 +95054,29 @@
       <c r="PF16">
         <v>8</v>
       </c>
+      <c r="PG16">
+        <v>8</v>
+      </c>
+      <c r="PH16">
+        <v>8</v>
+      </c>
+      <c r="PI16">
+        <v>8</v>
+      </c>
+      <c r="PJ16">
+        <v>8</v>
+      </c>
+      <c r="PK16">
+        <v>8</v>
+      </c>
+      <c r="PL16">
+        <v>8</v>
+      </c>
+      <c r="PM16">
+        <v>8</v>
+      </c>
     </row>
-    <row r="17" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -94839,8 +96343,29 @@
       <c r="PF17">
         <v>14</v>
       </c>
+      <c r="PG17">
+        <v>14</v>
+      </c>
+      <c r="PH17">
+        <v>14</v>
+      </c>
+      <c r="PI17">
+        <v>14</v>
+      </c>
+      <c r="PJ17">
+        <v>14</v>
+      </c>
+      <c r="PK17">
+        <v>14</v>
+      </c>
+      <c r="PL17">
+        <v>14</v>
+      </c>
+      <c r="PM17">
+        <v>14</v>
+      </c>
     </row>
-    <row r="18" spans="1:422" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -96528,110 +98053,143 @@
         <f t="shared" si="17"/>
         <v>1331</v>
       </c>
+      <c r="PG18" s="6">
+        <f t="shared" ref="PG18:PM18" si="18">SUM(PG2:PG17)</f>
+        <v>1331</v>
+      </c>
+      <c r="PH18" s="6">
+        <f t="shared" si="18"/>
+        <v>1331</v>
+      </c>
+      <c r="PI18" s="6">
+        <f t="shared" si="18"/>
+        <v>1331</v>
+      </c>
+      <c r="PJ18" s="6">
+        <f t="shared" si="18"/>
+        <v>1331</v>
+      </c>
+      <c r="PK18" s="6">
+        <f t="shared" si="18"/>
+        <v>1331</v>
+      </c>
+      <c r="PL18" s="6">
+        <f t="shared" si="18"/>
+        <v>1331</v>
+      </c>
+      <c r="PM18" s="6">
+        <f t="shared" si="18"/>
+        <v>1331</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="20" priority="253" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="254" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B18">
-    <cfRule type="cellIs" dxfId="19" priority="251" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="252" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="18" priority="250" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="251" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:MF17">
-    <cfRule type="cellIs" dxfId="17" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:MF18">
-    <cfRule type="cellIs" dxfId="16" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:MF17">
-    <cfRule type="cellIs" dxfId="15" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MG2:MG17">
-    <cfRule type="cellIs" dxfId="14" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MG3:MG18">
-    <cfRule type="cellIs" dxfId="13" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MG2:MG17">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MH18">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MI18:MN18">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MO18:MU18">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="MV18:NB18">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="NC18:NI18">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="NJ18:NP18">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="NQ18:NW18">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="NX18:OD18">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="OE18:OK18">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="OL18:OR18">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="OS18:OY18">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="OZ18:PF18">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="PG18:PM18">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-23-2021 19-15-27
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci_diario.xlsx
+++ b/input/Camas_uci/last_uci_diario.xlsx
@@ -259,7 +259,17 @@
     <cellStyle name="Millares [0] 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="258">
+  <dxfs count="259">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3150,12 +3160,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PM20"/>
+  <dimension ref="A1:PT20"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="PC1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="PK1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="PJ22" sqref="PJ22"/>
+      <selection pane="topRight" activeCell="PN18" sqref="PN18:PT18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3176,7 +3186,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4464,8 +4474,29 @@
       <c r="PM1" s="8">
         <v>44362</v>
       </c>
+      <c r="PN1" s="8">
+        <v>44363</v>
+      </c>
+      <c r="PO1" s="8">
+        <v>44364</v>
+      </c>
+      <c r="PP1" s="8">
+        <v>44365</v>
+      </c>
+      <c r="PQ1" s="8">
+        <v>44366</v>
+      </c>
+      <c r="PR1" s="8">
+        <v>44367</v>
+      </c>
+      <c r="PS1" s="8">
+        <v>44368</v>
+      </c>
+      <c r="PT1" s="8">
+        <v>44369</v>
+      </c>
     </row>
-    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5753,8 +5784,29 @@
       <c r="PM2" s="11">
         <v>33</v>
       </c>
+      <c r="PN2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PO2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PP2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PQ2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PR2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PS2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PT2" s="11">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -7042,8 +7094,29 @@
       <c r="PM3" s="11">
         <v>61</v>
       </c>
+      <c r="PN3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PO3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PP3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PQ3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PR3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PS3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PT3" s="11">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -8331,8 +8404,29 @@
       <c r="PM4" s="11">
         <v>163</v>
       </c>
+      <c r="PN4" s="11">
+        <v>164</v>
+      </c>
+      <c r="PO4" s="11">
+        <v>164</v>
+      </c>
+      <c r="PP4" s="11">
+        <v>162</v>
+      </c>
+      <c r="PQ4" s="11">
+        <v>163</v>
+      </c>
+      <c r="PR4" s="11">
+        <v>163</v>
+      </c>
+      <c r="PS4" s="11">
+        <v>163</v>
+      </c>
+      <c r="PT4" s="11">
+        <v>164</v>
+      </c>
     </row>
-    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -9620,8 +9714,29 @@
       <c r="PM5" s="11">
         <v>34</v>
       </c>
+      <c r="PN5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PO5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PP5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PQ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PR5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PS5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PT5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -10909,8 +11024,29 @@
       <c r="PM6" s="11">
         <v>136</v>
       </c>
+      <c r="PN6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PO6" s="11">
+        <v>134</v>
+      </c>
+      <c r="PP6" s="11">
+        <v>136</v>
+      </c>
+      <c r="PQ6" s="11">
+        <v>136</v>
+      </c>
+      <c r="PR6" s="11">
+        <v>136</v>
+      </c>
+      <c r="PS6" s="11">
+        <v>136</v>
+      </c>
+      <c r="PT6" s="11">
+        <v>135</v>
+      </c>
     </row>
-    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -12198,8 +12334,29 @@
       <c r="PM7" s="11">
         <v>335</v>
       </c>
+      <c r="PN7" s="11">
+        <v>336</v>
+      </c>
+      <c r="PO7" s="11">
+        <v>336</v>
+      </c>
+      <c r="PP7" s="11">
+        <v>335</v>
+      </c>
+      <c r="PQ7" s="11">
+        <v>335</v>
+      </c>
+      <c r="PR7" s="11">
+        <v>333</v>
+      </c>
+      <c r="PS7" s="11">
+        <v>334</v>
+      </c>
+      <c r="PT7" s="11">
+        <v>332</v>
+      </c>
     </row>
-    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -13487,8 +13644,29 @@
       <c r="PM8" s="11">
         <v>2621</v>
       </c>
+      <c r="PN8" s="11">
+        <v>2619</v>
+      </c>
+      <c r="PO8" s="11">
+        <v>2614</v>
+      </c>
+      <c r="PP8" s="11">
+        <v>2615</v>
+      </c>
+      <c r="PQ8" s="11">
+        <v>2614</v>
+      </c>
+      <c r="PR8" s="11">
+        <v>2611</v>
+      </c>
+      <c r="PS8" s="11">
+        <v>2615</v>
+      </c>
+      <c r="PT8" s="11">
+        <v>2613</v>
+      </c>
     </row>
-    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -14776,8 +14954,29 @@
       <c r="PM9" s="11">
         <v>206</v>
       </c>
+      <c r="PN9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PO9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PP9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PQ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PR9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PS9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PT9" s="11">
+        <v>206</v>
+      </c>
     </row>
-    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -16065,8 +16264,29 @@
       <c r="PM10" s="11">
         <v>158</v>
       </c>
+      <c r="PN10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PO10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PP10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PQ10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PR10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PS10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PT10" s="11">
+        <v>158</v>
+      </c>
     </row>
-    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -17354,8 +17574,29 @@
       <c r="PM11" s="11">
         <v>70</v>
       </c>
+      <c r="PN11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PO11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PP11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PQ11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PR11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PS11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PT11" s="11">
+        <v>70</v>
+      </c>
     </row>
-    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -18643,8 +18884,29 @@
       <c r="PM12" s="11">
         <v>311</v>
       </c>
+      <c r="PN12" s="11">
+        <v>312</v>
+      </c>
+      <c r="PO12" s="11">
+        <v>312</v>
+      </c>
+      <c r="PP12" s="11">
+        <v>312</v>
+      </c>
+      <c r="PQ12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PR12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PS12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PT12" s="11">
+        <v>311</v>
+      </c>
     </row>
-    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -19932,8 +20194,29 @@
       <c r="PM13" s="11">
         <v>150</v>
       </c>
+      <c r="PN13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PO13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PP13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PQ13" s="11">
+        <v>148</v>
+      </c>
+      <c r="PR13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PS13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PT13" s="11">
+        <v>150</v>
+      </c>
     </row>
-    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -21221,8 +21504,29 @@
       <c r="PM14" s="11">
         <v>44</v>
       </c>
+      <c r="PN14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PO14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PP14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PQ14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PR14" s="11">
+        <v>44</v>
+      </c>
+      <c r="PS14" s="11">
+        <v>41</v>
+      </c>
+      <c r="PT14" s="11">
+        <v>41</v>
+      </c>
     </row>
-    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -22510,8 +22814,29 @@
       <c r="PM15" s="11">
         <v>139</v>
       </c>
+      <c r="PN15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PO15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PP15" s="11">
+        <v>140</v>
+      </c>
+      <c r="PQ15" s="11">
+        <v>140</v>
+      </c>
+      <c r="PR15" s="11">
+        <v>141</v>
+      </c>
+      <c r="PS15" s="11">
+        <v>141</v>
+      </c>
+      <c r="PT15" s="11">
+        <v>141</v>
+      </c>
     </row>
-    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -23799,8 +24124,29 @@
       <c r="PM16" s="11">
         <v>17</v>
       </c>
+      <c r="PN16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PO16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PP16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PQ16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PR16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PS16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PT16" s="11">
+        <v>17</v>
+      </c>
     </row>
-    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -25088,8 +25434,29 @@
       <c r="PM17" s="11">
         <v>47</v>
       </c>
+      <c r="PN17" s="11">
+        <v>47</v>
+      </c>
+      <c r="PO17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PP17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PQ17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PR17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PS17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PT17" s="11">
+        <v>43</v>
+      </c>
     </row>
-    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -26509,7 +26876,7 @@
         <v>4498</v>
       </c>
       <c r="PH18" s="6">
-        <f t="shared" ref="PH18:PM18" si="8">SUM(PH2:PH17)</f>
+        <f t="shared" ref="PH18:PT18" si="8">SUM(PH2:PH17)</f>
         <v>4513</v>
       </c>
       <c r="PI18" s="6">
@@ -26532,13 +26899,41 @@
         <f t="shared" si="8"/>
         <v>4525</v>
       </c>
+      <c r="PN18" s="6">
+        <f t="shared" si="8"/>
+        <v>4525</v>
+      </c>
+      <c r="PO18" s="6">
+        <f t="shared" si="8"/>
+        <v>4515</v>
+      </c>
+      <c r="PP18" s="6">
+        <f t="shared" si="8"/>
+        <v>4516</v>
+      </c>
+      <c r="PQ18" s="6">
+        <f t="shared" si="8"/>
+        <v>4513</v>
+      </c>
+      <c r="PR18" s="6">
+        <f t="shared" si="8"/>
+        <v>4511</v>
+      </c>
+      <c r="PS18" s="6">
+        <f t="shared" si="8"/>
+        <v>4513</v>
+      </c>
+      <c r="PT18" s="6">
+        <f t="shared" si="8"/>
+        <v>4509</v>
+      </c>
     </row>
-    <row r="19" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:436" x14ac:dyDescent="0.25">
       <c r="HV19" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:436" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -26556,12 +26951,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PM34"/>
+  <dimension ref="A1:PT34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="PD1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="PJ1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="PG18" sqref="PG18:PM18"/>
+      <selection pane="topRight" activeCell="PU13" sqref="PU13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26581,7 +26976,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -27869,8 +28264,29 @@
       <c r="PM1" s="8">
         <v>44362</v>
       </c>
+      <c r="PN1" s="8">
+        <v>44363</v>
+      </c>
+      <c r="PO1" s="8">
+        <v>44364</v>
+      </c>
+      <c r="PP1" s="8">
+        <v>44365</v>
+      </c>
+      <c r="PQ1" s="8">
+        <v>44366</v>
+      </c>
+      <c r="PR1" s="8">
+        <v>44367</v>
+      </c>
+      <c r="PS1" s="8">
+        <v>44368</v>
+      </c>
+      <c r="PT1" s="8">
+        <v>44369</v>
+      </c>
     </row>
-    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -29158,8 +29574,29 @@
       <c r="PM2">
         <v>25</v>
       </c>
+      <c r="PN2">
+        <v>27</v>
+      </c>
+      <c r="PO2">
+        <v>26</v>
+      </c>
+      <c r="PP2">
+        <v>26</v>
+      </c>
+      <c r="PQ2">
+        <v>26</v>
+      </c>
+      <c r="PR2">
+        <v>26</v>
+      </c>
+      <c r="PS2">
+        <v>28</v>
+      </c>
+      <c r="PT2">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -30447,8 +30884,29 @@
       <c r="PM3">
         <v>53</v>
       </c>
+      <c r="PN3">
+        <v>55</v>
+      </c>
+      <c r="PO3">
+        <v>54</v>
+      </c>
+      <c r="PP3">
+        <v>54</v>
+      </c>
+      <c r="PQ3">
+        <v>53</v>
+      </c>
+      <c r="PR3">
+        <v>52</v>
+      </c>
+      <c r="PS3">
+        <v>58</v>
+      </c>
+      <c r="PT3">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -31736,8 +32194,29 @@
       <c r="PM4">
         <v>90</v>
       </c>
+      <c r="PN4">
+        <v>90</v>
+      </c>
+      <c r="PO4">
+        <v>88</v>
+      </c>
+      <c r="PP4">
+        <v>89</v>
+      </c>
+      <c r="PQ4">
+        <v>91</v>
+      </c>
+      <c r="PR4">
+        <v>89</v>
+      </c>
+      <c r="PS4">
+        <v>96</v>
+      </c>
+      <c r="PT4">
+        <v>96</v>
+      </c>
     </row>
-    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -33025,8 +33504,29 @@
       <c r="PM5">
         <v>24</v>
       </c>
+      <c r="PN5">
+        <v>26</v>
+      </c>
+      <c r="PO5">
+        <v>25</v>
+      </c>
+      <c r="PP5">
+        <v>25</v>
+      </c>
+      <c r="PQ5">
+        <v>26</v>
+      </c>
+      <c r="PR5">
+        <v>28</v>
+      </c>
+      <c r="PS5">
+        <v>27</v>
+      </c>
+      <c r="PT5">
+        <v>28</v>
+      </c>
     </row>
-    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -34314,8 +34814,29 @@
       <c r="PM6">
         <v>104</v>
       </c>
+      <c r="PN6">
+        <v>103</v>
+      </c>
+      <c r="PO6">
+        <v>103</v>
+      </c>
+      <c r="PP6">
+        <v>104</v>
+      </c>
+      <c r="PQ6">
+        <v>105</v>
+      </c>
+      <c r="PR6">
+        <v>101</v>
+      </c>
+      <c r="PS6">
+        <v>102</v>
+      </c>
+      <c r="PT6">
+        <v>101</v>
+      </c>
     </row>
-    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -35603,8 +36124,29 @@
       <c r="PM7">
         <v>223</v>
       </c>
+      <c r="PN7">
+        <v>222</v>
+      </c>
+      <c r="PO7">
+        <v>222</v>
+      </c>
+      <c r="PP7">
+        <v>226</v>
+      </c>
+      <c r="PQ7">
+        <v>223</v>
+      </c>
+      <c r="PR7">
+        <v>216</v>
+      </c>
+      <c r="PS7">
+        <v>216</v>
+      </c>
+      <c r="PT7">
+        <v>210</v>
+      </c>
     </row>
-    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -36892,8 +37434,29 @@
       <c r="PM8">
         <v>1974</v>
       </c>
+      <c r="PN8">
+        <v>1992</v>
+      </c>
+      <c r="PO8">
+        <v>1985</v>
+      </c>
+      <c r="PP8">
+        <v>1975</v>
+      </c>
+      <c r="PQ8">
+        <v>1971</v>
+      </c>
+      <c r="PR8">
+        <v>1948</v>
+      </c>
+      <c r="PS8">
+        <v>1942</v>
+      </c>
+      <c r="PT8">
+        <v>1950</v>
+      </c>
     </row>
-    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -38181,8 +38744,29 @@
       <c r="PM9">
         <v>151</v>
       </c>
+      <c r="PN9">
+        <v>157</v>
+      </c>
+      <c r="PO9">
+        <v>165</v>
+      </c>
+      <c r="PP9">
+        <v>159</v>
+      </c>
+      <c r="PQ9">
+        <v>160</v>
+      </c>
+      <c r="PR9">
+        <v>160</v>
+      </c>
+      <c r="PS9">
+        <v>162</v>
+      </c>
+      <c r="PT9">
+        <v>161</v>
+      </c>
     </row>
-    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -39470,8 +40054,29 @@
       <c r="PM10">
         <v>108</v>
       </c>
+      <c r="PN10">
+        <v>111</v>
+      </c>
+      <c r="PO10">
+        <v>111</v>
+      </c>
+      <c r="PP10">
+        <v>113</v>
+      </c>
+      <c r="PQ10">
+        <v>113</v>
+      </c>
+      <c r="PR10">
+        <v>109</v>
+      </c>
+      <c r="PS10">
+        <v>109</v>
+      </c>
+      <c r="PT10">
+        <v>116</v>
+      </c>
     </row>
-    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -40759,8 +41364,29 @@
       <c r="PM11">
         <v>46</v>
       </c>
+      <c r="PN11">
+        <v>47</v>
+      </c>
+      <c r="PO11">
+        <v>49</v>
+      </c>
+      <c r="PP11">
+        <v>46</v>
+      </c>
+      <c r="PQ11">
+        <v>45</v>
+      </c>
+      <c r="PR11">
+        <v>46</v>
+      </c>
+      <c r="PS11">
+        <v>44</v>
+      </c>
+      <c r="PT11">
+        <v>43</v>
+      </c>
     </row>
-    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -42048,8 +42674,29 @@
       <c r="PM12">
         <v>200</v>
       </c>
+      <c r="PN12">
+        <v>196</v>
+      </c>
+      <c r="PO12">
+        <v>198</v>
+      </c>
+      <c r="PP12">
+        <v>196</v>
+      </c>
+      <c r="PQ12">
+        <v>193</v>
+      </c>
+      <c r="PR12">
+        <v>186</v>
+      </c>
+      <c r="PS12">
+        <v>186</v>
+      </c>
+      <c r="PT12">
+        <v>183</v>
+      </c>
     </row>
-    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -43337,8 +43984,29 @@
       <c r="PM13">
         <v>103</v>
       </c>
+      <c r="PN13">
+        <v>106</v>
+      </c>
+      <c r="PO13">
+        <v>107</v>
+      </c>
+      <c r="PP13">
+        <v>107</v>
+      </c>
+      <c r="PQ13">
+        <v>105</v>
+      </c>
+      <c r="PR13">
+        <v>106</v>
+      </c>
+      <c r="PS13">
+        <v>105</v>
+      </c>
+      <c r="PT13">
+        <v>105</v>
+      </c>
     </row>
-    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -44626,8 +45294,29 @@
       <c r="PM14">
         <v>29</v>
       </c>
+      <c r="PN14">
+        <v>27</v>
+      </c>
+      <c r="PO14">
+        <v>26</v>
+      </c>
+      <c r="PP14">
+        <v>26</v>
+      </c>
+      <c r="PQ14">
+        <v>24</v>
+      </c>
+      <c r="PR14">
+        <v>26</v>
+      </c>
+      <c r="PS14">
+        <v>24</v>
+      </c>
+      <c r="PT14">
+        <v>24</v>
+      </c>
     </row>
-    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -45915,8 +46604,29 @@
       <c r="PM15">
         <v>103</v>
       </c>
+      <c r="PN15">
+        <v>101</v>
+      </c>
+      <c r="PO15">
+        <v>103</v>
+      </c>
+      <c r="PP15">
+        <v>103</v>
+      </c>
+      <c r="PQ15">
+        <v>100</v>
+      </c>
+      <c r="PR15">
+        <v>99</v>
+      </c>
+      <c r="PS15">
+        <v>101</v>
+      </c>
+      <c r="PT15">
+        <v>100</v>
+      </c>
     </row>
-    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -47204,8 +47914,29 @@
       <c r="PM16">
         <v>13</v>
       </c>
+      <c r="PN16">
+        <v>13</v>
+      </c>
+      <c r="PO16">
+        <v>11</v>
+      </c>
+      <c r="PP16">
+        <v>10</v>
+      </c>
+      <c r="PQ16">
+        <v>13</v>
+      </c>
+      <c r="PR16">
+        <v>12</v>
+      </c>
+      <c r="PS16">
+        <v>12</v>
+      </c>
+      <c r="PT16">
+        <v>12</v>
+      </c>
     </row>
-    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -48493,8 +49224,29 @@
       <c r="PM17">
         <v>29</v>
       </c>
+      <c r="PN17">
+        <v>28</v>
+      </c>
+      <c r="PO17">
+        <v>29</v>
+      </c>
+      <c r="PP17">
+        <v>27</v>
+      </c>
+      <c r="PQ17">
+        <v>27</v>
+      </c>
+      <c r="PR17">
+        <v>26</v>
+      </c>
+      <c r="PS17">
+        <v>24</v>
+      </c>
+      <c r="PT17">
+        <v>23</v>
+      </c>
     </row>
-    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -49922,50 +50674,71 @@
         <f t="shared" si="2"/>
         <v>3275</v>
       </c>
+      <c r="PN18" s="6">
+        <v>3301</v>
+      </c>
+      <c r="PO18" s="6">
+        <v>3302</v>
+      </c>
+      <c r="PP18" s="6">
+        <v>3286</v>
+      </c>
+      <c r="PQ18" s="6">
+        <v>3275</v>
+      </c>
+      <c r="PR18" s="6">
+        <v>3230</v>
+      </c>
+      <c r="PS18" s="6">
+        <v>3236</v>
+      </c>
+      <c r="PT18" s="6">
+        <v>3232</v>
+      </c>
     </row>
-    <row r="19" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:436" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:436" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:436" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:436" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -49985,12 +50758,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:PM34"/>
+  <dimension ref="A1:PT34"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="PC1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="PJ1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="PM22" sqref="PM22"/>
+      <selection pane="topRight" activeCell="PN18" sqref="PN18:PT18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50007,7 +50780,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -51295,8 +52068,29 @@
       <c r="PM1" s="8">
         <v>44362</v>
       </c>
+      <c r="PN1" s="8">
+        <v>44363</v>
+      </c>
+      <c r="PO1" s="8">
+        <v>44364</v>
+      </c>
+      <c r="PP1" s="8">
+        <v>44365</v>
+      </c>
+      <c r="PQ1" s="8">
+        <v>44366</v>
+      </c>
+      <c r="PR1" s="8">
+        <v>44367</v>
+      </c>
+      <c r="PS1" s="8">
+        <v>44368</v>
+      </c>
+      <c r="PT1" s="8">
+        <v>44369</v>
+      </c>
     </row>
-    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -52584,8 +53378,29 @@
       <c r="PM2">
         <v>3</v>
       </c>
+      <c r="PN2">
+        <v>3</v>
+      </c>
+      <c r="PO2">
+        <v>3</v>
+      </c>
+      <c r="PP2">
+        <v>3</v>
+      </c>
+      <c r="PQ2">
+        <v>3</v>
+      </c>
+      <c r="PR2">
+        <v>3</v>
+      </c>
+      <c r="PS2">
+        <v>3</v>
+      </c>
+      <c r="PT2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -53873,8 +54688,29 @@
       <c r="PM3">
         <v>7</v>
       </c>
+      <c r="PN3">
+        <v>5</v>
+      </c>
+      <c r="PO3">
+        <v>6</v>
+      </c>
+      <c r="PP3">
+        <v>5</v>
+      </c>
+      <c r="PQ3">
+        <v>7</v>
+      </c>
+      <c r="PR3">
+        <v>8</v>
+      </c>
+      <c r="PS3">
+        <v>1</v>
+      </c>
+      <c r="PT3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -55162,8 +55998,29 @@
       <c r="PM4">
         <v>66</v>
       </c>
+      <c r="PN4">
+        <v>63</v>
+      </c>
+      <c r="PO4">
+        <v>62</v>
+      </c>
+      <c r="PP4">
+        <v>62</v>
+      </c>
+      <c r="PQ4">
+        <v>56</v>
+      </c>
+      <c r="PR4">
+        <v>61</v>
+      </c>
+      <c r="PS4">
+        <v>58</v>
+      </c>
+      <c r="PT4">
+        <v>60</v>
+      </c>
     </row>
-    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -56451,8 +57308,29 @@
       <c r="PM5">
         <v>5</v>
       </c>
+      <c r="PN5">
+        <v>5</v>
+      </c>
+      <c r="PO5">
+        <v>5</v>
+      </c>
+      <c r="PP5">
+        <v>5</v>
+      </c>
+      <c r="PQ5">
+        <v>6</v>
+      </c>
+      <c r="PR5">
+        <v>4</v>
+      </c>
+      <c r="PS5">
+        <v>5</v>
+      </c>
+      <c r="PT5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -57740,8 +58618,29 @@
       <c r="PM6">
         <v>30</v>
       </c>
+      <c r="PN6">
+        <v>25</v>
+      </c>
+      <c r="PO6">
+        <v>24</v>
+      </c>
+      <c r="PP6">
+        <v>27</v>
+      </c>
+      <c r="PQ6">
+        <v>28</v>
+      </c>
+      <c r="PR6">
+        <v>30</v>
+      </c>
+      <c r="PS6">
+        <v>28</v>
+      </c>
+      <c r="PT6">
+        <v>30</v>
+      </c>
     </row>
-    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -59029,8 +59928,29 @@
       <c r="PM7">
         <v>99</v>
       </c>
+      <c r="PN7">
+        <v>104</v>
+      </c>
+      <c r="PO7">
+        <v>106</v>
+      </c>
+      <c r="PP7">
+        <v>103</v>
+      </c>
+      <c r="PQ7">
+        <v>103</v>
+      </c>
+      <c r="PR7">
+        <v>109</v>
+      </c>
+      <c r="PS7">
+        <v>100</v>
+      </c>
+      <c r="PT7">
+        <v>104</v>
+      </c>
     </row>
-    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -60318,8 +61238,29 @@
       <c r="PM8">
         <v>612</v>
       </c>
+      <c r="PN8">
+        <v>591</v>
+      </c>
+      <c r="PO8">
+        <v>594</v>
+      </c>
+      <c r="PP8">
+        <v>585</v>
+      </c>
+      <c r="PQ8">
+        <v>592</v>
+      </c>
+      <c r="PR8">
+        <v>600</v>
+      </c>
+      <c r="PS8">
+        <v>611</v>
+      </c>
+      <c r="PT8">
+        <v>606</v>
+      </c>
     </row>
-    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -61607,8 +62548,29 @@
       <c r="PM9">
         <v>34</v>
       </c>
+      <c r="PN9">
+        <v>24</v>
+      </c>
+      <c r="PO9">
+        <v>19</v>
+      </c>
+      <c r="PP9">
+        <v>28</v>
+      </c>
+      <c r="PQ9">
+        <v>24</v>
+      </c>
+      <c r="PR9">
+        <v>27</v>
+      </c>
+      <c r="PS9">
+        <v>21</v>
+      </c>
+      <c r="PT9">
+        <v>27</v>
+      </c>
     </row>
-    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -62896,8 +63858,29 @@
       <c r="PM10">
         <v>26</v>
       </c>
+      <c r="PN10">
+        <v>24</v>
+      </c>
+      <c r="PO10">
+        <v>26</v>
+      </c>
+      <c r="PP10">
+        <v>23</v>
+      </c>
+      <c r="PQ10">
+        <v>25</v>
+      </c>
+      <c r="PR10">
+        <v>26</v>
+      </c>
+      <c r="PS10">
+        <v>22</v>
+      </c>
+      <c r="PT10">
+        <v>17</v>
+      </c>
     </row>
-    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -64185,8 +65168,29 @@
       <c r="PM11">
         <v>14</v>
       </c>
+      <c r="PN11">
+        <v>14</v>
+      </c>
+      <c r="PO11">
+        <v>16</v>
+      </c>
+      <c r="PP11">
+        <v>17</v>
+      </c>
+      <c r="PQ11">
+        <v>16</v>
+      </c>
+      <c r="PR11">
+        <v>17</v>
+      </c>
+      <c r="PS11">
+        <v>15</v>
+      </c>
+      <c r="PT11">
+        <v>18</v>
+      </c>
     </row>
-    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -65474,8 +66478,29 @@
       <c r="PM12">
         <v>94</v>
       </c>
+      <c r="PN12">
+        <v>94</v>
+      </c>
+      <c r="PO12">
+        <v>92</v>
+      </c>
+      <c r="PP12">
+        <v>97</v>
+      </c>
+      <c r="PQ12">
+        <v>94</v>
+      </c>
+      <c r="PR12">
+        <v>91</v>
+      </c>
+      <c r="PS12">
+        <v>98</v>
+      </c>
+      <c r="PT12">
+        <v>103</v>
+      </c>
     </row>
-    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -66763,8 +67788,29 @@
       <c r="PM13">
         <v>44</v>
       </c>
+      <c r="PN13">
+        <v>37</v>
+      </c>
+      <c r="PO13">
+        <v>34</v>
+      </c>
+      <c r="PP13">
+        <v>35</v>
+      </c>
+      <c r="PQ13">
+        <v>36</v>
+      </c>
+      <c r="PR13">
+        <v>30</v>
+      </c>
+      <c r="PS13">
+        <v>31</v>
+      </c>
+      <c r="PT13">
+        <v>32</v>
+      </c>
     </row>
-    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -68052,8 +69098,29 @@
       <c r="PM14">
         <v>10</v>
       </c>
+      <c r="PN14">
+        <v>16</v>
+      </c>
+      <c r="PO14">
+        <v>15</v>
+      </c>
+      <c r="PP14">
+        <v>15</v>
+      </c>
+      <c r="PQ14">
+        <v>15</v>
+      </c>
+      <c r="PR14">
+        <v>16</v>
+      </c>
+      <c r="PS14">
+        <v>15</v>
+      </c>
+      <c r="PT14">
+        <v>14</v>
+      </c>
     </row>
-    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -69341,8 +70408,29 @@
       <c r="PM15">
         <v>30</v>
       </c>
+      <c r="PN15">
+        <v>28</v>
+      </c>
+      <c r="PO15">
+        <v>29</v>
+      </c>
+      <c r="PP15">
+        <v>29</v>
+      </c>
+      <c r="PQ15">
+        <v>35</v>
+      </c>
+      <c r="PR15">
+        <v>32</v>
+      </c>
+      <c r="PS15">
+        <v>33</v>
+      </c>
+      <c r="PT15">
+        <v>33</v>
+      </c>
     </row>
-    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -70630,8 +71718,29 @@
       <c r="PM16">
         <v>1</v>
       </c>
+      <c r="PN16">
+        <v>1</v>
+      </c>
+      <c r="PO16">
+        <v>1</v>
+      </c>
+      <c r="PP16">
+        <v>1</v>
+      </c>
+      <c r="PQ16">
+        <v>1</v>
+      </c>
+      <c r="PR16">
+        <v>1</v>
+      </c>
+      <c r="PS16">
+        <v>1</v>
+      </c>
+      <c r="PT16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -71919,8 +73028,29 @@
       <c r="PM17">
         <v>8</v>
       </c>
+      <c r="PN17">
+        <v>7</v>
+      </c>
+      <c r="PO17">
+        <v>6</v>
+      </c>
+      <c r="PP17">
+        <v>7</v>
+      </c>
+      <c r="PQ17">
+        <v>6</v>
+      </c>
+      <c r="PR17">
+        <v>6</v>
+      </c>
+      <c r="PS17">
+        <v>8</v>
+      </c>
+      <c r="PT17">
+        <v>8</v>
+      </c>
     </row>
-    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -73208,48 +74338,69 @@
       <c r="PM18" s="20">
         <v>1083</v>
       </c>
+      <c r="PN18" s="20">
+        <v>1041</v>
+      </c>
+      <c r="PO18" s="20">
+        <v>1038</v>
+      </c>
+      <c r="PP18" s="20">
+        <v>1042</v>
+      </c>
+      <c r="PQ18" s="20">
+        <v>1047</v>
+      </c>
+      <c r="PR18" s="20">
+        <v>1061</v>
+      </c>
+      <c r="PS18" s="20">
+        <v>1050</v>
+      </c>
+      <c r="PT18" s="20">
+        <v>1067</v>
+      </c>
     </row>
-    <row r="19" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:436" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">
@@ -73260,1177 +74411,1177 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:JP17">
-    <cfRule type="cellIs" dxfId="257" priority="317" operator="lessThan">
+    <cfRule type="cellIs" dxfId="258" priority="317" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DE2:DH2">
-    <cfRule type="cellIs" dxfId="256" priority="316" operator="lessThan">
+    <cfRule type="cellIs" dxfId="257" priority="316" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL2">
-    <cfRule type="cellIs" dxfId="255" priority="236" operator="lessThan">
+    <cfRule type="cellIs" dxfId="256" priority="236" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL2">
-    <cfRule type="cellIs" dxfId="254" priority="235" operator="lessThan">
+    <cfRule type="cellIs" dxfId="255" priority="235" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:JP17 B18:JN18">
-    <cfRule type="cellIs" dxfId="253" priority="238" operator="lessThan">
+    <cfRule type="cellIs" dxfId="254" priority="238" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:JP17">
-    <cfRule type="cellIs" dxfId="252" priority="237" operator="lessThan">
+    <cfRule type="cellIs" dxfId="253" priority="237" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI3:DL18">
-    <cfRule type="cellIs" dxfId="251" priority="234" operator="lessThan">
+    <cfRule type="cellIs" dxfId="252" priority="234" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL17">
-    <cfRule type="cellIs" dxfId="250" priority="233" operator="lessThan">
+    <cfRule type="cellIs" dxfId="251" priority="233" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE2">
-    <cfRule type="cellIs" dxfId="249" priority="232" operator="lessThan">
+    <cfRule type="cellIs" dxfId="250" priority="232" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE2">
-    <cfRule type="cellIs" dxfId="248" priority="231" operator="lessThan">
+    <cfRule type="cellIs" dxfId="249" priority="231" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM3:FE18">
-    <cfRule type="cellIs" dxfId="247" priority="230" operator="lessThan">
+    <cfRule type="cellIs" dxfId="248" priority="230" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE17">
-    <cfRule type="cellIs" dxfId="246" priority="229" operator="lessThan">
+    <cfRule type="cellIs" dxfId="247" priority="229" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2">
-    <cfRule type="cellIs" dxfId="245" priority="228" operator="lessThan">
+    <cfRule type="cellIs" dxfId="246" priority="228" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2">
-    <cfRule type="cellIs" dxfId="244" priority="227" operator="lessThan">
+    <cfRule type="cellIs" dxfId="245" priority="227" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF3:FF18">
-    <cfRule type="cellIs" dxfId="243" priority="226" operator="lessThan">
+    <cfRule type="cellIs" dxfId="244" priority="226" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2:FF17">
-    <cfRule type="cellIs" dxfId="242" priority="225" operator="lessThan">
+    <cfRule type="cellIs" dxfId="243" priority="225" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2">
-    <cfRule type="cellIs" dxfId="241" priority="224" operator="lessThan">
+    <cfRule type="cellIs" dxfId="242" priority="224" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2">
-    <cfRule type="cellIs" dxfId="240" priority="223" operator="lessThan">
+    <cfRule type="cellIs" dxfId="241" priority="223" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG3:FG18">
-    <cfRule type="cellIs" dxfId="239" priority="222" operator="lessThan">
+    <cfRule type="cellIs" dxfId="240" priority="222" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2:FG17">
-    <cfRule type="cellIs" dxfId="238" priority="221" operator="lessThan">
+    <cfRule type="cellIs" dxfId="239" priority="221" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2">
-    <cfRule type="cellIs" dxfId="237" priority="220" operator="lessThan">
+    <cfRule type="cellIs" dxfId="238" priority="220" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2">
-    <cfRule type="cellIs" dxfId="236" priority="219" operator="lessThan">
+    <cfRule type="cellIs" dxfId="237" priority="219" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH3:FH18">
-    <cfRule type="cellIs" dxfId="235" priority="218" operator="lessThan">
+    <cfRule type="cellIs" dxfId="236" priority="218" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2:FH17">
-    <cfRule type="cellIs" dxfId="234" priority="217" operator="lessThan">
+    <cfRule type="cellIs" dxfId="235" priority="217" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2">
-    <cfRule type="cellIs" dxfId="233" priority="216" operator="lessThan">
+    <cfRule type="cellIs" dxfId="234" priority="216" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2">
-    <cfRule type="cellIs" dxfId="232" priority="215" operator="lessThan">
+    <cfRule type="cellIs" dxfId="233" priority="215" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI3:FI18">
-    <cfRule type="cellIs" dxfId="231" priority="214" operator="lessThan">
+    <cfRule type="cellIs" dxfId="232" priority="214" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2:FI17">
-    <cfRule type="cellIs" dxfId="230" priority="213" operator="lessThan">
+    <cfRule type="cellIs" dxfId="231" priority="213" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2">
-    <cfRule type="cellIs" dxfId="229" priority="212" operator="lessThan">
+    <cfRule type="cellIs" dxfId="230" priority="212" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2">
-    <cfRule type="cellIs" dxfId="228" priority="211" operator="lessThan">
+    <cfRule type="cellIs" dxfId="229" priority="211" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ3:FJ18">
-    <cfRule type="cellIs" dxfId="227" priority="210" operator="lessThan">
+    <cfRule type="cellIs" dxfId="228" priority="210" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2:FJ17">
-    <cfRule type="cellIs" dxfId="226" priority="209" operator="lessThan">
+    <cfRule type="cellIs" dxfId="227" priority="209" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2">
-    <cfRule type="cellIs" dxfId="225" priority="208" operator="lessThan">
+    <cfRule type="cellIs" dxfId="226" priority="208" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2">
-    <cfRule type="cellIs" dxfId="224" priority="207" operator="lessThan">
+    <cfRule type="cellIs" dxfId="225" priority="207" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK3:FK18">
-    <cfRule type="cellIs" dxfId="223" priority="206" operator="lessThan">
+    <cfRule type="cellIs" dxfId="224" priority="206" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2:FK17">
-    <cfRule type="cellIs" dxfId="222" priority="205" operator="lessThan">
+    <cfRule type="cellIs" dxfId="223" priority="205" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2">
-    <cfRule type="cellIs" dxfId="221" priority="204" operator="lessThan">
+    <cfRule type="cellIs" dxfId="222" priority="204" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2">
-    <cfRule type="cellIs" dxfId="220" priority="203" operator="lessThan">
+    <cfRule type="cellIs" dxfId="221" priority="203" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL3:FL18">
-    <cfRule type="cellIs" dxfId="219" priority="202" operator="lessThan">
+    <cfRule type="cellIs" dxfId="220" priority="202" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2:FL17">
-    <cfRule type="cellIs" dxfId="218" priority="201" operator="lessThan">
+    <cfRule type="cellIs" dxfId="219" priority="201" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2">
-    <cfRule type="cellIs" dxfId="217" priority="200" operator="lessThan">
+    <cfRule type="cellIs" dxfId="218" priority="200" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2">
-    <cfRule type="cellIs" dxfId="216" priority="199" operator="lessThan">
+    <cfRule type="cellIs" dxfId="217" priority="199" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM3:FM18">
-    <cfRule type="cellIs" dxfId="215" priority="198" operator="lessThan">
+    <cfRule type="cellIs" dxfId="216" priority="198" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2:FM17">
-    <cfRule type="cellIs" dxfId="214" priority="197" operator="lessThan">
+    <cfRule type="cellIs" dxfId="215" priority="197" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2">
-    <cfRule type="cellIs" dxfId="213" priority="196" operator="lessThan">
+    <cfRule type="cellIs" dxfId="214" priority="196" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2">
-    <cfRule type="cellIs" dxfId="212" priority="195" operator="lessThan">
+    <cfRule type="cellIs" dxfId="213" priority="195" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN3:FN18">
-    <cfRule type="cellIs" dxfId="211" priority="194" operator="lessThan">
+    <cfRule type="cellIs" dxfId="212" priority="194" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2:FN17">
-    <cfRule type="cellIs" dxfId="210" priority="193" operator="lessThan">
+    <cfRule type="cellIs" dxfId="211" priority="193" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2">
-    <cfRule type="cellIs" dxfId="209" priority="192" operator="lessThan">
+    <cfRule type="cellIs" dxfId="210" priority="192" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2">
-    <cfRule type="cellIs" dxfId="208" priority="191" operator="lessThan">
+    <cfRule type="cellIs" dxfId="209" priority="191" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO3:FO18">
-    <cfRule type="cellIs" dxfId="207" priority="190" operator="lessThan">
+    <cfRule type="cellIs" dxfId="208" priority="190" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2:FO17">
-    <cfRule type="cellIs" dxfId="206" priority="189" operator="lessThan">
+    <cfRule type="cellIs" dxfId="207" priority="189" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP18:GB18">
-    <cfRule type="cellIs" dxfId="205" priority="188" operator="lessThan">
+    <cfRule type="cellIs" dxfId="206" priority="188" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB2">
-    <cfRule type="cellIs" dxfId="204" priority="187" operator="lessThan">
+    <cfRule type="cellIs" dxfId="205" priority="187" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB2">
-    <cfRule type="cellIs" dxfId="203" priority="186" operator="lessThan">
+    <cfRule type="cellIs" dxfId="204" priority="186" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP3:GB17">
-    <cfRule type="cellIs" dxfId="202" priority="185" operator="lessThan">
+    <cfRule type="cellIs" dxfId="203" priority="185" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB17">
-    <cfRule type="cellIs" dxfId="201" priority="184" operator="lessThan">
+    <cfRule type="cellIs" dxfId="202" priority="184" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC18:GL18">
-    <cfRule type="cellIs" dxfId="200" priority="183" operator="lessThan">
+    <cfRule type="cellIs" dxfId="201" priority="183" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL2">
-    <cfRule type="cellIs" dxfId="199" priority="182" operator="lessThan">
+    <cfRule type="cellIs" dxfId="200" priority="182" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL2">
-    <cfRule type="cellIs" dxfId="198" priority="181" operator="lessThan">
+    <cfRule type="cellIs" dxfId="199" priority="181" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC3:GL17">
-    <cfRule type="cellIs" dxfId="197" priority="180" operator="lessThan">
+    <cfRule type="cellIs" dxfId="198" priority="180" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL17">
-    <cfRule type="cellIs" dxfId="196" priority="179" operator="lessThan">
+    <cfRule type="cellIs" dxfId="197" priority="179" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM18">
-    <cfRule type="cellIs" dxfId="195" priority="178" operator="lessThan">
+    <cfRule type="cellIs" dxfId="196" priority="178" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2">
-    <cfRule type="cellIs" dxfId="194" priority="177" operator="lessThan">
+    <cfRule type="cellIs" dxfId="195" priority="177" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2">
-    <cfRule type="cellIs" dxfId="193" priority="176" operator="lessThan">
+    <cfRule type="cellIs" dxfId="194" priority="176" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM3:GM17">
-    <cfRule type="cellIs" dxfId="192" priority="175" operator="lessThan">
+    <cfRule type="cellIs" dxfId="193" priority="175" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2:GM17">
-    <cfRule type="cellIs" dxfId="191" priority="174" operator="lessThan">
+    <cfRule type="cellIs" dxfId="192" priority="174" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN18">
-    <cfRule type="cellIs" dxfId="190" priority="173" operator="lessThan">
+    <cfRule type="cellIs" dxfId="191" priority="173" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2">
-    <cfRule type="cellIs" dxfId="189" priority="172" operator="lessThan">
+    <cfRule type="cellIs" dxfId="190" priority="172" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2">
-    <cfRule type="cellIs" dxfId="188" priority="171" operator="lessThan">
+    <cfRule type="cellIs" dxfId="189" priority="171" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN3:GN17">
-    <cfRule type="cellIs" dxfId="187" priority="170" operator="lessThan">
+    <cfRule type="cellIs" dxfId="188" priority="170" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2:GN17">
-    <cfRule type="cellIs" dxfId="186" priority="169" operator="lessThan">
+    <cfRule type="cellIs" dxfId="187" priority="169" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO18">
-    <cfRule type="cellIs" dxfId="185" priority="168" operator="lessThan">
+    <cfRule type="cellIs" dxfId="186" priority="168" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2">
-    <cfRule type="cellIs" dxfId="184" priority="167" operator="lessThan">
+    <cfRule type="cellIs" dxfId="185" priority="167" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2">
-    <cfRule type="cellIs" dxfId="183" priority="166" operator="lessThan">
+    <cfRule type="cellIs" dxfId="184" priority="166" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO3:GO17">
-    <cfRule type="cellIs" dxfId="182" priority="165" operator="lessThan">
+    <cfRule type="cellIs" dxfId="183" priority="165" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2:GO17">
-    <cfRule type="cellIs" dxfId="181" priority="164" operator="lessThan">
+    <cfRule type="cellIs" dxfId="182" priority="164" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP18">
-    <cfRule type="cellIs" dxfId="180" priority="163" operator="lessThan">
+    <cfRule type="cellIs" dxfId="181" priority="163" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2">
-    <cfRule type="cellIs" dxfId="179" priority="162" operator="lessThan">
+    <cfRule type="cellIs" dxfId="180" priority="162" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2">
-    <cfRule type="cellIs" dxfId="178" priority="161" operator="lessThan">
+    <cfRule type="cellIs" dxfId="179" priority="161" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP3:GP17">
-    <cfRule type="cellIs" dxfId="177" priority="160" operator="lessThan">
+    <cfRule type="cellIs" dxfId="178" priority="160" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2:GP17">
-    <cfRule type="cellIs" dxfId="176" priority="159" operator="lessThan">
+    <cfRule type="cellIs" dxfId="177" priority="159" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ18:GV18">
-    <cfRule type="cellIs" dxfId="175" priority="158" operator="lessThan">
+    <cfRule type="cellIs" dxfId="176" priority="158" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV2">
-    <cfRule type="cellIs" dxfId="174" priority="157" operator="lessThan">
+    <cfRule type="cellIs" dxfId="175" priority="157" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV2">
-    <cfRule type="cellIs" dxfId="173" priority="156" operator="lessThan">
+    <cfRule type="cellIs" dxfId="174" priority="156" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ3:GV17">
-    <cfRule type="cellIs" dxfId="172" priority="155" operator="lessThan">
+    <cfRule type="cellIs" dxfId="173" priority="155" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV17">
-    <cfRule type="cellIs" dxfId="171" priority="154" operator="lessThan">
+    <cfRule type="cellIs" dxfId="172" priority="154" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW18">
-    <cfRule type="cellIs" dxfId="170" priority="153" operator="lessThan">
+    <cfRule type="cellIs" dxfId="171" priority="153" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2">
-    <cfRule type="cellIs" dxfId="169" priority="152" operator="lessThan">
+    <cfRule type="cellIs" dxfId="170" priority="152" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2">
-    <cfRule type="cellIs" dxfId="168" priority="151" operator="lessThan">
+    <cfRule type="cellIs" dxfId="169" priority="151" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW3:GW17">
-    <cfRule type="cellIs" dxfId="167" priority="150" operator="lessThan">
+    <cfRule type="cellIs" dxfId="168" priority="150" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2:GW17">
-    <cfRule type="cellIs" dxfId="166" priority="149" operator="lessThan">
+    <cfRule type="cellIs" dxfId="167" priority="149" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX18">
-    <cfRule type="cellIs" dxfId="165" priority="148" operator="lessThan">
+    <cfRule type="cellIs" dxfId="166" priority="148" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2">
-    <cfRule type="cellIs" dxfId="164" priority="147" operator="lessThan">
+    <cfRule type="cellIs" dxfId="165" priority="147" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2">
-    <cfRule type="cellIs" dxfId="163" priority="146" operator="lessThan">
+    <cfRule type="cellIs" dxfId="164" priority="146" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX3:GX17">
-    <cfRule type="cellIs" dxfId="162" priority="145" operator="lessThan">
+    <cfRule type="cellIs" dxfId="163" priority="145" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2:GX17">
-    <cfRule type="cellIs" dxfId="161" priority="144" operator="lessThan">
+    <cfRule type="cellIs" dxfId="162" priority="144" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY18">
-    <cfRule type="cellIs" dxfId="160" priority="143" operator="lessThan">
+    <cfRule type="cellIs" dxfId="161" priority="143" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2">
-    <cfRule type="cellIs" dxfId="159" priority="142" operator="lessThan">
+    <cfRule type="cellIs" dxfId="160" priority="142" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2">
-    <cfRule type="cellIs" dxfId="158" priority="141" operator="lessThan">
+    <cfRule type="cellIs" dxfId="159" priority="141" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY3:GY17">
-    <cfRule type="cellIs" dxfId="157" priority="140" operator="lessThan">
+    <cfRule type="cellIs" dxfId="158" priority="140" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2:GY17">
-    <cfRule type="cellIs" dxfId="156" priority="139" operator="lessThan">
+    <cfRule type="cellIs" dxfId="157" priority="139" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ18:HF18">
-    <cfRule type="cellIs" dxfId="155" priority="138" operator="lessThan">
+    <cfRule type="cellIs" dxfId="156" priority="138" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF2">
-    <cfRule type="cellIs" dxfId="154" priority="137" operator="lessThan">
+    <cfRule type="cellIs" dxfId="155" priority="137" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF2">
-    <cfRule type="cellIs" dxfId="153" priority="136" operator="lessThan">
+    <cfRule type="cellIs" dxfId="154" priority="136" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ3:HF17">
-    <cfRule type="cellIs" dxfId="152" priority="135" operator="lessThan">
+    <cfRule type="cellIs" dxfId="153" priority="135" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF17">
-    <cfRule type="cellIs" dxfId="151" priority="134" operator="lessThan">
+    <cfRule type="cellIs" dxfId="152" priority="134" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG18">
-    <cfRule type="cellIs" dxfId="150" priority="128" operator="lessThan">
+    <cfRule type="cellIs" dxfId="151" priority="128" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2">
-    <cfRule type="cellIs" dxfId="149" priority="127" operator="lessThan">
+    <cfRule type="cellIs" dxfId="150" priority="127" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2">
-    <cfRule type="cellIs" dxfId="148" priority="126" operator="lessThan">
+    <cfRule type="cellIs" dxfId="149" priority="126" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG3:HG17">
-    <cfRule type="cellIs" dxfId="147" priority="125" operator="lessThan">
+    <cfRule type="cellIs" dxfId="148" priority="125" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2:HG17">
-    <cfRule type="cellIs" dxfId="146" priority="124" operator="lessThan">
+    <cfRule type="cellIs" dxfId="147" priority="124" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH18">
-    <cfRule type="cellIs" dxfId="145" priority="123" operator="lessThan">
+    <cfRule type="cellIs" dxfId="146" priority="123" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2">
-    <cfRule type="cellIs" dxfId="144" priority="122" operator="lessThan">
+    <cfRule type="cellIs" dxfId="145" priority="122" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2">
-    <cfRule type="cellIs" dxfId="143" priority="121" operator="lessThan">
+    <cfRule type="cellIs" dxfId="144" priority="121" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH3:HH17">
-    <cfRule type="cellIs" dxfId="142" priority="120" operator="lessThan">
+    <cfRule type="cellIs" dxfId="143" priority="120" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2:HH17">
-    <cfRule type="cellIs" dxfId="141" priority="119" operator="lessThan">
+    <cfRule type="cellIs" dxfId="142" priority="119" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI18">
-    <cfRule type="cellIs" dxfId="140" priority="118" operator="lessThan">
+    <cfRule type="cellIs" dxfId="141" priority="118" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2">
-    <cfRule type="cellIs" dxfId="139" priority="117" operator="lessThan">
+    <cfRule type="cellIs" dxfId="140" priority="117" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2">
-    <cfRule type="cellIs" dxfId="138" priority="116" operator="lessThan">
+    <cfRule type="cellIs" dxfId="139" priority="116" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI3:HI17">
-    <cfRule type="cellIs" dxfId="137" priority="115" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="115" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2:HI17">
-    <cfRule type="cellIs" dxfId="136" priority="114" operator="lessThan">
+    <cfRule type="cellIs" dxfId="137" priority="114" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ18">
-    <cfRule type="cellIs" dxfId="135" priority="113" operator="lessThan">
+    <cfRule type="cellIs" dxfId="136" priority="113" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2">
-    <cfRule type="cellIs" dxfId="134" priority="112" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="112" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2">
-    <cfRule type="cellIs" dxfId="133" priority="111" operator="lessThan">
+    <cfRule type="cellIs" dxfId="134" priority="111" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ3:HJ17">
-    <cfRule type="cellIs" dxfId="132" priority="110" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="110" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2:HJ17">
-    <cfRule type="cellIs" dxfId="131" priority="109" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="109" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK18">
-    <cfRule type="cellIs" dxfId="130" priority="108" operator="lessThan">
+    <cfRule type="cellIs" dxfId="131" priority="108" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2">
-    <cfRule type="cellIs" dxfId="129" priority="107" operator="lessThan">
+    <cfRule type="cellIs" dxfId="130" priority="107" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2">
-    <cfRule type="cellIs" dxfId="128" priority="106" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="106" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK3:HK17">
-    <cfRule type="cellIs" dxfId="127" priority="105" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="105" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2:HK17">
-    <cfRule type="cellIs" dxfId="126" priority="104" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="104" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL18">
-    <cfRule type="cellIs" dxfId="125" priority="103" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="103" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2">
-    <cfRule type="cellIs" dxfId="124" priority="102" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="102" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2">
-    <cfRule type="cellIs" dxfId="123" priority="101" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="101" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL3:HL17">
-    <cfRule type="cellIs" dxfId="122" priority="100" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="100" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2:HL17">
-    <cfRule type="cellIs" dxfId="121" priority="99" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="99" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM18">
-    <cfRule type="cellIs" dxfId="120" priority="98" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="98" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2">
-    <cfRule type="cellIs" dxfId="119" priority="97" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="97" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2">
-    <cfRule type="cellIs" dxfId="118" priority="96" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="96" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM3:HM17">
-    <cfRule type="cellIs" dxfId="117" priority="95" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="95" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2:HM17">
-    <cfRule type="cellIs" dxfId="116" priority="94" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="94" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN18">
-    <cfRule type="cellIs" dxfId="115" priority="93" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="93" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2">
-    <cfRule type="cellIs" dxfId="114" priority="92" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="92" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2">
-    <cfRule type="cellIs" dxfId="113" priority="91" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="91" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN3:HN17">
-    <cfRule type="cellIs" dxfId="112" priority="90" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="90" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2:HN17">
-    <cfRule type="cellIs" dxfId="111" priority="89" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="89" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO18">
-    <cfRule type="cellIs" dxfId="110" priority="88" operator="lessThan">
+    <cfRule type="cellIs" dxfId="111" priority="88" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2">
-    <cfRule type="cellIs" dxfId="109" priority="87" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="87" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2">
-    <cfRule type="cellIs" dxfId="108" priority="86" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="86" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO3:HO17">
-    <cfRule type="cellIs" dxfId="107" priority="85" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="85" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2:HO17">
-    <cfRule type="cellIs" dxfId="106" priority="84" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="84" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP18">
-    <cfRule type="cellIs" dxfId="105" priority="83" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="83" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2">
-    <cfRule type="cellIs" dxfId="104" priority="82" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="82" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2">
-    <cfRule type="cellIs" dxfId="103" priority="81" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="81" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP3:HP17">
-    <cfRule type="cellIs" dxfId="102" priority="80" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="80" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2:HP17">
-    <cfRule type="cellIs" dxfId="101" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="79" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ18">
-    <cfRule type="cellIs" dxfId="100" priority="78" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="78" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2">
-    <cfRule type="cellIs" dxfId="99" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="77" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2">
-    <cfRule type="cellIs" dxfId="98" priority="76" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="76" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ3:HQ17">
-    <cfRule type="cellIs" dxfId="97" priority="75" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="75" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2:HQ17">
-    <cfRule type="cellIs" dxfId="96" priority="74" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="74" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR18:HZ18">
-    <cfRule type="cellIs" dxfId="95" priority="73" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="73" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ2">
-    <cfRule type="cellIs" dxfId="94" priority="72" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="72" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ2">
-    <cfRule type="cellIs" dxfId="93" priority="71" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="71" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR3:HZ17">
-    <cfRule type="cellIs" dxfId="92" priority="70" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="70" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ17">
-    <cfRule type="cellIs" dxfId="91" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="69" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA18">
-    <cfRule type="cellIs" dxfId="90" priority="68" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="68" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2">
-    <cfRule type="cellIs" dxfId="89" priority="67" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="67" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2">
-    <cfRule type="cellIs" dxfId="88" priority="66" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="66" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA3:IA17">
-    <cfRule type="cellIs" dxfId="87" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="65" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2:IA17">
-    <cfRule type="cellIs" dxfId="86" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="64" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB18:IG18">
-    <cfRule type="cellIs" dxfId="85" priority="63" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="63" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG2">
-    <cfRule type="cellIs" dxfId="84" priority="62" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="62" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG2">
-    <cfRule type="cellIs" dxfId="83" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="61" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB3:IG17">
-    <cfRule type="cellIs" dxfId="82" priority="60" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="60" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG17">
-    <cfRule type="cellIs" dxfId="81" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="59" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH18:IL18">
-    <cfRule type="cellIs" dxfId="80" priority="58" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="58" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL2">
-    <cfRule type="cellIs" dxfId="79" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="57" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL2">
-    <cfRule type="cellIs" dxfId="78" priority="56" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="56" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH3:IL17">
-    <cfRule type="cellIs" dxfId="77" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="55" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL17">
-    <cfRule type="cellIs" dxfId="76" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="54" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM18:IT18">
-    <cfRule type="cellIs" dxfId="75" priority="53" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="53" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT2">
-    <cfRule type="cellIs" dxfId="74" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="52" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT2">
-    <cfRule type="cellIs" dxfId="73" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="51" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM3:IT17">
-    <cfRule type="cellIs" dxfId="72" priority="50" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="50" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT17">
-    <cfRule type="cellIs" dxfId="71" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU18">
-    <cfRule type="cellIs" dxfId="70" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="48" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2">
-    <cfRule type="cellIs" dxfId="69" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="47" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2">
-    <cfRule type="cellIs" dxfId="68" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="46" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU3:IU17">
-    <cfRule type="cellIs" dxfId="67" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="45" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2:IU17">
-    <cfRule type="cellIs" dxfId="66" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="44" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV18">
-    <cfRule type="cellIs" dxfId="65" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="43" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2">
-    <cfRule type="cellIs" dxfId="64" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="42" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2">
-    <cfRule type="cellIs" dxfId="63" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="41" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV3:IV17">
-    <cfRule type="cellIs" dxfId="62" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="40" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2:IV17">
-    <cfRule type="cellIs" dxfId="61" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="39" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW18">
-    <cfRule type="cellIs" dxfId="60" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="38" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2">
-    <cfRule type="cellIs" dxfId="59" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2">
-    <cfRule type="cellIs" dxfId="58" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="36" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW3:IW17">
-    <cfRule type="cellIs" dxfId="57" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2:IW17">
-    <cfRule type="cellIs" dxfId="56" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX18">
-    <cfRule type="cellIs" dxfId="55" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="33" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2">
-    <cfRule type="cellIs" dxfId="54" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="32" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2">
-    <cfRule type="cellIs" dxfId="53" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX3:IX17">
-    <cfRule type="cellIs" dxfId="52" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="30" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2:IX17">
-    <cfRule type="cellIs" dxfId="51" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="29" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY18">
-    <cfRule type="cellIs" dxfId="50" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="28" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2">
-    <cfRule type="cellIs" dxfId="49" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2">
-    <cfRule type="cellIs" dxfId="48" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY3:IY17">
-    <cfRule type="cellIs" dxfId="47" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2:IY17">
-    <cfRule type="cellIs" dxfId="46" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="24" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ18">
-    <cfRule type="cellIs" dxfId="45" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2">
-    <cfRule type="cellIs" dxfId="44" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2">
-    <cfRule type="cellIs" dxfId="43" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ3:IZ17">
-    <cfRule type="cellIs" dxfId="42" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2:IZ17">
-    <cfRule type="cellIs" dxfId="41" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA18">
-    <cfRule type="cellIs" dxfId="40" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2">
-    <cfRule type="cellIs" dxfId="39" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2">
-    <cfRule type="cellIs" dxfId="38" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA3:JA17">
-    <cfRule type="cellIs" dxfId="37" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2:JA17">
-    <cfRule type="cellIs" dxfId="36" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JO18:JU18">
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JQ2:JQ17">
-    <cfRule type="cellIs" dxfId="34" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JQ2:JQ17">
-    <cfRule type="cellIs" dxfId="33" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JR2:JR17">
-    <cfRule type="cellIs" dxfId="32" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JR2:JR17">
-    <cfRule type="cellIs" dxfId="31" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JS2:JS17">
-    <cfRule type="cellIs" dxfId="30" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JS2:JS17">
-    <cfRule type="cellIs" dxfId="29" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JT2:JT17">
-    <cfRule type="cellIs" dxfId="28" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JT2:JT17">
-    <cfRule type="cellIs" dxfId="27" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JU2:JU17">
-    <cfRule type="cellIs" dxfId="26" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JU2:JU17">
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JV18:KC18">
-    <cfRule type="cellIs" dxfId="24" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="KD18:KP18">
-    <cfRule type="cellIs" dxfId="23" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -74441,10 +75592,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PM18"/>
+  <dimension ref="A1:PT18"/>
   <sheetViews>
-    <sheetView topLeftCell="PC1" workbookViewId="0">
-      <selection activeCell="PO14" sqref="PO14"/>
+    <sheetView topLeftCell="PF1" workbookViewId="0">
+      <selection activeCell="PU11" sqref="PU11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -74452,7 +75603,7 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -75740,8 +76891,29 @@
       <c r="PM1" s="8">
         <v>44362</v>
       </c>
+      <c r="PN1" s="8">
+        <v>44363</v>
+      </c>
+      <c r="PO1" s="8">
+        <v>44364</v>
+      </c>
+      <c r="PP1" s="8">
+        <v>44365</v>
+      </c>
+      <c r="PQ1" s="8">
+        <v>44366</v>
+      </c>
+      <c r="PR1" s="8">
+        <v>44367</v>
+      </c>
+      <c r="PS1" s="8">
+        <v>44368</v>
+      </c>
+      <c r="PT1" s="8">
+        <v>44369</v>
+      </c>
     </row>
-    <row r="2" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -77029,8 +78201,29 @@
       <c r="PM2">
         <v>9</v>
       </c>
+      <c r="PN2">
+        <v>9</v>
+      </c>
+      <c r="PO2">
+        <v>9</v>
+      </c>
+      <c r="PP2">
+        <v>9</v>
+      </c>
+      <c r="PQ2">
+        <v>9</v>
+      </c>
+      <c r="PR2">
+        <v>9</v>
+      </c>
+      <c r="PS2">
+        <v>9</v>
+      </c>
+      <c r="PT2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -78318,8 +79511,29 @@
       <c r="PM3">
         <v>12</v>
       </c>
+      <c r="PN3">
+        <v>12</v>
+      </c>
+      <c r="PO3">
+        <v>12</v>
+      </c>
+      <c r="PP3">
+        <v>12</v>
+      </c>
+      <c r="PQ3">
+        <v>12</v>
+      </c>
+      <c r="PR3">
+        <v>12</v>
+      </c>
+      <c r="PS3">
+        <v>12</v>
+      </c>
+      <c r="PT3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -79607,8 +80821,29 @@
       <c r="PM4">
         <v>48</v>
       </c>
+      <c r="PN4">
+        <v>48</v>
+      </c>
+      <c r="PO4">
+        <v>48</v>
+      </c>
+      <c r="PP4">
+        <v>48</v>
+      </c>
+      <c r="PQ4">
+        <v>48</v>
+      </c>
+      <c r="PR4">
+        <v>48</v>
+      </c>
+      <c r="PS4">
+        <v>48</v>
+      </c>
+      <c r="PT4">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -80896,8 +82131,29 @@
       <c r="PM5">
         <v>11</v>
       </c>
+      <c r="PN5">
+        <v>11</v>
+      </c>
+      <c r="PO5">
+        <v>11</v>
+      </c>
+      <c r="PP5">
+        <v>11</v>
+      </c>
+      <c r="PQ5">
+        <v>11</v>
+      </c>
+      <c r="PR5">
+        <v>11</v>
+      </c>
+      <c r="PS5">
+        <v>11</v>
+      </c>
+      <c r="PT5">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -82185,8 +83441,29 @@
       <c r="PM6">
         <v>29</v>
       </c>
+      <c r="PN6">
+        <v>29</v>
+      </c>
+      <c r="PO6">
+        <v>29</v>
+      </c>
+      <c r="PP6">
+        <v>29</v>
+      </c>
+      <c r="PQ6">
+        <v>29</v>
+      </c>
+      <c r="PR6">
+        <v>29</v>
+      </c>
+      <c r="PS6">
+        <v>29</v>
+      </c>
+      <c r="PT6">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -83474,8 +84751,29 @@
       <c r="PM7">
         <v>125</v>
       </c>
+      <c r="PN7">
+        <v>125</v>
+      </c>
+      <c r="PO7">
+        <v>125</v>
+      </c>
+      <c r="PP7">
+        <v>125</v>
+      </c>
+      <c r="PQ7">
+        <v>125</v>
+      </c>
+      <c r="PR7">
+        <v>125</v>
+      </c>
+      <c r="PS7">
+        <v>125</v>
+      </c>
+      <c r="PT7">
+        <v>125</v>
+      </c>
     </row>
-    <row r="8" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -84763,8 +86061,29 @@
       <c r="PM8">
         <v>745</v>
       </c>
+      <c r="PN8">
+        <v>745</v>
+      </c>
+      <c r="PO8">
+        <v>745</v>
+      </c>
+      <c r="PP8">
+        <v>745</v>
+      </c>
+      <c r="PQ8">
+        <v>745</v>
+      </c>
+      <c r="PR8">
+        <v>745</v>
+      </c>
+      <c r="PS8">
+        <v>745</v>
+      </c>
+      <c r="PT8">
+        <v>745</v>
+      </c>
     </row>
-    <row r="9" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -86052,8 +87371,29 @@
       <c r="PM9">
         <v>61</v>
       </c>
+      <c r="PN9">
+        <v>61</v>
+      </c>
+      <c r="PO9">
+        <v>61</v>
+      </c>
+      <c r="PP9">
+        <v>61</v>
+      </c>
+      <c r="PQ9">
+        <v>61</v>
+      </c>
+      <c r="PR9">
+        <v>61</v>
+      </c>
+      <c r="PS9">
+        <v>61</v>
+      </c>
+      <c r="PT9">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -87341,8 +88681,29 @@
       <c r="PM10">
         <v>45</v>
       </c>
+      <c r="PN10">
+        <v>45</v>
+      </c>
+      <c r="PO10">
+        <v>45</v>
+      </c>
+      <c r="PP10">
+        <v>45</v>
+      </c>
+      <c r="PQ10">
+        <v>45</v>
+      </c>
+      <c r="PR10">
+        <v>45</v>
+      </c>
+      <c r="PS10">
+        <v>45</v>
+      </c>
+      <c r="PT10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="11" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -88630,8 +89991,29 @@
       <c r="PM11">
         <v>16</v>
       </c>
+      <c r="PN11">
+        <v>16</v>
+      </c>
+      <c r="PO11">
+        <v>16</v>
+      </c>
+      <c r="PP11">
+        <v>16</v>
+      </c>
+      <c r="PQ11">
+        <v>16</v>
+      </c>
+      <c r="PR11">
+        <v>16</v>
+      </c>
+      <c r="PS11">
+        <v>16</v>
+      </c>
+      <c r="PT11">
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -89919,8 +91301,29 @@
       <c r="PM12">
         <v>97</v>
       </c>
+      <c r="PN12">
+        <v>97</v>
+      </c>
+      <c r="PO12">
+        <v>97</v>
+      </c>
+      <c r="PP12">
+        <v>97</v>
+      </c>
+      <c r="PQ12">
+        <v>97</v>
+      </c>
+      <c r="PR12">
+        <v>97</v>
+      </c>
+      <c r="PS12">
+        <v>97</v>
+      </c>
+      <c r="PT12">
+        <v>97</v>
+      </c>
     </row>
-    <row r="13" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -91208,8 +92611,29 @@
       <c r="PM13">
         <v>49</v>
       </c>
+      <c r="PN13">
+        <v>49</v>
+      </c>
+      <c r="PO13">
+        <v>49</v>
+      </c>
+      <c r="PP13">
+        <v>49</v>
+      </c>
+      <c r="PQ13">
+        <v>49</v>
+      </c>
+      <c r="PR13">
+        <v>49</v>
+      </c>
+      <c r="PS13">
+        <v>49</v>
+      </c>
+      <c r="PT13">
+        <v>49</v>
+      </c>
     </row>
-    <row r="14" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -92497,8 +93921,29 @@
       <c r="PM14">
         <v>13</v>
       </c>
+      <c r="PN14">
+        <v>13</v>
+      </c>
+      <c r="PO14">
+        <v>13</v>
+      </c>
+      <c r="PP14">
+        <v>13</v>
+      </c>
+      <c r="PQ14">
+        <v>13</v>
+      </c>
+      <c r="PR14">
+        <v>13</v>
+      </c>
+      <c r="PS14">
+        <v>13</v>
+      </c>
+      <c r="PT14">
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -93786,8 +95231,29 @@
       <c r="PM15">
         <v>49</v>
       </c>
+      <c r="PN15">
+        <v>49</v>
+      </c>
+      <c r="PO15">
+        <v>49</v>
+      </c>
+      <c r="PP15">
+        <v>49</v>
+      </c>
+      <c r="PQ15">
+        <v>49</v>
+      </c>
+      <c r="PR15">
+        <v>49</v>
+      </c>
+      <c r="PS15">
+        <v>49</v>
+      </c>
+      <c r="PT15">
+        <v>49</v>
+      </c>
     </row>
-    <row r="16" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -95075,8 +96541,29 @@
       <c r="PM16">
         <v>8</v>
       </c>
+      <c r="PN16">
+        <v>8</v>
+      </c>
+      <c r="PO16">
+        <v>8</v>
+      </c>
+      <c r="PP16">
+        <v>8</v>
+      </c>
+      <c r="PQ16">
+        <v>8</v>
+      </c>
+      <c r="PR16">
+        <v>8</v>
+      </c>
+      <c r="PS16">
+        <v>8</v>
+      </c>
+      <c r="PT16">
+        <v>8</v>
+      </c>
     </row>
-    <row r="17" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -96364,8 +97851,29 @@
       <c r="PM17">
         <v>14</v>
       </c>
+      <c r="PN17">
+        <v>14</v>
+      </c>
+      <c r="PO17">
+        <v>14</v>
+      </c>
+      <c r="PP17">
+        <v>14</v>
+      </c>
+      <c r="PQ17">
+        <v>14</v>
+      </c>
+      <c r="PR17">
+        <v>14</v>
+      </c>
+      <c r="PS17">
+        <v>14</v>
+      </c>
+      <c r="PT17">
+        <v>14</v>
+      </c>
     </row>
-    <row r="18" spans="1:429" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -98081,114 +99589,147 @@
         <f t="shared" si="18"/>
         <v>1331</v>
       </c>
+      <c r="PN18" s="6">
+        <f t="shared" ref="PN18:PT18" si="19">SUM(PN2:PN17)</f>
+        <v>1331</v>
+      </c>
+      <c r="PO18" s="6">
+        <f t="shared" si="19"/>
+        <v>1331</v>
+      </c>
+      <c r="PP18" s="6">
+        <f t="shared" si="19"/>
+        <v>1331</v>
+      </c>
+      <c r="PQ18" s="6">
+        <f t="shared" si="19"/>
+        <v>1331</v>
+      </c>
+      <c r="PR18" s="6">
+        <f t="shared" si="19"/>
+        <v>1331</v>
+      </c>
+      <c r="PS18" s="6">
+        <f t="shared" si="19"/>
+        <v>1331</v>
+      </c>
+      <c r="PT18" s="6">
+        <f t="shared" si="19"/>
+        <v>1331</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="22" priority="254" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="255" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B18">
+    <cfRule type="cellIs" dxfId="22" priority="253" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B17">
     <cfRule type="cellIs" dxfId="21" priority="252" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="20" priority="251" operator="lessThan">
+  <conditionalFormatting sqref="C2:MF17">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:MF18">
+    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:MF17">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:MF18">
     <cfRule type="cellIs" dxfId="18" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:MF17">
+  <conditionalFormatting sqref="MG2:MG17">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MG2:MG17">
+  <conditionalFormatting sqref="MG3:MG18">
     <cfRule type="cellIs" dxfId="16" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MG3:MG18">
+  <conditionalFormatting sqref="MG2:MG17">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MG2:MG17">
+  <conditionalFormatting sqref="MH18">
     <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MH18">
+  <conditionalFormatting sqref="MI18:MN18">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MI18:MN18">
+  <conditionalFormatting sqref="MO18:MU18">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MO18:MU18">
+  <conditionalFormatting sqref="MV18:NB18">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MV18:NB18">
+  <conditionalFormatting sqref="NC18:NI18">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NC18:NI18">
+  <conditionalFormatting sqref="NJ18:NP18">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NJ18:NP18">
+  <conditionalFormatting sqref="NQ18:NW18">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NQ18:NW18">
+  <conditionalFormatting sqref="NX18:OD18">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NX18:OD18">
+  <conditionalFormatting sqref="OE18:OK18">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OE18:OK18">
+  <conditionalFormatting sqref="OL18:OR18">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OL18:OR18">
+  <conditionalFormatting sqref="OS18:OY18">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OS18:OY18">
+  <conditionalFormatting sqref="OZ18:PF18">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OZ18:PF18">
+  <conditionalFormatting sqref="PG18:PM18">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="PG18:PM18">
+  <conditionalFormatting sqref="PN18:PT18">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update automatico via Actualizar 06-29-2021 16-07-44
</commit_message>
<xml_diff>
--- a/input/Camas_uci/last_uci_diario.xlsx
+++ b/input/Camas_uci/last_uci_diario.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="676" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="676"/>
   </bookViews>
   <sheets>
     <sheet name="UCI HABILITADA" sheetId="2" r:id="rId1"/>
@@ -259,7 +259,17 @@
     <cellStyle name="Millares [0] 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="259">
+  <dxfs count="260">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3160,12 +3170,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PT20"/>
+  <dimension ref="A1:QA20"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="PK1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="PT1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="PN18" sqref="PN18:PT18"/>
+      <selection pane="topRight" activeCell="QC11" sqref="QC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3186,7 +3196,7 @@
     <col min="276" max="16384" width="11.42578125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>34</v>
       </c>
@@ -4495,8 +4505,29 @@
       <c r="PT1" s="8">
         <v>44369</v>
       </c>
+      <c r="PU1" s="8">
+        <v>44370</v>
+      </c>
+      <c r="PV1" s="8">
+        <v>44371</v>
+      </c>
+      <c r="PW1" s="8">
+        <v>44372</v>
+      </c>
+      <c r="PX1" s="8">
+        <v>44373</v>
+      </c>
+      <c r="PY1" s="8">
+        <v>44374</v>
+      </c>
+      <c r="PZ1" s="8">
+        <v>44375</v>
+      </c>
+      <c r="QA1" s="8">
+        <v>44376</v>
+      </c>
     </row>
-    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
@@ -5805,8 +5836,29 @@
       <c r="PT2" s="11">
         <v>33</v>
       </c>
+      <c r="PU2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PV2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PW2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PX2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PY2" s="11">
+        <v>33</v>
+      </c>
+      <c r="PZ2" s="11">
+        <v>33</v>
+      </c>
+      <c r="QA2" s="11">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>1</v>
       </c>
@@ -7115,8 +7167,29 @@
       <c r="PT3" s="11">
         <v>61</v>
       </c>
+      <c r="PU3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PV3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PW3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PX3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PY3" s="11">
+        <v>61</v>
+      </c>
+      <c r="PZ3" s="11">
+        <v>61</v>
+      </c>
+      <c r="QA3" s="11">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>2</v>
       </c>
@@ -8425,8 +8498,29 @@
       <c r="PT4" s="11">
         <v>164</v>
       </c>
+      <c r="PU4" s="11">
+        <v>170</v>
+      </c>
+      <c r="PV4" s="11">
+        <v>170</v>
+      </c>
+      <c r="PW4" s="11">
+        <v>170</v>
+      </c>
+      <c r="PX4" s="11">
+        <v>170</v>
+      </c>
+      <c r="PY4" s="11">
+        <v>170</v>
+      </c>
+      <c r="PZ4" s="11">
+        <v>170</v>
+      </c>
+      <c r="QA4" s="11">
+        <v>171</v>
+      </c>
     </row>
-    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>3</v>
       </c>
@@ -9735,8 +9829,29 @@
       <c r="PT5" s="11">
         <v>34</v>
       </c>
+      <c r="PU5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PV5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PW5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PX5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PY5" s="11">
+        <v>34</v>
+      </c>
+      <c r="PZ5" s="11">
+        <v>34</v>
+      </c>
+      <c r="QA5" s="11">
+        <v>34</v>
+      </c>
     </row>
-    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -11045,8 +11160,29 @@
       <c r="PT6" s="11">
         <v>135</v>
       </c>
+      <c r="PU6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PV6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PW6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PX6" s="11">
+        <v>134</v>
+      </c>
+      <c r="PY6" s="11">
+        <v>135</v>
+      </c>
+      <c r="PZ6" s="11">
+        <v>136</v>
+      </c>
+      <c r="QA6" s="11">
+        <v>136</v>
+      </c>
     </row>
-    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>5</v>
       </c>
@@ -12355,8 +12491,29 @@
       <c r="PT7" s="11">
         <v>332</v>
       </c>
+      <c r="PU7" s="11">
+        <v>333</v>
+      </c>
+      <c r="PV7" s="11">
+        <v>329</v>
+      </c>
+      <c r="PW7" s="11">
+        <v>331</v>
+      </c>
+      <c r="PX7" s="11">
+        <v>330</v>
+      </c>
+      <c r="PY7" s="11">
+        <v>328</v>
+      </c>
+      <c r="PZ7" s="11">
+        <v>326</v>
+      </c>
+      <c r="QA7" s="11">
+        <v>326</v>
+      </c>
     </row>
-    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>6</v>
       </c>
@@ -13665,8 +13822,29 @@
       <c r="PT8" s="11">
         <v>2613</v>
       </c>
+      <c r="PU8" s="11">
+        <v>2616</v>
+      </c>
+      <c r="PV8" s="11">
+        <v>2605</v>
+      </c>
+      <c r="PW8" s="11">
+        <v>2602</v>
+      </c>
+      <c r="PX8" s="11">
+        <v>2600</v>
+      </c>
+      <c r="PY8" s="11">
+        <v>2597</v>
+      </c>
+      <c r="PZ8" s="11">
+        <v>2596</v>
+      </c>
+      <c r="QA8" s="11">
+        <v>2596</v>
+      </c>
     </row>
-    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>7</v>
       </c>
@@ -14975,8 +15153,29 @@
       <c r="PT9" s="11">
         <v>206</v>
       </c>
+      <c r="PU9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PV9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PW9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PX9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PY9" s="11">
+        <v>206</v>
+      </c>
+      <c r="PZ9" s="11">
+        <v>206</v>
+      </c>
+      <c r="QA9" s="11">
+        <v>198</v>
+      </c>
     </row>
-    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>8</v>
       </c>
@@ -16285,8 +16484,29 @@
       <c r="PT10" s="11">
         <v>158</v>
       </c>
+      <c r="PU10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PV10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PW10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PX10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PY10" s="11">
+        <v>158</v>
+      </c>
+      <c r="PZ10" s="11">
+        <v>158</v>
+      </c>
+      <c r="QA10" s="11">
+        <v>158</v>
+      </c>
     </row>
-    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>9</v>
       </c>
@@ -17595,8 +17815,29 @@
       <c r="PT11" s="11">
         <v>70</v>
       </c>
+      <c r="PU11" s="11">
+        <v>70</v>
+      </c>
+      <c r="PV11" s="11">
+        <v>76</v>
+      </c>
+      <c r="PW11" s="11">
+        <v>76</v>
+      </c>
+      <c r="PX11" s="11">
+        <v>76</v>
+      </c>
+      <c r="PY11" s="11">
+        <v>76</v>
+      </c>
+      <c r="PZ11" s="11">
+        <v>76</v>
+      </c>
+      <c r="QA11" s="11">
+        <v>76</v>
+      </c>
     </row>
-    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>10</v>
       </c>
@@ -18905,8 +19146,29 @@
       <c r="PT12" s="11">
         <v>311</v>
       </c>
+      <c r="PU12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PV12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PW12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PX12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PY12" s="11">
+        <v>311</v>
+      </c>
+      <c r="PZ12" s="11">
+        <v>311</v>
+      </c>
+      <c r="QA12" s="11">
+        <v>311</v>
+      </c>
     </row>
-    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
@@ -20215,8 +20477,29 @@
       <c r="PT13" s="11">
         <v>150</v>
       </c>
+      <c r="PU13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PV13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PW13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PX13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PY13" s="11">
+        <v>150</v>
+      </c>
+      <c r="PZ13" s="11">
+        <v>150</v>
+      </c>
+      <c r="QA13" s="11">
+        <v>150</v>
+      </c>
     </row>
-    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>12</v>
       </c>
@@ -21525,8 +21808,29 @@
       <c r="PT14" s="11">
         <v>41</v>
       </c>
+      <c r="PU14" s="11">
+        <v>41</v>
+      </c>
+      <c r="PV14" s="11">
+        <v>40</v>
+      </c>
+      <c r="PW14" s="11">
+        <v>42</v>
+      </c>
+      <c r="PX14" s="11">
+        <v>42</v>
+      </c>
+      <c r="PY14" s="11">
+        <v>37</v>
+      </c>
+      <c r="PZ14" s="11">
+        <v>38</v>
+      </c>
+      <c r="QA14" s="11">
+        <v>38</v>
+      </c>
     </row>
-    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>13</v>
       </c>
@@ -22835,8 +23139,29 @@
       <c r="PT15" s="11">
         <v>141</v>
       </c>
+      <c r="PU15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PV15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PW15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PX15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PY15" s="11">
+        <v>139</v>
+      </c>
+      <c r="PZ15" s="11">
+        <v>139</v>
+      </c>
+      <c r="QA15" s="11">
+        <v>136</v>
+      </c>
     </row>
-    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>14</v>
       </c>
@@ -24145,8 +24470,29 @@
       <c r="PT16" s="11">
         <v>17</v>
       </c>
+      <c r="PU16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PV16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PW16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PX16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PY16" s="11">
+        <v>17</v>
+      </c>
+      <c r="PZ16" s="11">
+        <v>17</v>
+      </c>
+      <c r="QA16" s="11">
+        <v>17</v>
+      </c>
     </row>
-    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>15</v>
       </c>
@@ -25455,8 +25801,29 @@
       <c r="PT17" s="11">
         <v>43</v>
       </c>
+      <c r="PU17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PV17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PW17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PX17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PY17" s="11">
+        <v>43</v>
+      </c>
+      <c r="PZ17" s="11">
+        <v>43</v>
+      </c>
+      <c r="QA17" s="11">
+        <v>43</v>
+      </c>
     </row>
-    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>16</v>
       </c>
@@ -26876,7 +27243,7 @@
         <v>4498</v>
       </c>
       <c r="PH18" s="6">
-        <f t="shared" ref="PH18:PT18" si="8">SUM(PH2:PH17)</f>
+        <f t="shared" ref="PH18:QA18" si="8">SUM(PH2:PH17)</f>
         <v>4513</v>
       </c>
       <c r="PI18" s="6">
@@ -26927,13 +27294,41 @@
         <f t="shared" si="8"/>
         <v>4509</v>
       </c>
+      <c r="PU18" s="6">
+        <f t="shared" si="8"/>
+        <v>4517</v>
+      </c>
+      <c r="PV18" s="6">
+        <f t="shared" si="8"/>
+        <v>4507</v>
+      </c>
+      <c r="PW18" s="6">
+        <f t="shared" si="8"/>
+        <v>4508</v>
+      </c>
+      <c r="PX18" s="6">
+        <f t="shared" si="8"/>
+        <v>4504</v>
+      </c>
+      <c r="PY18" s="6">
+        <f t="shared" si="8"/>
+        <v>4495</v>
+      </c>
+      <c r="PZ18" s="6">
+        <f t="shared" si="8"/>
+        <v>4494</v>
+      </c>
+      <c r="QA18" s="6">
+        <f t="shared" si="8"/>
+        <v>4484</v>
+      </c>
     </row>
-    <row r="19" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:443" x14ac:dyDescent="0.25">
       <c r="HV19" s="11" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:443" x14ac:dyDescent="0.25">
       <c r="JV20" s="19"/>
       <c r="JW20" s="19"/>
       <c r="JX20" s="19"/>
@@ -26951,12 +27346,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PT34"/>
+  <dimension ref="A1:QA34"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="PJ1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="PS1" activePane="topRight" state="frozen"/>
       <selection activeCell="FM17" sqref="FM17"/>
-      <selection pane="topRight" activeCell="PU13" sqref="PU13"/>
+      <selection pane="topRight" activeCell="PU19" sqref="PU19:QA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26976,7 +27371,7 @@
     <col min="272" max="272" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>17</v>
       </c>
@@ -28285,8 +28680,29 @@
       <c r="PT1" s="8">
         <v>44369</v>
       </c>
+      <c r="PU1" s="8">
+        <v>44370</v>
+      </c>
+      <c r="PV1" s="8">
+        <v>44371</v>
+      </c>
+      <c r="PW1" s="8">
+        <v>44372</v>
+      </c>
+      <c r="PX1" s="8">
+        <v>44373</v>
+      </c>
+      <c r="PY1" s="8">
+        <v>44374</v>
+      </c>
+      <c r="PZ1" s="8">
+        <v>44375</v>
+      </c>
+      <c r="QA1" s="8">
+        <v>44376</v>
+      </c>
     </row>
-    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -29595,8 +30011,29 @@
       <c r="PT2">
         <v>27</v>
       </c>
+      <c r="PU2">
+        <v>28</v>
+      </c>
+      <c r="PV2">
+        <v>27</v>
+      </c>
+      <c r="PW2">
+        <v>27</v>
+      </c>
+      <c r="PX2">
+        <v>26</v>
+      </c>
+      <c r="PY2">
+        <v>25</v>
+      </c>
+      <c r="PZ2">
+        <v>26</v>
+      </c>
+      <c r="QA2">
+        <v>26</v>
+      </c>
     </row>
-    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -30905,8 +31342,29 @@
       <c r="PT3">
         <v>53</v>
       </c>
+      <c r="PU3">
+        <v>53</v>
+      </c>
+      <c r="PV3">
+        <v>53</v>
+      </c>
+      <c r="PW3">
+        <v>53</v>
+      </c>
+      <c r="PX3">
+        <v>53</v>
+      </c>
+      <c r="PY3">
+        <v>53</v>
+      </c>
+      <c r="PZ3">
+        <v>54</v>
+      </c>
+      <c r="QA3">
+        <v>51</v>
+      </c>
     </row>
-    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -32215,8 +32673,29 @@
       <c r="PT4">
         <v>96</v>
       </c>
+      <c r="PU4">
+        <v>96</v>
+      </c>
+      <c r="PV4">
+        <v>93</v>
+      </c>
+      <c r="PW4">
+        <v>93</v>
+      </c>
+      <c r="PX4">
+        <v>92</v>
+      </c>
+      <c r="PY4">
+        <v>90</v>
+      </c>
+      <c r="PZ4">
+        <v>90</v>
+      </c>
+      <c r="QA4">
+        <v>92</v>
+      </c>
     </row>
-    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -33525,8 +34004,29 @@
       <c r="PT5">
         <v>28</v>
       </c>
+      <c r="PU5">
+        <v>28</v>
+      </c>
+      <c r="PV5">
+        <v>27</v>
+      </c>
+      <c r="PW5">
+        <v>26</v>
+      </c>
+      <c r="PX5">
+        <v>25</v>
+      </c>
+      <c r="PY5">
+        <v>25</v>
+      </c>
+      <c r="PZ5">
+        <v>25</v>
+      </c>
+      <c r="QA5">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -34835,8 +35335,29 @@
       <c r="PT6">
         <v>101</v>
       </c>
+      <c r="PU6">
+        <v>103</v>
+      </c>
+      <c r="PV6">
+        <v>102</v>
+      </c>
+      <c r="PW6">
+        <v>100</v>
+      </c>
+      <c r="PX6">
+        <v>100</v>
+      </c>
+      <c r="PY6">
+        <v>100</v>
+      </c>
+      <c r="PZ6">
+        <v>102</v>
+      </c>
+      <c r="QA6">
+        <v>104</v>
+      </c>
     </row>
-    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -36145,8 +36666,29 @@
       <c r="PT7">
         <v>210</v>
       </c>
+      <c r="PU7">
+        <v>217</v>
+      </c>
+      <c r="PV7">
+        <v>212</v>
+      </c>
+      <c r="PW7">
+        <v>204</v>
+      </c>
+      <c r="PX7">
+        <v>208</v>
+      </c>
+      <c r="PY7">
+        <v>203</v>
+      </c>
+      <c r="PZ7">
+        <v>205</v>
+      </c>
+      <c r="QA7">
+        <v>213</v>
+      </c>
     </row>
-    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -37455,8 +37997,29 @@
       <c r="PT8">
         <v>1950</v>
       </c>
+      <c r="PU8">
+        <v>1953</v>
+      </c>
+      <c r="PV8">
+        <v>1907</v>
+      </c>
+      <c r="PW8">
+        <v>1887</v>
+      </c>
+      <c r="PX8">
+        <v>1876</v>
+      </c>
+      <c r="PY8">
+        <v>1855</v>
+      </c>
+      <c r="PZ8">
+        <v>1850</v>
+      </c>
+      <c r="QA8">
+        <v>1832</v>
+      </c>
     </row>
-    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -38765,8 +39328,29 @@
       <c r="PT9">
         <v>161</v>
       </c>
+      <c r="PU9">
+        <v>158</v>
+      </c>
+      <c r="PV9">
+        <v>154</v>
+      </c>
+      <c r="PW9">
+        <v>152</v>
+      </c>
+      <c r="PX9">
+        <v>148</v>
+      </c>
+      <c r="PY9">
+        <v>150</v>
+      </c>
+      <c r="PZ9">
+        <v>141</v>
+      </c>
+      <c r="QA9">
+        <v>139</v>
+      </c>
     </row>
-    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -40075,8 +40659,29 @@
       <c r="PT10">
         <v>116</v>
       </c>
+      <c r="PU10">
+        <v>109</v>
+      </c>
+      <c r="PV10">
+        <v>108</v>
+      </c>
+      <c r="PW10">
+        <v>109</v>
+      </c>
+      <c r="PX10">
+        <v>109</v>
+      </c>
+      <c r="PY10">
+        <v>107</v>
+      </c>
+      <c r="PZ10">
+        <v>107</v>
+      </c>
+      <c r="QA10">
+        <v>98</v>
+      </c>
     </row>
-    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -41385,8 +41990,29 @@
       <c r="PT11">
         <v>43</v>
       </c>
+      <c r="PU11">
+        <v>46</v>
+      </c>
+      <c r="PV11">
+        <v>46</v>
+      </c>
+      <c r="PW11">
+        <v>47</v>
+      </c>
+      <c r="PX11">
+        <v>47</v>
+      </c>
+      <c r="PY11">
+        <v>46</v>
+      </c>
+      <c r="PZ11">
+        <v>46</v>
+      </c>
+      <c r="QA11">
+        <v>44</v>
+      </c>
     </row>
-    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -42695,8 +43321,29 @@
       <c r="PT12">
         <v>183</v>
       </c>
+      <c r="PU12">
+        <v>179</v>
+      </c>
+      <c r="PV12">
+        <v>178</v>
+      </c>
+      <c r="PW12">
+        <v>169</v>
+      </c>
+      <c r="PX12">
+        <v>171</v>
+      </c>
+      <c r="PY12">
+        <v>177</v>
+      </c>
+      <c r="PZ12">
+        <v>176</v>
+      </c>
+      <c r="QA12">
+        <v>167</v>
+      </c>
     </row>
-    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -44005,8 +44652,29 @@
       <c r="PT13">
         <v>105</v>
       </c>
+      <c r="PU13">
+        <v>100</v>
+      </c>
+      <c r="PV13">
+        <v>95</v>
+      </c>
+      <c r="PW13">
+        <v>96</v>
+      </c>
+      <c r="PX13">
+        <v>96</v>
+      </c>
+      <c r="PY13">
+        <v>96</v>
+      </c>
+      <c r="PZ13">
+        <v>94</v>
+      </c>
+      <c r="QA13">
+        <v>94</v>
+      </c>
     </row>
-    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -45315,8 +45983,29 @@
       <c r="PT14">
         <v>24</v>
       </c>
+      <c r="PU14">
+        <v>25</v>
+      </c>
+      <c r="PV14">
+        <v>26</v>
+      </c>
+      <c r="PW14">
+        <v>25</v>
+      </c>
+      <c r="PX14">
+        <v>23</v>
+      </c>
+      <c r="PY14">
+        <v>22</v>
+      </c>
+      <c r="PZ14">
+        <v>24</v>
+      </c>
+      <c r="QA14">
+        <v>24</v>
+      </c>
     </row>
-    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -46625,8 +47314,29 @@
       <c r="PT15">
         <v>100</v>
       </c>
+      <c r="PU15">
+        <v>98</v>
+      </c>
+      <c r="PV15">
+        <v>93</v>
+      </c>
+      <c r="PW15">
+        <v>87</v>
+      </c>
+      <c r="PX15">
+        <v>88</v>
+      </c>
+      <c r="PY15">
+        <v>86</v>
+      </c>
+      <c r="PZ15">
+        <v>83</v>
+      </c>
+      <c r="QA15">
+        <v>81</v>
+      </c>
     </row>
-    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -47935,8 +48645,29 @@
       <c r="PT16">
         <v>12</v>
       </c>
+      <c r="PU16">
+        <v>12</v>
+      </c>
+      <c r="PV16">
+        <v>10</v>
+      </c>
+      <c r="PW16">
+        <v>9</v>
+      </c>
+      <c r="PX16">
+        <v>10</v>
+      </c>
+      <c r="PY16">
+        <v>7</v>
+      </c>
+      <c r="PZ16">
+        <v>7</v>
+      </c>
+      <c r="QA16">
+        <v>7</v>
+      </c>
     </row>
-    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -49245,8 +49976,29 @@
       <c r="PT17">
         <v>23</v>
       </c>
+      <c r="PU17">
+        <v>24</v>
+      </c>
+      <c r="PV17">
+        <v>24</v>
+      </c>
+      <c r="PW17">
+        <v>21</v>
+      </c>
+      <c r="PX17">
+        <v>19</v>
+      </c>
+      <c r="PY17">
+        <v>19</v>
+      </c>
+      <c r="PZ17">
+        <v>20</v>
+      </c>
+      <c r="QA17">
+        <v>19</v>
+      </c>
     </row>
-    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -50563,7 +51315,7 @@
         <v>2979</v>
       </c>
       <c r="OL18" s="6">
-        <f t="shared" ref="OL18:PM18" si="2">SUM(OL2:OL17)</f>
+        <f t="shared" ref="OL18:QA18" si="2">SUM(OL2:OL17)</f>
         <v>2972</v>
       </c>
       <c r="OM18" s="6">
@@ -50675,70 +51427,105 @@
         <v>3275</v>
       </c>
       <c r="PN18" s="6">
+        <f t="shared" si="2"/>
         <v>3301</v>
       </c>
       <c r="PO18" s="6">
+        <f t="shared" si="2"/>
         <v>3302</v>
       </c>
       <c r="PP18" s="6">
+        <f t="shared" si="2"/>
         <v>3286</v>
       </c>
       <c r="PQ18" s="6">
+        <f t="shared" si="2"/>
         <v>3275</v>
       </c>
       <c r="PR18" s="6">
+        <f t="shared" si="2"/>
         <v>3230</v>
       </c>
       <c r="PS18" s="6">
+        <f t="shared" si="2"/>
         <v>3236</v>
       </c>
       <c r="PT18" s="6">
+        <f t="shared" si="2"/>
         <v>3232</v>
       </c>
+      <c r="PU18" s="6">
+        <f t="shared" si="2"/>
+        <v>3229</v>
+      </c>
+      <c r="PV18" s="6">
+        <f t="shared" si="2"/>
+        <v>3155</v>
+      </c>
+      <c r="PW18" s="6">
+        <f t="shared" si="2"/>
+        <v>3105</v>
+      </c>
+      <c r="PX18" s="6">
+        <f t="shared" si="2"/>
+        <v>3091</v>
+      </c>
+      <c r="PY18" s="6">
+        <f t="shared" si="2"/>
+        <v>3061</v>
+      </c>
+      <c r="PZ18" s="6">
+        <f t="shared" si="2"/>
+        <v>3050</v>
+      </c>
+      <c r="QA18" s="6">
+        <f t="shared" si="2"/>
+        <v>3017</v>
+      </c>
     </row>
-    <row r="19" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ19" s="1"/>
     </row>
-    <row r="20" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:443" x14ac:dyDescent="0.25">
       <c r="B20" s="9"/>
       <c r="AZ20" s="1"/>
     </row>
-    <row r="21" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:443" x14ac:dyDescent="0.25">
       <c r="B21" s="9"/>
       <c r="AZ21" s="1"/>
     </row>
-    <row r="22" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:443" x14ac:dyDescent="0.25">
       <c r="B22" s="9"/>
       <c r="AZ22" s="1"/>
     </row>
-    <row r="23" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ23" s="1"/>
     </row>
-    <row r="24" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ24" s="1"/>
     </row>
-    <row r="25" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ25" s="1"/>
     </row>
-    <row r="26" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ26" s="1"/>
     </row>
-    <row r="27" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ27" s="1"/>
     </row>
-    <row r="28" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ28" s="1"/>
     </row>
-    <row r="29" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ29" s="1"/>
     </row>
-    <row r="30" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ30" s="1"/>
     </row>
-    <row r="31" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ31" s="1"/>
     </row>
-    <row r="32" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:443" x14ac:dyDescent="0.25">
       <c r="AZ32" s="1"/>
     </row>
     <row r="33" spans="52:52" x14ac:dyDescent="0.25">
@@ -50758,12 +51545,12 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:PT34"/>
+  <dimension ref="A1:QA34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="PJ1" activePane="topRight" state="frozen"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="PS1" activePane="topRight" state="frozen"/>
       <selection activeCell="FW2" sqref="FW2:FW18"/>
-      <selection pane="topRight" activeCell="PN18" sqref="PN18:PT18"/>
+      <selection pane="topRight" activeCell="QA21" sqref="QA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50780,7 +51567,7 @@
     <col min="262" max="274" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
@@ -52089,8 +52876,29 @@
       <c r="PT1" s="8">
         <v>44369</v>
       </c>
+      <c r="PU1" s="8">
+        <v>44370</v>
+      </c>
+      <c r="PV1" s="8">
+        <v>44371</v>
+      </c>
+      <c r="PW1" s="8">
+        <v>44372</v>
+      </c>
+      <c r="PX1" s="8">
+        <v>44373</v>
+      </c>
+      <c r="PY1" s="8">
+        <v>44374</v>
+      </c>
+      <c r="PZ1" s="8">
+        <v>44375</v>
+      </c>
+      <c r="QA1" s="8">
+        <v>44376</v>
+      </c>
     </row>
-    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -53399,8 +54207,29 @@
       <c r="PT2">
         <v>5</v>
       </c>
+      <c r="PU2">
+        <v>2</v>
+      </c>
+      <c r="PV2">
+        <v>2</v>
+      </c>
+      <c r="PW2">
+        <v>4</v>
+      </c>
+      <c r="PX2">
+        <v>3</v>
+      </c>
+      <c r="PY2">
+        <v>3</v>
+      </c>
+      <c r="PZ2">
+        <v>2</v>
+      </c>
+      <c r="QA2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -54709,8 +55538,29 @@
       <c r="PT3">
         <v>5</v>
       </c>
+      <c r="PU3">
+        <v>5</v>
+      </c>
+      <c r="PV3">
+        <v>5</v>
+      </c>
+      <c r="PW3">
+        <v>5</v>
+      </c>
+      <c r="PX3">
+        <v>3</v>
+      </c>
+      <c r="PY3">
+        <v>2</v>
+      </c>
+      <c r="PZ3">
+        <v>4</v>
+      </c>
+      <c r="QA3">
+        <v>5</v>
+      </c>
     </row>
-    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -56019,8 +56869,29 @@
       <c r="PT4">
         <v>60</v>
       </c>
+      <c r="PU4">
+        <v>66</v>
+      </c>
+      <c r="PV4">
+        <v>69</v>
+      </c>
+      <c r="PW4">
+        <v>72</v>
+      </c>
+      <c r="PX4">
+        <v>72</v>
+      </c>
+      <c r="PY4">
+        <v>68</v>
+      </c>
+      <c r="PZ4">
+        <v>74</v>
+      </c>
+      <c r="QA4">
+        <v>67</v>
+      </c>
     </row>
-    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -57329,8 +58200,29 @@
       <c r="PT5">
         <v>5</v>
       </c>
+      <c r="PU5">
+        <v>4</v>
+      </c>
+      <c r="PV5">
+        <v>4</v>
+      </c>
+      <c r="PW5">
+        <v>6</v>
+      </c>
+      <c r="PX5">
+        <v>8</v>
+      </c>
+      <c r="PY5">
+        <v>8</v>
+      </c>
+      <c r="PZ5">
+        <v>7</v>
+      </c>
+      <c r="QA5">
+        <v>6</v>
+      </c>
     </row>
-    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -58639,8 +59531,29 @@
       <c r="PT6">
         <v>30</v>
       </c>
+      <c r="PU6">
+        <v>29</v>
+      </c>
+      <c r="PV6">
+        <v>27</v>
+      </c>
+      <c r="PW6">
+        <v>27</v>
+      </c>
+      <c r="PX6">
+        <v>27</v>
+      </c>
+      <c r="PY6">
+        <v>25</v>
+      </c>
+      <c r="PZ6">
+        <v>28</v>
+      </c>
+      <c r="QA6">
+        <v>27</v>
+      </c>
     </row>
-    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -59949,8 +60862,29 @@
       <c r="PT7">
         <v>104</v>
       </c>
+      <c r="PU7">
+        <v>105</v>
+      </c>
+      <c r="PV7">
+        <v>104</v>
+      </c>
+      <c r="PW7">
+        <v>114</v>
+      </c>
+      <c r="PX7">
+        <v>109</v>
+      </c>
+      <c r="PY7">
+        <v>110</v>
+      </c>
+      <c r="PZ7">
+        <v>114</v>
+      </c>
+      <c r="QA7">
+        <v>109</v>
+      </c>
     </row>
-    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -61259,8 +62193,29 @@
       <c r="PT8">
         <v>606</v>
       </c>
+      <c r="PU8">
+        <v>623</v>
+      </c>
+      <c r="PV8">
+        <v>632</v>
+      </c>
+      <c r="PW8">
+        <v>632</v>
+      </c>
+      <c r="PX8">
+        <v>657</v>
+      </c>
+      <c r="PY8">
+        <v>660</v>
+      </c>
+      <c r="PZ8">
+        <v>662</v>
+      </c>
+      <c r="QA8">
+        <v>684</v>
+      </c>
     </row>
-    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -62569,8 +63524,29 @@
       <c r="PT9">
         <v>27</v>
       </c>
+      <c r="PU9">
+        <v>33</v>
+      </c>
+      <c r="PV9">
+        <v>28</v>
+      </c>
+      <c r="PW9">
+        <v>30</v>
+      </c>
+      <c r="PX9">
+        <v>34</v>
+      </c>
+      <c r="PY9">
+        <v>29</v>
+      </c>
+      <c r="PZ9">
+        <v>31</v>
+      </c>
+      <c r="QA9">
+        <v>24</v>
+      </c>
     </row>
-    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -63879,8 +64855,29 @@
       <c r="PT10">
         <v>17</v>
       </c>
+      <c r="PU10">
+        <v>23</v>
+      </c>
+      <c r="PV10">
+        <v>24</v>
+      </c>
+      <c r="PW10">
+        <v>22</v>
+      </c>
+      <c r="PX10">
+        <v>23</v>
+      </c>
+      <c r="PY10">
+        <v>25</v>
+      </c>
+      <c r="PZ10">
+        <v>25</v>
+      </c>
+      <c r="QA10">
+        <v>28</v>
+      </c>
     </row>
-    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -65189,8 +66186,29 @@
       <c r="PT11">
         <v>18</v>
       </c>
+      <c r="PU11">
+        <v>18</v>
+      </c>
+      <c r="PV11">
+        <v>17</v>
+      </c>
+      <c r="PW11">
+        <v>16</v>
+      </c>
+      <c r="PX11">
+        <v>17</v>
+      </c>
+      <c r="PY11">
+        <v>18</v>
+      </c>
+      <c r="PZ11">
+        <v>18</v>
+      </c>
+      <c r="QA11">
+        <v>18</v>
+      </c>
     </row>
-    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -66499,8 +67517,29 @@
       <c r="PT12">
         <v>103</v>
       </c>
+      <c r="PU12">
+        <v>102</v>
+      </c>
+      <c r="PV12">
+        <v>107</v>
+      </c>
+      <c r="PW12">
+        <v>103</v>
+      </c>
+      <c r="PX12">
+        <v>101</v>
+      </c>
+      <c r="PY12">
+        <v>99</v>
+      </c>
+      <c r="PZ12">
+        <v>101</v>
+      </c>
+      <c r="QA12">
+        <v>110</v>
+      </c>
     </row>
-    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -67809,8 +68848,29 @@
       <c r="PT13">
         <v>32</v>
       </c>
+      <c r="PU13">
+        <v>34</v>
+      </c>
+      <c r="PV13">
+        <v>43</v>
+      </c>
+      <c r="PW13">
+        <v>44</v>
+      </c>
+      <c r="PX13">
+        <v>48</v>
+      </c>
+      <c r="PY13">
+        <v>45</v>
+      </c>
+      <c r="PZ13">
+        <v>44</v>
+      </c>
+      <c r="QA13">
+        <v>41</v>
+      </c>
     </row>
-    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -69119,8 +70179,29 @@
       <c r="PT14">
         <v>14</v>
       </c>
+      <c r="PU14">
+        <v>14</v>
+      </c>
+      <c r="PV14">
+        <v>13</v>
+      </c>
+      <c r="PW14">
+        <v>13</v>
+      </c>
+      <c r="PX14">
+        <v>12</v>
+      </c>
+      <c r="PY14">
+        <v>13</v>
+      </c>
+      <c r="PZ14">
+        <v>13</v>
+      </c>
+      <c r="QA14">
+        <v>14</v>
+      </c>
     </row>
-    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -70429,8 +71510,29 @@
       <c r="PT15">
         <v>33</v>
       </c>
+      <c r="PU15">
+        <v>32</v>
+      </c>
+      <c r="PV15">
+        <v>39</v>
+      </c>
+      <c r="PW15">
+        <v>42</v>
+      </c>
+      <c r="PX15">
+        <v>43</v>
+      </c>
+      <c r="PY15">
+        <v>39</v>
+      </c>
+      <c r="PZ15">
+        <v>44</v>
+      </c>
+      <c r="QA15">
+        <v>44</v>
+      </c>
     </row>
-    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -71739,8 +72841,29 @@
       <c r="PT16">
         <v>0</v>
       </c>
+      <c r="PU16">
+        <v>0</v>
+      </c>
+      <c r="PV16">
+        <v>0</v>
+      </c>
+      <c r="PW16">
+        <v>0</v>
+      </c>
+      <c r="PX16">
+        <v>0</v>
+      </c>
+      <c r="PY16">
+        <v>1</v>
+      </c>
+      <c r="PZ16">
+        <v>2</v>
+      </c>
+      <c r="QA16">
+        <v>4</v>
+      </c>
     </row>
-    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -73049,8 +74172,29 @@
       <c r="PT17">
         <v>8</v>
       </c>
+      <c r="PU17">
+        <v>10</v>
+      </c>
+      <c r="PV17">
+        <v>9</v>
+      </c>
+      <c r="PW17">
+        <v>10</v>
+      </c>
+      <c r="PX17">
+        <v>9</v>
+      </c>
+      <c r="PY17">
+        <v>10</v>
+      </c>
+      <c r="PZ17">
+        <v>9</v>
+      </c>
+      <c r="QA17">
+        <v>9</v>
+      </c>
     </row>
-    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -74359,48 +75503,69 @@
       <c r="PT18" s="20">
         <v>1067</v>
       </c>
+      <c r="PU18" s="20">
+        <v>1100</v>
+      </c>
+      <c r="PV18" s="20">
+        <v>1123</v>
+      </c>
+      <c r="PW18" s="20">
+        <v>1140</v>
+      </c>
+      <c r="PX18" s="20">
+        <v>1166</v>
+      </c>
+      <c r="PY18" s="20">
+        <v>1155</v>
+      </c>
+      <c r="PZ18" s="20">
+        <v>1178</v>
+      </c>
+      <c r="QA18" s="20">
+        <v>1193</v>
+      </c>
     </row>
-    <row r="19" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA19" s="1"/>
       <c r="KP19" s="9"/>
     </row>
-    <row r="20" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA20" s="1"/>
     </row>
-    <row r="21" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA21" s="1"/>
     </row>
-    <row r="22" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA22" s="1"/>
     </row>
-    <row r="23" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA23" s="1"/>
     </row>
-    <row r="24" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA24" s="1"/>
     </row>
-    <row r="25" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA25" s="1"/>
     </row>
-    <row r="26" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA26" s="1"/>
     </row>
-    <row r="27" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA27" s="1"/>
     </row>
-    <row r="28" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA28" s="1"/>
     </row>
-    <row r="29" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA29" s="1"/>
     </row>
-    <row r="30" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA30" s="1"/>
     </row>
-    <row r="31" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA31" s="1"/>
     </row>
-    <row r="32" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:443" x14ac:dyDescent="0.25">
       <c r="BA32" s="1"/>
     </row>
     <row r="33" spans="53:53" x14ac:dyDescent="0.25">
@@ -74411,1177 +75576,1177 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:JP17">
-    <cfRule type="cellIs" dxfId="258" priority="317" operator="lessThan">
+    <cfRule type="cellIs" dxfId="259" priority="317" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DE2:DH2">
-    <cfRule type="cellIs" dxfId="257" priority="316" operator="lessThan">
+    <cfRule type="cellIs" dxfId="258" priority="316" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL2">
-    <cfRule type="cellIs" dxfId="256" priority="236" operator="lessThan">
+    <cfRule type="cellIs" dxfId="257" priority="236" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL2">
-    <cfRule type="cellIs" dxfId="255" priority="235" operator="lessThan">
+    <cfRule type="cellIs" dxfId="256" priority="235" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:JP17 B18:JN18">
-    <cfRule type="cellIs" dxfId="254" priority="238" operator="lessThan">
+    <cfRule type="cellIs" dxfId="255" priority="238" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:JP17">
-    <cfRule type="cellIs" dxfId="253" priority="237" operator="lessThan">
+    <cfRule type="cellIs" dxfId="254" priority="237" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI3:DL18">
-    <cfRule type="cellIs" dxfId="252" priority="234" operator="lessThan">
+    <cfRule type="cellIs" dxfId="253" priority="234" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DI2:DL17">
-    <cfRule type="cellIs" dxfId="251" priority="233" operator="lessThan">
+    <cfRule type="cellIs" dxfId="252" priority="233" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE2">
-    <cfRule type="cellIs" dxfId="250" priority="232" operator="lessThan">
+    <cfRule type="cellIs" dxfId="251" priority="232" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE2">
-    <cfRule type="cellIs" dxfId="249" priority="231" operator="lessThan">
+    <cfRule type="cellIs" dxfId="250" priority="231" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM3:FE18">
-    <cfRule type="cellIs" dxfId="248" priority="230" operator="lessThan">
+    <cfRule type="cellIs" dxfId="249" priority="230" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DM2:FE17">
-    <cfRule type="cellIs" dxfId="247" priority="229" operator="lessThan">
+    <cfRule type="cellIs" dxfId="248" priority="229" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2">
-    <cfRule type="cellIs" dxfId="246" priority="228" operator="lessThan">
+    <cfRule type="cellIs" dxfId="247" priority="228" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2">
-    <cfRule type="cellIs" dxfId="245" priority="227" operator="lessThan">
+    <cfRule type="cellIs" dxfId="246" priority="227" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF3:FF18">
-    <cfRule type="cellIs" dxfId="244" priority="226" operator="lessThan">
+    <cfRule type="cellIs" dxfId="245" priority="226" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FF2:FF17">
-    <cfRule type="cellIs" dxfId="243" priority="225" operator="lessThan">
+    <cfRule type="cellIs" dxfId="244" priority="225" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2">
-    <cfRule type="cellIs" dxfId="242" priority="224" operator="lessThan">
+    <cfRule type="cellIs" dxfId="243" priority="224" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2">
-    <cfRule type="cellIs" dxfId="241" priority="223" operator="lessThan">
+    <cfRule type="cellIs" dxfId="242" priority="223" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG3:FG18">
-    <cfRule type="cellIs" dxfId="240" priority="222" operator="lessThan">
+    <cfRule type="cellIs" dxfId="241" priority="222" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FG2:FG17">
-    <cfRule type="cellIs" dxfId="239" priority="221" operator="lessThan">
+    <cfRule type="cellIs" dxfId="240" priority="221" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2">
-    <cfRule type="cellIs" dxfId="238" priority="220" operator="lessThan">
+    <cfRule type="cellIs" dxfId="239" priority="220" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2">
-    <cfRule type="cellIs" dxfId="237" priority="219" operator="lessThan">
+    <cfRule type="cellIs" dxfId="238" priority="219" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH3:FH18">
-    <cfRule type="cellIs" dxfId="236" priority="218" operator="lessThan">
+    <cfRule type="cellIs" dxfId="237" priority="218" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FH2:FH17">
-    <cfRule type="cellIs" dxfId="235" priority="217" operator="lessThan">
+    <cfRule type="cellIs" dxfId="236" priority="217" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2">
-    <cfRule type="cellIs" dxfId="234" priority="216" operator="lessThan">
+    <cfRule type="cellIs" dxfId="235" priority="216" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2">
-    <cfRule type="cellIs" dxfId="233" priority="215" operator="lessThan">
+    <cfRule type="cellIs" dxfId="234" priority="215" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI3:FI18">
-    <cfRule type="cellIs" dxfId="232" priority="214" operator="lessThan">
+    <cfRule type="cellIs" dxfId="233" priority="214" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI2:FI17">
-    <cfRule type="cellIs" dxfId="231" priority="213" operator="lessThan">
+    <cfRule type="cellIs" dxfId="232" priority="213" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2">
-    <cfRule type="cellIs" dxfId="230" priority="212" operator="lessThan">
+    <cfRule type="cellIs" dxfId="231" priority="212" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2">
-    <cfRule type="cellIs" dxfId="229" priority="211" operator="lessThan">
+    <cfRule type="cellIs" dxfId="230" priority="211" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ3:FJ18">
-    <cfRule type="cellIs" dxfId="228" priority="210" operator="lessThan">
+    <cfRule type="cellIs" dxfId="229" priority="210" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FJ2:FJ17">
-    <cfRule type="cellIs" dxfId="227" priority="209" operator="lessThan">
+    <cfRule type="cellIs" dxfId="228" priority="209" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2">
-    <cfRule type="cellIs" dxfId="226" priority="208" operator="lessThan">
+    <cfRule type="cellIs" dxfId="227" priority="208" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2">
-    <cfRule type="cellIs" dxfId="225" priority="207" operator="lessThan">
+    <cfRule type="cellIs" dxfId="226" priority="207" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK3:FK18">
-    <cfRule type="cellIs" dxfId="224" priority="206" operator="lessThan">
+    <cfRule type="cellIs" dxfId="225" priority="206" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FK2:FK17">
-    <cfRule type="cellIs" dxfId="223" priority="205" operator="lessThan">
+    <cfRule type="cellIs" dxfId="224" priority="205" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2">
-    <cfRule type="cellIs" dxfId="222" priority="204" operator="lessThan">
+    <cfRule type="cellIs" dxfId="223" priority="204" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2">
-    <cfRule type="cellIs" dxfId="221" priority="203" operator="lessThan">
+    <cfRule type="cellIs" dxfId="222" priority="203" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL3:FL18">
-    <cfRule type="cellIs" dxfId="220" priority="202" operator="lessThan">
+    <cfRule type="cellIs" dxfId="221" priority="202" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FL2:FL17">
-    <cfRule type="cellIs" dxfId="219" priority="201" operator="lessThan">
+    <cfRule type="cellIs" dxfId="220" priority="201" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2">
-    <cfRule type="cellIs" dxfId="218" priority="200" operator="lessThan">
+    <cfRule type="cellIs" dxfId="219" priority="200" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2">
-    <cfRule type="cellIs" dxfId="217" priority="199" operator="lessThan">
+    <cfRule type="cellIs" dxfId="218" priority="199" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM3:FM18">
-    <cfRule type="cellIs" dxfId="216" priority="198" operator="lessThan">
+    <cfRule type="cellIs" dxfId="217" priority="198" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FM2:FM17">
-    <cfRule type="cellIs" dxfId="215" priority="197" operator="lessThan">
+    <cfRule type="cellIs" dxfId="216" priority="197" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2">
-    <cfRule type="cellIs" dxfId="214" priority="196" operator="lessThan">
+    <cfRule type="cellIs" dxfId="215" priority="196" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2">
-    <cfRule type="cellIs" dxfId="213" priority="195" operator="lessThan">
+    <cfRule type="cellIs" dxfId="214" priority="195" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN3:FN18">
-    <cfRule type="cellIs" dxfId="212" priority="194" operator="lessThan">
+    <cfRule type="cellIs" dxfId="213" priority="194" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FN2:FN17">
-    <cfRule type="cellIs" dxfId="211" priority="193" operator="lessThan">
+    <cfRule type="cellIs" dxfId="212" priority="193" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2">
-    <cfRule type="cellIs" dxfId="210" priority="192" operator="lessThan">
+    <cfRule type="cellIs" dxfId="211" priority="192" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2">
-    <cfRule type="cellIs" dxfId="209" priority="191" operator="lessThan">
+    <cfRule type="cellIs" dxfId="210" priority="191" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO3:FO18">
-    <cfRule type="cellIs" dxfId="208" priority="190" operator="lessThan">
+    <cfRule type="cellIs" dxfId="209" priority="190" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FO2:FO17">
-    <cfRule type="cellIs" dxfId="207" priority="189" operator="lessThan">
+    <cfRule type="cellIs" dxfId="208" priority="189" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP18:GB18">
-    <cfRule type="cellIs" dxfId="206" priority="188" operator="lessThan">
+    <cfRule type="cellIs" dxfId="207" priority="188" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB2">
-    <cfRule type="cellIs" dxfId="205" priority="187" operator="lessThan">
+    <cfRule type="cellIs" dxfId="206" priority="187" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB2">
-    <cfRule type="cellIs" dxfId="204" priority="186" operator="lessThan">
+    <cfRule type="cellIs" dxfId="205" priority="186" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP3:GB17">
-    <cfRule type="cellIs" dxfId="203" priority="185" operator="lessThan">
+    <cfRule type="cellIs" dxfId="204" priority="185" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FP2:GB17">
-    <cfRule type="cellIs" dxfId="202" priority="184" operator="lessThan">
+    <cfRule type="cellIs" dxfId="203" priority="184" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC18:GL18">
-    <cfRule type="cellIs" dxfId="201" priority="183" operator="lessThan">
+    <cfRule type="cellIs" dxfId="202" priority="183" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL2">
-    <cfRule type="cellIs" dxfId="200" priority="182" operator="lessThan">
+    <cfRule type="cellIs" dxfId="201" priority="182" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL2">
-    <cfRule type="cellIs" dxfId="199" priority="181" operator="lessThan">
+    <cfRule type="cellIs" dxfId="200" priority="181" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC3:GL17">
-    <cfRule type="cellIs" dxfId="198" priority="180" operator="lessThan">
+    <cfRule type="cellIs" dxfId="199" priority="180" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GC2:GL17">
-    <cfRule type="cellIs" dxfId="197" priority="179" operator="lessThan">
+    <cfRule type="cellIs" dxfId="198" priority="179" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM18">
-    <cfRule type="cellIs" dxfId="196" priority="178" operator="lessThan">
+    <cfRule type="cellIs" dxfId="197" priority="178" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2">
-    <cfRule type="cellIs" dxfId="195" priority="177" operator="lessThan">
+    <cfRule type="cellIs" dxfId="196" priority="177" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2">
-    <cfRule type="cellIs" dxfId="194" priority="176" operator="lessThan">
+    <cfRule type="cellIs" dxfId="195" priority="176" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM3:GM17">
-    <cfRule type="cellIs" dxfId="193" priority="175" operator="lessThan">
+    <cfRule type="cellIs" dxfId="194" priority="175" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GM2:GM17">
-    <cfRule type="cellIs" dxfId="192" priority="174" operator="lessThan">
+    <cfRule type="cellIs" dxfId="193" priority="174" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN18">
-    <cfRule type="cellIs" dxfId="191" priority="173" operator="lessThan">
+    <cfRule type="cellIs" dxfId="192" priority="173" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2">
-    <cfRule type="cellIs" dxfId="190" priority="172" operator="lessThan">
+    <cfRule type="cellIs" dxfId="191" priority="172" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2">
-    <cfRule type="cellIs" dxfId="189" priority="171" operator="lessThan">
+    <cfRule type="cellIs" dxfId="190" priority="171" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN3:GN17">
-    <cfRule type="cellIs" dxfId="188" priority="170" operator="lessThan">
+    <cfRule type="cellIs" dxfId="189" priority="170" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GN2:GN17">
-    <cfRule type="cellIs" dxfId="187" priority="169" operator="lessThan">
+    <cfRule type="cellIs" dxfId="188" priority="169" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO18">
-    <cfRule type="cellIs" dxfId="186" priority="168" operator="lessThan">
+    <cfRule type="cellIs" dxfId="187" priority="168" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2">
-    <cfRule type="cellIs" dxfId="185" priority="167" operator="lessThan">
+    <cfRule type="cellIs" dxfId="186" priority="167" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2">
-    <cfRule type="cellIs" dxfId="184" priority="166" operator="lessThan">
+    <cfRule type="cellIs" dxfId="185" priority="166" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO3:GO17">
-    <cfRule type="cellIs" dxfId="183" priority="165" operator="lessThan">
+    <cfRule type="cellIs" dxfId="184" priority="165" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GO2:GO17">
-    <cfRule type="cellIs" dxfId="182" priority="164" operator="lessThan">
+    <cfRule type="cellIs" dxfId="183" priority="164" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP18">
-    <cfRule type="cellIs" dxfId="181" priority="163" operator="lessThan">
+    <cfRule type="cellIs" dxfId="182" priority="163" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2">
-    <cfRule type="cellIs" dxfId="180" priority="162" operator="lessThan">
+    <cfRule type="cellIs" dxfId="181" priority="162" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2">
-    <cfRule type="cellIs" dxfId="179" priority="161" operator="lessThan">
+    <cfRule type="cellIs" dxfId="180" priority="161" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP3:GP17">
-    <cfRule type="cellIs" dxfId="178" priority="160" operator="lessThan">
+    <cfRule type="cellIs" dxfId="179" priority="160" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GP2:GP17">
-    <cfRule type="cellIs" dxfId="177" priority="159" operator="lessThan">
+    <cfRule type="cellIs" dxfId="178" priority="159" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ18:GV18">
-    <cfRule type="cellIs" dxfId="176" priority="158" operator="lessThan">
+    <cfRule type="cellIs" dxfId="177" priority="158" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV2">
-    <cfRule type="cellIs" dxfId="175" priority="157" operator="lessThan">
+    <cfRule type="cellIs" dxfId="176" priority="157" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV2">
-    <cfRule type="cellIs" dxfId="174" priority="156" operator="lessThan">
+    <cfRule type="cellIs" dxfId="175" priority="156" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ3:GV17">
-    <cfRule type="cellIs" dxfId="173" priority="155" operator="lessThan">
+    <cfRule type="cellIs" dxfId="174" priority="155" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GQ2:GV17">
-    <cfRule type="cellIs" dxfId="172" priority="154" operator="lessThan">
+    <cfRule type="cellIs" dxfId="173" priority="154" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW18">
-    <cfRule type="cellIs" dxfId="171" priority="153" operator="lessThan">
+    <cfRule type="cellIs" dxfId="172" priority="153" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2">
-    <cfRule type="cellIs" dxfId="170" priority="152" operator="lessThan">
+    <cfRule type="cellIs" dxfId="171" priority="152" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2">
-    <cfRule type="cellIs" dxfId="169" priority="151" operator="lessThan">
+    <cfRule type="cellIs" dxfId="170" priority="151" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW3:GW17">
-    <cfRule type="cellIs" dxfId="168" priority="150" operator="lessThan">
+    <cfRule type="cellIs" dxfId="169" priority="150" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GW2:GW17">
-    <cfRule type="cellIs" dxfId="167" priority="149" operator="lessThan">
+    <cfRule type="cellIs" dxfId="168" priority="149" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX18">
-    <cfRule type="cellIs" dxfId="166" priority="148" operator="lessThan">
+    <cfRule type="cellIs" dxfId="167" priority="148" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2">
-    <cfRule type="cellIs" dxfId="165" priority="147" operator="lessThan">
+    <cfRule type="cellIs" dxfId="166" priority="147" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2">
-    <cfRule type="cellIs" dxfId="164" priority="146" operator="lessThan">
+    <cfRule type="cellIs" dxfId="165" priority="146" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX3:GX17">
-    <cfRule type="cellIs" dxfId="163" priority="145" operator="lessThan">
+    <cfRule type="cellIs" dxfId="164" priority="145" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GX2:GX17">
-    <cfRule type="cellIs" dxfId="162" priority="144" operator="lessThan">
+    <cfRule type="cellIs" dxfId="163" priority="144" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY18">
-    <cfRule type="cellIs" dxfId="161" priority="143" operator="lessThan">
+    <cfRule type="cellIs" dxfId="162" priority="143" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2">
-    <cfRule type="cellIs" dxfId="160" priority="142" operator="lessThan">
+    <cfRule type="cellIs" dxfId="161" priority="142" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2">
-    <cfRule type="cellIs" dxfId="159" priority="141" operator="lessThan">
+    <cfRule type="cellIs" dxfId="160" priority="141" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY3:GY17">
-    <cfRule type="cellIs" dxfId="158" priority="140" operator="lessThan">
+    <cfRule type="cellIs" dxfId="159" priority="140" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GY2:GY17">
-    <cfRule type="cellIs" dxfId="157" priority="139" operator="lessThan">
+    <cfRule type="cellIs" dxfId="158" priority="139" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ18:HF18">
-    <cfRule type="cellIs" dxfId="156" priority="138" operator="lessThan">
+    <cfRule type="cellIs" dxfId="157" priority="138" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF2">
-    <cfRule type="cellIs" dxfId="155" priority="137" operator="lessThan">
+    <cfRule type="cellIs" dxfId="156" priority="137" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF2">
-    <cfRule type="cellIs" dxfId="154" priority="136" operator="lessThan">
+    <cfRule type="cellIs" dxfId="155" priority="136" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ3:HF17">
-    <cfRule type="cellIs" dxfId="153" priority="135" operator="lessThan">
+    <cfRule type="cellIs" dxfId="154" priority="135" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="GZ2:HF17">
-    <cfRule type="cellIs" dxfId="152" priority="134" operator="lessThan">
+    <cfRule type="cellIs" dxfId="153" priority="134" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG18">
-    <cfRule type="cellIs" dxfId="151" priority="128" operator="lessThan">
+    <cfRule type="cellIs" dxfId="152" priority="128" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2">
-    <cfRule type="cellIs" dxfId="150" priority="127" operator="lessThan">
+    <cfRule type="cellIs" dxfId="151" priority="127" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2">
-    <cfRule type="cellIs" dxfId="149" priority="126" operator="lessThan">
+    <cfRule type="cellIs" dxfId="150" priority="126" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG3:HG17">
-    <cfRule type="cellIs" dxfId="148" priority="125" operator="lessThan">
+    <cfRule type="cellIs" dxfId="149" priority="125" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HG2:HG17">
-    <cfRule type="cellIs" dxfId="147" priority="124" operator="lessThan">
+    <cfRule type="cellIs" dxfId="148" priority="124" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH18">
-    <cfRule type="cellIs" dxfId="146" priority="123" operator="lessThan">
+    <cfRule type="cellIs" dxfId="147" priority="123" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2">
-    <cfRule type="cellIs" dxfId="145" priority="122" operator="lessThan">
+    <cfRule type="cellIs" dxfId="146" priority="122" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2">
-    <cfRule type="cellIs" dxfId="144" priority="121" operator="lessThan">
+    <cfRule type="cellIs" dxfId="145" priority="121" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH3:HH17">
-    <cfRule type="cellIs" dxfId="143" priority="120" operator="lessThan">
+    <cfRule type="cellIs" dxfId="144" priority="120" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HH2:HH17">
-    <cfRule type="cellIs" dxfId="142" priority="119" operator="lessThan">
+    <cfRule type="cellIs" dxfId="143" priority="119" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI18">
-    <cfRule type="cellIs" dxfId="141" priority="118" operator="lessThan">
+    <cfRule type="cellIs" dxfId="142" priority="118" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2">
-    <cfRule type="cellIs" dxfId="140" priority="117" operator="lessThan">
+    <cfRule type="cellIs" dxfId="141" priority="117" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2">
-    <cfRule type="cellIs" dxfId="139" priority="116" operator="lessThan">
+    <cfRule type="cellIs" dxfId="140" priority="116" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI3:HI17">
-    <cfRule type="cellIs" dxfId="138" priority="115" operator="lessThan">
+    <cfRule type="cellIs" dxfId="139" priority="115" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HI2:HI17">
-    <cfRule type="cellIs" dxfId="137" priority="114" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="114" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ18">
-    <cfRule type="cellIs" dxfId="136" priority="113" operator="lessThan">
+    <cfRule type="cellIs" dxfId="137" priority="113" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2">
-    <cfRule type="cellIs" dxfId="135" priority="112" operator="lessThan">
+    <cfRule type="cellIs" dxfId="136" priority="112" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2">
-    <cfRule type="cellIs" dxfId="134" priority="111" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="111" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ3:HJ17">
-    <cfRule type="cellIs" dxfId="133" priority="110" operator="lessThan">
+    <cfRule type="cellIs" dxfId="134" priority="110" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HJ2:HJ17">
-    <cfRule type="cellIs" dxfId="132" priority="109" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="109" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK18">
-    <cfRule type="cellIs" dxfId="131" priority="108" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="108" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2">
-    <cfRule type="cellIs" dxfId="130" priority="107" operator="lessThan">
+    <cfRule type="cellIs" dxfId="131" priority="107" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2">
-    <cfRule type="cellIs" dxfId="129" priority="106" operator="lessThan">
+    <cfRule type="cellIs" dxfId="130" priority="106" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK3:HK17">
-    <cfRule type="cellIs" dxfId="128" priority="105" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="105" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HK2:HK17">
-    <cfRule type="cellIs" dxfId="127" priority="104" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="104" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL18">
-    <cfRule type="cellIs" dxfId="126" priority="103" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="103" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2">
-    <cfRule type="cellIs" dxfId="125" priority="102" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="102" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2">
-    <cfRule type="cellIs" dxfId="124" priority="101" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="101" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL3:HL17">
-    <cfRule type="cellIs" dxfId="123" priority="100" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="100" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HL2:HL17">
-    <cfRule type="cellIs" dxfId="122" priority="99" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="99" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM18">
-    <cfRule type="cellIs" dxfId="121" priority="98" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="98" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2">
-    <cfRule type="cellIs" dxfId="120" priority="97" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="97" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2">
-    <cfRule type="cellIs" dxfId="119" priority="96" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="96" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM3:HM17">
-    <cfRule type="cellIs" dxfId="118" priority="95" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="95" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HM2:HM17">
-    <cfRule type="cellIs" dxfId="117" priority="94" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="94" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN18">
-    <cfRule type="cellIs" dxfId="116" priority="93" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="93" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2">
-    <cfRule type="cellIs" dxfId="115" priority="92" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="92" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2">
-    <cfRule type="cellIs" dxfId="114" priority="91" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="91" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN3:HN17">
-    <cfRule type="cellIs" dxfId="113" priority="90" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="90" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HN2:HN17">
-    <cfRule type="cellIs" dxfId="112" priority="89" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="89" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO18">
-    <cfRule type="cellIs" dxfId="111" priority="88" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="88" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2">
-    <cfRule type="cellIs" dxfId="110" priority="87" operator="lessThan">
+    <cfRule type="cellIs" dxfId="111" priority="87" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2">
-    <cfRule type="cellIs" dxfId="109" priority="86" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="86" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO3:HO17">
-    <cfRule type="cellIs" dxfId="108" priority="85" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="85" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HO2:HO17">
-    <cfRule type="cellIs" dxfId="107" priority="84" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="84" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP18">
-    <cfRule type="cellIs" dxfId="106" priority="83" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="83" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2">
-    <cfRule type="cellIs" dxfId="105" priority="82" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="82" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2">
-    <cfRule type="cellIs" dxfId="104" priority="81" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="81" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP3:HP17">
-    <cfRule type="cellIs" dxfId="103" priority="80" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="80" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HP2:HP17">
-    <cfRule type="cellIs" dxfId="102" priority="79" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="79" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ18">
-    <cfRule type="cellIs" dxfId="101" priority="78" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="78" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2">
-    <cfRule type="cellIs" dxfId="100" priority="77" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="77" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2">
-    <cfRule type="cellIs" dxfId="99" priority="76" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="76" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ3:HQ17">
-    <cfRule type="cellIs" dxfId="98" priority="75" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="75" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HQ2:HQ17">
-    <cfRule type="cellIs" dxfId="97" priority="74" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="74" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR18:HZ18">
-    <cfRule type="cellIs" dxfId="96" priority="73" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="73" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ2">
-    <cfRule type="cellIs" dxfId="95" priority="72" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="72" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ2">
-    <cfRule type="cellIs" dxfId="94" priority="71" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="71" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR3:HZ17">
-    <cfRule type="cellIs" dxfId="93" priority="70" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="70" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="HR2:HZ17">
-    <cfRule type="cellIs" dxfId="92" priority="69" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="69" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA18">
-    <cfRule type="cellIs" dxfId="91" priority="68" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="68" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2">
-    <cfRule type="cellIs" dxfId="90" priority="67" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="67" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2">
-    <cfRule type="cellIs" dxfId="89" priority="66" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="66" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA3:IA17">
-    <cfRule type="cellIs" dxfId="88" priority="65" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="65" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IA2:IA17">
-    <cfRule type="cellIs" dxfId="87" priority="64" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="64" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB18:IG18">
-    <cfRule type="cellIs" dxfId="86" priority="63" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="63" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG2">
-    <cfRule type="cellIs" dxfId="85" priority="62" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="62" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG2">
-    <cfRule type="cellIs" dxfId="84" priority="61" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="61" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB3:IG17">
-    <cfRule type="cellIs" dxfId="83" priority="60" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="60" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IB2:IG17">
-    <cfRule type="cellIs" dxfId="82" priority="59" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="59" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH18:IL18">
-    <cfRule type="cellIs" dxfId="81" priority="58" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="58" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL2">
-    <cfRule type="cellIs" dxfId="80" priority="57" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="57" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL2">
-    <cfRule type="cellIs" dxfId="79" priority="56" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="56" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH3:IL17">
-    <cfRule type="cellIs" dxfId="78" priority="55" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="55" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IH2:IL17">
-    <cfRule type="cellIs" dxfId="77" priority="54" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="54" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM18:IT18">
-    <cfRule type="cellIs" dxfId="76" priority="53" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="53" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT2">
-    <cfRule type="cellIs" dxfId="75" priority="52" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="52" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT2">
-    <cfRule type="cellIs" dxfId="74" priority="51" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="51" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM3:IT17">
-    <cfRule type="cellIs" dxfId="73" priority="50" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="50" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IM2:IT17">
-    <cfRule type="cellIs" dxfId="72" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="49" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU18">
-    <cfRule type="cellIs" dxfId="71" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="48" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2">
-    <cfRule type="cellIs" dxfId="70" priority="47" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="47" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2">
-    <cfRule type="cellIs" dxfId="69" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="46" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU3:IU17">
-    <cfRule type="cellIs" dxfId="68" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="45" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IU2:IU17">
-    <cfRule type="cellIs" dxfId="67" priority="44" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="44" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV18">
-    <cfRule type="cellIs" dxfId="66" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="43" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2">
-    <cfRule type="cellIs" dxfId="65" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="42" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2">
-    <cfRule type="cellIs" dxfId="64" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="41" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV3:IV17">
-    <cfRule type="cellIs" dxfId="63" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="40" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IV2:IV17">
-    <cfRule type="cellIs" dxfId="62" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="39" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW18">
-    <cfRule type="cellIs" dxfId="61" priority="38" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="38" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2">
-    <cfRule type="cellIs" dxfId="60" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="37" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2">
-    <cfRule type="cellIs" dxfId="59" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="36" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW3:IW17">
-    <cfRule type="cellIs" dxfId="58" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="35" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IW2:IW17">
-    <cfRule type="cellIs" dxfId="57" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="34" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX18">
-    <cfRule type="cellIs" dxfId="56" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="33" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2">
-    <cfRule type="cellIs" dxfId="55" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="32" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2">
-    <cfRule type="cellIs" dxfId="54" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="31" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX3:IX17">
-    <cfRule type="cellIs" dxfId="53" priority="30" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="30" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IX2:IX17">
-    <cfRule type="cellIs" dxfId="52" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="29" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY18">
-    <cfRule type="cellIs" dxfId="51" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="28" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2">
-    <cfRule type="cellIs" dxfId="50" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="27" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2">
-    <cfRule type="cellIs" dxfId="49" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="26" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY3:IY17">
-    <cfRule type="cellIs" dxfId="48" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="25" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IY2:IY17">
-    <cfRule type="cellIs" dxfId="47" priority="24" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ18">
-    <cfRule type="cellIs" dxfId="46" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="23" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2">
-    <cfRule type="cellIs" dxfId="45" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="22" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2">
-    <cfRule type="cellIs" dxfId="44" priority="21" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="21" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ3:IZ17">
-    <cfRule type="cellIs" dxfId="43" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="IZ2:IZ17">
-    <cfRule type="cellIs" dxfId="42" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA18">
-    <cfRule type="cellIs" dxfId="41" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2">
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2">
-    <cfRule type="cellIs" dxfId="39" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA3:JA17">
-    <cfRule type="cellIs" dxfId="38" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JA2:JA17">
-    <cfRule type="cellIs" dxfId="37" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JO18:JU18">
-    <cfRule type="cellIs" dxfId="36" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JQ2:JQ17">
-    <cfRule type="cellIs" dxfId="35" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JQ2:JQ17">
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JR2:JR17">
-    <cfRule type="cellIs" dxfId="33" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JR2:JR17">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JS2:JS17">
-    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JS2:JS17">
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JT2:JT17">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JT2:JT17">
-    <cfRule type="cellIs" dxfId="28" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JU2:JU17">
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JU2:JU17">
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="JV18:KC18">
-    <cfRule type="cellIs" dxfId="25" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="KD18:KP18">
-    <cfRule type="cellIs" dxfId="24" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -75592,10 +76757,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:PT18"/>
+  <dimension ref="A1:QA18"/>
   <sheetViews>
-    <sheetView topLeftCell="PF1" workbookViewId="0">
-      <selection activeCell="PU11" sqref="PU11"/>
+    <sheetView topLeftCell="PL1" workbookViewId="0">
+      <selection activeCell="PW22" sqref="PW22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -75603,7 +76768,7 @@
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>36</v>
       </c>
@@ -76912,8 +78077,29 @@
       <c r="PT1" s="8">
         <v>44369</v>
       </c>
+      <c r="PU1" s="8">
+        <v>44370</v>
+      </c>
+      <c r="PV1" s="8">
+        <v>44371</v>
+      </c>
+      <c r="PW1" s="8">
+        <v>44372</v>
+      </c>
+      <c r="PX1" s="8">
+        <v>44373</v>
+      </c>
+      <c r="PY1" s="8">
+        <v>44374</v>
+      </c>
+      <c r="PZ1" s="8">
+        <v>44375</v>
+      </c>
+      <c r="QA1" s="8">
+        <v>44376</v>
+      </c>
     </row>
-    <row r="2" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -78222,8 +79408,29 @@
       <c r="PT2">
         <v>9</v>
       </c>
+      <c r="PU2">
+        <v>9</v>
+      </c>
+      <c r="PV2">
+        <v>9</v>
+      </c>
+      <c r="PW2">
+        <v>9</v>
+      </c>
+      <c r="PX2">
+        <v>9</v>
+      </c>
+      <c r="PY2">
+        <v>9</v>
+      </c>
+      <c r="PZ2">
+        <v>9</v>
+      </c>
+      <c r="QA2">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -79532,8 +80739,29 @@
       <c r="PT3">
         <v>12</v>
       </c>
+      <c r="PU3">
+        <v>12</v>
+      </c>
+      <c r="PV3">
+        <v>12</v>
+      </c>
+      <c r="PW3">
+        <v>12</v>
+      </c>
+      <c r="PX3">
+        <v>12</v>
+      </c>
+      <c r="PY3">
+        <v>12</v>
+      </c>
+      <c r="PZ3">
+        <v>12</v>
+      </c>
+      <c r="QA3">
+        <v>12</v>
+      </c>
     </row>
-    <row r="4" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -80842,8 +82070,29 @@
       <c r="PT4">
         <v>48</v>
       </c>
+      <c r="PU4">
+        <v>48</v>
+      </c>
+      <c r="PV4">
+        <v>48</v>
+      </c>
+      <c r="PW4">
+        <v>48</v>
+      </c>
+      <c r="PX4">
+        <v>48</v>
+      </c>
+      <c r="PY4">
+        <v>48</v>
+      </c>
+      <c r="PZ4">
+        <v>48</v>
+      </c>
+      <c r="QA4">
+        <v>48</v>
+      </c>
     </row>
-    <row r="5" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -82152,8 +83401,29 @@
       <c r="PT5">
         <v>11</v>
       </c>
+      <c r="PU5">
+        <v>11</v>
+      </c>
+      <c r="PV5">
+        <v>11</v>
+      </c>
+      <c r="PW5">
+        <v>11</v>
+      </c>
+      <c r="PX5">
+        <v>11</v>
+      </c>
+      <c r="PY5">
+        <v>11</v>
+      </c>
+      <c r="PZ5">
+        <v>11</v>
+      </c>
+      <c r="QA5">
+        <v>11</v>
+      </c>
     </row>
-    <row r="6" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -83462,8 +84732,29 @@
       <c r="PT6">
         <v>29</v>
       </c>
+      <c r="PU6">
+        <v>29</v>
+      </c>
+      <c r="PV6">
+        <v>29</v>
+      </c>
+      <c r="PW6">
+        <v>29</v>
+      </c>
+      <c r="PX6">
+        <v>29</v>
+      </c>
+      <c r="PY6">
+        <v>29</v>
+      </c>
+      <c r="PZ6">
+        <v>29</v>
+      </c>
+      <c r="QA6">
+        <v>29</v>
+      </c>
     </row>
-    <row r="7" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -84772,8 +86063,29 @@
       <c r="PT7">
         <v>125</v>
       </c>
+      <c r="PU7">
+        <v>125</v>
+      </c>
+      <c r="PV7">
+        <v>125</v>
+      </c>
+      <c r="PW7">
+        <v>125</v>
+      </c>
+      <c r="PX7">
+        <v>125</v>
+      </c>
+      <c r="PY7">
+        <v>125</v>
+      </c>
+      <c r="PZ7">
+        <v>125</v>
+      </c>
+      <c r="QA7">
+        <v>125</v>
+      </c>
     </row>
-    <row r="8" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -86082,8 +87394,29 @@
       <c r="PT8">
         <v>745</v>
       </c>
+      <c r="PU8">
+        <v>745</v>
+      </c>
+      <c r="PV8">
+        <v>745</v>
+      </c>
+      <c r="PW8">
+        <v>745</v>
+      </c>
+      <c r="PX8">
+        <v>745</v>
+      </c>
+      <c r="PY8">
+        <v>745</v>
+      </c>
+      <c r="PZ8">
+        <v>745</v>
+      </c>
+      <c r="QA8">
+        <v>745</v>
+      </c>
     </row>
-    <row r="9" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -87392,8 +88725,29 @@
       <c r="PT9">
         <v>61</v>
       </c>
+      <c r="PU9">
+        <v>61</v>
+      </c>
+      <c r="PV9">
+        <v>61</v>
+      </c>
+      <c r="PW9">
+        <v>61</v>
+      </c>
+      <c r="PX9">
+        <v>61</v>
+      </c>
+      <c r="PY9">
+        <v>61</v>
+      </c>
+      <c r="PZ9">
+        <v>61</v>
+      </c>
+      <c r="QA9">
+        <v>61</v>
+      </c>
     </row>
-    <row r="10" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -88702,8 +90056,29 @@
       <c r="PT10">
         <v>45</v>
       </c>
+      <c r="PU10">
+        <v>45</v>
+      </c>
+      <c r="PV10">
+        <v>45</v>
+      </c>
+      <c r="PW10">
+        <v>45</v>
+      </c>
+      <c r="PX10">
+        <v>45</v>
+      </c>
+      <c r="PY10">
+        <v>45</v>
+      </c>
+      <c r="PZ10">
+        <v>45</v>
+      </c>
+      <c r="QA10">
+        <v>45</v>
+      </c>
     </row>
-    <row r="11" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -90012,8 +91387,29 @@
       <c r="PT11">
         <v>16</v>
       </c>
+      <c r="PU11">
+        <v>16</v>
+      </c>
+      <c r="PV11">
+        <v>16</v>
+      </c>
+      <c r="PW11">
+        <v>16</v>
+      </c>
+      <c r="PX11">
+        <v>16</v>
+      </c>
+      <c r="PY11">
+        <v>16</v>
+      </c>
+      <c r="PZ11">
+        <v>16</v>
+      </c>
+      <c r="QA11">
+        <v>16</v>
+      </c>
     </row>
-    <row r="12" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -91322,8 +92718,29 @@
       <c r="PT12">
         <v>97</v>
       </c>
+      <c r="PU12">
+        <v>97</v>
+      </c>
+      <c r="PV12">
+        <v>97</v>
+      </c>
+      <c r="PW12">
+        <v>97</v>
+      </c>
+      <c r="PX12">
+        <v>97</v>
+      </c>
+      <c r="PY12">
+        <v>97</v>
+      </c>
+      <c r="PZ12">
+        <v>97</v>
+      </c>
+      <c r="QA12">
+        <v>97</v>
+      </c>
     </row>
-    <row r="13" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -92632,8 +94049,29 @@
       <c r="PT13">
         <v>49</v>
       </c>
+      <c r="PU13">
+        <v>49</v>
+      </c>
+      <c r="PV13">
+        <v>49</v>
+      </c>
+      <c r="PW13">
+        <v>49</v>
+      </c>
+      <c r="PX13">
+        <v>49</v>
+      </c>
+      <c r="PY13">
+        <v>49</v>
+      </c>
+      <c r="PZ13">
+        <v>49</v>
+      </c>
+      <c r="QA13">
+        <v>49</v>
+      </c>
     </row>
-    <row r="14" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -93942,8 +95380,29 @@
       <c r="PT14">
         <v>13</v>
       </c>
+      <c r="PU14">
+        <v>13</v>
+      </c>
+      <c r="PV14">
+        <v>13</v>
+      </c>
+      <c r="PW14">
+        <v>13</v>
+      </c>
+      <c r="PX14">
+        <v>13</v>
+      </c>
+      <c r="PY14">
+        <v>13</v>
+      </c>
+      <c r="PZ14">
+        <v>13</v>
+      </c>
+      <c r="QA14">
+        <v>13</v>
+      </c>
     </row>
-    <row r="15" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -95252,8 +96711,29 @@
       <c r="PT15">
         <v>49</v>
       </c>
+      <c r="PU15">
+        <v>49</v>
+      </c>
+      <c r="PV15">
+        <v>49</v>
+      </c>
+      <c r="PW15">
+        <v>49</v>
+      </c>
+      <c r="PX15">
+        <v>49</v>
+      </c>
+      <c r="PY15">
+        <v>49</v>
+      </c>
+      <c r="PZ15">
+        <v>49</v>
+      </c>
+      <c r="QA15">
+        <v>49</v>
+      </c>
     </row>
-    <row r="16" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -96562,8 +98042,29 @@
       <c r="PT16">
         <v>8</v>
       </c>
+      <c r="PU16">
+        <v>8</v>
+      </c>
+      <c r="PV16">
+        <v>8</v>
+      </c>
+      <c r="PW16">
+        <v>8</v>
+      </c>
+      <c r="PX16">
+        <v>8</v>
+      </c>
+      <c r="PY16">
+        <v>8</v>
+      </c>
+      <c r="PZ16">
+        <v>8</v>
+      </c>
+      <c r="QA16">
+        <v>8</v>
+      </c>
     </row>
-    <row r="17" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -97872,8 +99373,29 @@
       <c r="PT17">
         <v>14</v>
       </c>
+      <c r="PU17">
+        <v>14</v>
+      </c>
+      <c r="PV17">
+        <v>14</v>
+      </c>
+      <c r="PW17">
+        <v>14</v>
+      </c>
+      <c r="PX17">
+        <v>14</v>
+      </c>
+      <c r="PY17">
+        <v>14</v>
+      </c>
+      <c r="PZ17">
+        <v>14</v>
+      </c>
+      <c r="QA17">
+        <v>14</v>
+      </c>
     </row>
-    <row r="18" spans="1:436" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:443" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -99617,119 +101139,152 @@
         <f t="shared" si="19"/>
         <v>1331</v>
       </c>
+      <c r="PU18" s="6">
+        <f t="shared" ref="PU18:QA18" si="20">SUM(PU2:PU17)</f>
+        <v>1331</v>
+      </c>
+      <c r="PV18" s="6">
+        <f t="shared" si="20"/>
+        <v>1331</v>
+      </c>
+      <c r="PW18" s="6">
+        <f t="shared" si="20"/>
+        <v>1331</v>
+      </c>
+      <c r="PX18" s="6">
+        <f t="shared" si="20"/>
+        <v>1331</v>
+      </c>
+      <c r="PY18" s="6">
+        <f t="shared" si="20"/>
+        <v>1331</v>
+      </c>
+      <c r="PZ18" s="6">
+        <f t="shared" si="20"/>
+        <v>1331</v>
+      </c>
+      <c r="QA18" s="6">
+        <f t="shared" si="20"/>
+        <v>1331</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="23" priority="255" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="256" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3:B18">
+    <cfRule type="cellIs" dxfId="23" priority="254" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B17">
     <cfRule type="cellIs" dxfId="22" priority="253" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B17">
-    <cfRule type="cellIs" dxfId="21" priority="252" operator="lessThan">
+  <conditionalFormatting sqref="C2:MF17">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C3:MF18">
+    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:MF17">
-    <cfRule type="cellIs" dxfId="20" priority="20" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:MF18">
     <cfRule type="cellIs" dxfId="19" priority="19" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:MF17">
+  <conditionalFormatting sqref="MG2:MG17">
     <cfRule type="cellIs" dxfId="18" priority="18" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MG2:MG17">
+  <conditionalFormatting sqref="MG3:MG18">
     <cfRule type="cellIs" dxfId="17" priority="17" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MG3:MG18">
+  <conditionalFormatting sqref="MG2:MG17">
     <cfRule type="cellIs" dxfId="16" priority="16" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MG2:MG17">
+  <conditionalFormatting sqref="MH18">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MH18">
+  <conditionalFormatting sqref="MI18:MN18">
     <cfRule type="cellIs" dxfId="14" priority="14" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MI18:MN18">
+  <conditionalFormatting sqref="MO18:MU18">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MO18:MU18">
+  <conditionalFormatting sqref="MV18:NB18">
     <cfRule type="cellIs" dxfId="12" priority="12" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="MV18:NB18">
+  <conditionalFormatting sqref="NC18:NI18">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NC18:NI18">
+  <conditionalFormatting sqref="NJ18:NP18">
     <cfRule type="cellIs" dxfId="10" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NJ18:NP18">
+  <conditionalFormatting sqref="NQ18:NW18">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NQ18:NW18">
+  <conditionalFormatting sqref="NX18:OD18">
     <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="NX18:OD18">
+  <conditionalFormatting sqref="OE18:OK18">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OE18:OK18">
+  <conditionalFormatting sqref="OL18:OR18">
     <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OL18:OR18">
+  <conditionalFormatting sqref="OS18:OY18">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OS18:OY18">
+  <conditionalFormatting sqref="OZ18:PF18">
     <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="OZ18:PF18">
+  <conditionalFormatting sqref="PG18:PM18">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="PG18:PM18">
+  <conditionalFormatting sqref="PN18:PT18">
     <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="PN18:PT18">
+  <conditionalFormatting sqref="PU18:QA18">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>